<commit_message>
fixed an itty bitty bug (FocusAreas not plural)
</commit_message>
<xml_diff>
--- a/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
+++ b/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/fair-data-collective/zonmw-project-admin/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068191D3-86E2-4541-A092-F71E2FDF7879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381F6DCB-7C4D-DD46-8A0E-03CB54C7180F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9360" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-termilogy" sheetId="1" r:id="rId1"/>
@@ -602,19 +602,10 @@
     <t>This is a set of controlled terms for the Institutions category.</t>
   </si>
   <si>
-    <t>Focus Areas</t>
-  </si>
-  <si>
-    <t>This is a set of controlled terms for the Focus Areas category.</t>
-  </si>
-  <si>
     <t>zonmwpa:FocusArea</t>
   </si>
   <si>
     <t>Province</t>
-  </si>
-  <si>
-    <t>This is a set of controlled terms for the Themes category.</t>
   </si>
   <si>
     <t>This is a set of controlled terms for the Province category.</t>
@@ -987,6 +978,15 @@
   </si>
   <si>
     <t>2020-10-30T06:55:00+00:01</t>
+  </si>
+  <si>
+    <t>Focus Area</t>
+  </si>
+  <si>
+    <t>This is a set of controlled terms for the Focus Area category.</t>
+  </si>
+  <si>
+    <t>This is a set of controlled terms for the Theme category.</t>
   </si>
 </sst>
 </file>
@@ -1424,8 +1424,8 @@
   </sheetPr>
   <dimension ref="A1:T1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="D234" sqref="D234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1659,7 +1659,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1685,7 +1685,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1711,7 +1711,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -2487,11 +2487,11 @@
         <v>zonmwpa:Service</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="33" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="15" t="s">
@@ -2523,7 +2523,7 @@
       <c r="C40" s="27"/>
       <c r="D40" s="19"/>
       <c r="E40" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F40" s="27"/>
       <c r="G40" s="27"/>
@@ -2552,7 +2552,7 @@
       <c r="C41" s="27"/>
       <c r="D41" s="19"/>
       <c r="E41" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F41" s="27"/>
       <c r="G41" s="27"/>
@@ -2581,7 +2581,7 @@
       <c r="C42" s="27"/>
       <c r="D42" s="19"/>
       <c r="E42" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
@@ -2610,7 +2610,7 @@
       <c r="C43" s="27"/>
       <c r="D43" s="19"/>
       <c r="E43" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F43" s="27"/>
       <c r="G43" s="27"/>
@@ -2639,7 +2639,7 @@
       <c r="C44" s="27"/>
       <c r="D44" s="19"/>
       <c r="E44" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F44" s="27"/>
       <c r="G44" s="27"/>
@@ -2668,7 +2668,7 @@
       <c r="C45" s="27"/>
       <c r="D45" s="19"/>
       <c r="E45" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F45" s="27"/>
       <c r="G45" s="27"/>
@@ -2697,7 +2697,7 @@
       <c r="C46" s="27"/>
       <c r="D46" s="19"/>
       <c r="E46" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F46" s="27"/>
       <c r="G46" s="27"/>
@@ -2726,7 +2726,7 @@
       <c r="C47" s="27"/>
       <c r="D47" s="19"/>
       <c r="E47" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F47" s="27"/>
       <c r="G47" s="27"/>
@@ -2755,7 +2755,7 @@
       <c r="C48" s="27"/>
       <c r="D48" s="19"/>
       <c r="E48" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F48" s="27"/>
       <c r="G48" s="27"/>
@@ -2784,7 +2784,7 @@
       <c r="C49" s="27"/>
       <c r="D49" s="19"/>
       <c r="E49" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F49" s="27"/>
       <c r="G49" s="27"/>
@@ -2813,7 +2813,7 @@
       <c r="C50" s="27"/>
       <c r="D50" s="26"/>
       <c r="E50" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F50" s="27"/>
       <c r="G50" s="28"/>
@@ -2837,11 +2837,11 @@
         <v>zonmwpa:TypeOfMaterial</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="33" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E51" s="17"/>
       <c r="F51" s="15" t="s">
@@ -2873,7 +2873,7 @@
       <c r="C52" s="27"/>
       <c r="D52" s="19"/>
       <c r="E52" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
@@ -2902,7 +2902,7 @@
       <c r="C53" s="27"/>
       <c r="D53" s="19"/>
       <c r="E53" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F53" s="27"/>
       <c r="G53" s="27"/>
@@ -2931,7 +2931,7 @@
       <c r="C54" s="27"/>
       <c r="D54" s="19"/>
       <c r="E54" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F54" s="27"/>
       <c r="G54" s="27"/>
@@ -2960,7 +2960,7 @@
       <c r="C55" s="27"/>
       <c r="D55" s="19"/>
       <c r="E55" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F55" s="27"/>
       <c r="G55" s="27"/>
@@ -2989,7 +2989,7 @@
       <c r="C56" s="27"/>
       <c r="D56" s="19"/>
       <c r="E56" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F56" s="27"/>
       <c r="G56" s="27"/>
@@ -3018,7 +3018,7 @@
       <c r="C57" s="27"/>
       <c r="D57" s="19"/>
       <c r="E57" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F57" s="27"/>
       <c r="G57" s="27"/>
@@ -3047,7 +3047,7 @@
       <c r="C58" s="27"/>
       <c r="D58" s="19"/>
       <c r="E58" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F58" s="27"/>
       <c r="G58" s="27"/>
@@ -3076,7 +3076,7 @@
       <c r="C59" s="27"/>
       <c r="D59" s="19"/>
       <c r="E59" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F59" s="27"/>
       <c r="G59" s="27"/>
@@ -3105,7 +3105,7 @@
       <c r="C60" s="27"/>
       <c r="D60" s="19"/>
       <c r="E60" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F60" s="27"/>
       <c r="G60" s="27"/>
@@ -3134,7 +3134,7 @@
       <c r="C61" s="27"/>
       <c r="D61" s="19"/>
       <c r="E61" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F61" s="27"/>
       <c r="G61" s="27"/>
@@ -3163,7 +3163,7 @@
       <c r="C62" s="27"/>
       <c r="D62" s="19"/>
       <c r="E62" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F62" s="27"/>
       <c r="G62" s="27"/>
@@ -3192,7 +3192,7 @@
       <c r="C63" s="27"/>
       <c r="D63" s="19"/>
       <c r="E63" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F63" s="27"/>
       <c r="G63" s="27"/>
@@ -3221,7 +3221,7 @@
       <c r="C64" s="27"/>
       <c r="D64" s="19"/>
       <c r="E64" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F64" s="27"/>
       <c r="G64" s="27"/>
@@ -3250,7 +3250,7 @@
       <c r="C65" s="27"/>
       <c r="D65" s="19"/>
       <c r="E65" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F65" s="27"/>
       <c r="G65" s="27"/>
@@ -3279,7 +3279,7 @@
       <c r="C66" s="27"/>
       <c r="D66" s="19"/>
       <c r="E66" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F66" s="27"/>
       <c r="G66" s="27"/>
@@ -3308,7 +3308,7 @@
       <c r="C67" s="27"/>
       <c r="D67" s="19"/>
       <c r="E67" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F67" s="27"/>
       <c r="G67" s="27"/>
@@ -3337,7 +3337,7 @@
       <c r="C68" s="27"/>
       <c r="D68" s="19"/>
       <c r="E68" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F68" s="27"/>
       <c r="G68" s="27"/>
@@ -3366,7 +3366,7 @@
       <c r="C69" s="27"/>
       <c r="D69" s="19"/>
       <c r="E69" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F69" s="27"/>
       <c r="G69" s="27"/>
@@ -3395,7 +3395,7 @@
       <c r="C70" s="27"/>
       <c r="D70" s="19"/>
       <c r="E70" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F70" s="27"/>
       <c r="G70" s="27"/>
@@ -3424,7 +3424,7 @@
       <c r="C71" s="27"/>
       <c r="D71" s="19"/>
       <c r="E71" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F71" s="27"/>
       <c r="G71" s="27"/>
@@ -3453,7 +3453,7 @@
       <c r="C72" s="27"/>
       <c r="D72" s="26"/>
       <c r="E72" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F72" s="27"/>
       <c r="G72" s="28"/>
@@ -3477,11 +3477,11 @@
         <v>zonmwpa:TypeOfData</v>
       </c>
       <c r="B73" s="33" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="33" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E73" s="17"/>
       <c r="F73" s="15" t="s">
@@ -3513,7 +3513,7 @@
       <c r="C74" s="27"/>
       <c r="D74" s="19"/>
       <c r="E74" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F74" s="27"/>
       <c r="G74" s="27"/>
@@ -3542,7 +3542,7 @@
       <c r="C75" s="27"/>
       <c r="D75" s="19"/>
       <c r="E75" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F75" s="27"/>
       <c r="G75" s="27"/>
@@ -3571,7 +3571,7 @@
       <c r="C76" s="27"/>
       <c r="D76" s="19"/>
       <c r="E76" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F76" s="27"/>
       <c r="G76" s="27"/>
@@ -3600,7 +3600,7 @@
       <c r="C77" s="27"/>
       <c r="D77" s="19"/>
       <c r="E77" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F77" s="27"/>
       <c r="G77" s="27"/>
@@ -3629,7 +3629,7 @@
       <c r="C78" s="27"/>
       <c r="D78" s="19"/>
       <c r="E78" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F78" s="27"/>
       <c r="G78" s="27"/>
@@ -3658,7 +3658,7 @@
       <c r="C79" s="27"/>
       <c r="D79" s="19"/>
       <c r="E79" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F79" s="27"/>
       <c r="G79" s="27"/>
@@ -3687,7 +3687,7 @@
       <c r="C80" s="27"/>
       <c r="D80" s="19"/>
       <c r="E80" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F80" s="27"/>
       <c r="G80" s="27"/>
@@ -3716,7 +3716,7 @@
       <c r="C81" s="27"/>
       <c r="D81" s="19"/>
       <c r="E81" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F81" s="27"/>
       <c r="G81" s="27"/>
@@ -3745,7 +3745,7 @@
       <c r="C82" s="27"/>
       <c r="D82" s="19"/>
       <c r="E82" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F82" s="27"/>
       <c r="G82" s="27"/>
@@ -3774,7 +3774,7 @@
       <c r="C83" s="27"/>
       <c r="D83" s="19"/>
       <c r="E83" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F83" s="27"/>
       <c r="G83" s="27"/>
@@ -3803,7 +3803,7 @@
       <c r="C84" s="27"/>
       <c r="D84" s="19"/>
       <c r="E84" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="27"/>
@@ -3832,7 +3832,7 @@
       <c r="C85" s="27"/>
       <c r="D85" s="19"/>
       <c r="E85" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F85" s="27"/>
       <c r="G85" s="27"/>
@@ -3861,7 +3861,7 @@
       <c r="C86" s="27"/>
       <c r="D86" s="19"/>
       <c r="E86" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F86" s="27"/>
       <c r="G86" s="27"/>
@@ -3890,7 +3890,7 @@
       <c r="C87" s="27"/>
       <c r="D87" s="19"/>
       <c r="E87" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F87" s="27"/>
       <c r="G87" s="27"/>
@@ -3919,7 +3919,7 @@
       <c r="C88" s="27"/>
       <c r="D88" s="26"/>
       <c r="E88" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F88" s="27"/>
       <c r="G88" s="28"/>
@@ -3943,11 +3943,11 @@
         <v>zonmwpa:TypeOfCollection</v>
       </c>
       <c r="B89" s="33" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C89" s="15"/>
       <c r="D89" s="33" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E89" s="17"/>
       <c r="F89" s="15" t="s">
@@ -3979,7 +3979,7 @@
       <c r="C90" s="27"/>
       <c r="D90" s="19"/>
       <c r="E90" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F90" s="27"/>
       <c r="G90" s="27"/>
@@ -4008,7 +4008,7 @@
       <c r="C91" s="27"/>
       <c r="D91" s="19"/>
       <c r="E91" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F91" s="27"/>
       <c r="G91" s="27"/>
@@ -4037,7 +4037,7 @@
       <c r="C92" s="27"/>
       <c r="D92" s="19"/>
       <c r="E92" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F92" s="27"/>
       <c r="G92" s="27"/>
@@ -4066,7 +4066,7 @@
       <c r="C93" s="27"/>
       <c r="D93" s="19"/>
       <c r="E93" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F93" s="27"/>
       <c r="G93" s="27"/>
@@ -4095,7 +4095,7 @@
       <c r="C94" s="27"/>
       <c r="D94" s="19"/>
       <c r="E94" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F94" s="27"/>
       <c r="G94" s="27"/>
@@ -4124,7 +4124,7 @@
       <c r="C95" s="27"/>
       <c r="D95" s="19"/>
       <c r="E95" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F95" s="27"/>
       <c r="G95" s="27"/>
@@ -4153,7 +4153,7 @@
       <c r="C96" s="27"/>
       <c r="D96" s="19"/>
       <c r="E96" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F96" s="27"/>
       <c r="G96" s="27"/>
@@ -4182,7 +4182,7 @@
       <c r="C97" s="27"/>
       <c r="D97" s="19"/>
       <c r="E97" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F97" s="27"/>
       <c r="G97" s="27"/>
@@ -4211,7 +4211,7 @@
       <c r="C98" s="27"/>
       <c r="D98" s="19"/>
       <c r="E98" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F98" s="27"/>
       <c r="G98" s="27"/>
@@ -4240,7 +4240,7 @@
       <c r="C99" s="27"/>
       <c r="D99" s="26"/>
       <c r="E99" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F99" s="27"/>
       <c r="G99" s="27"/>
@@ -4269,7 +4269,7 @@
       <c r="C100" s="27"/>
       <c r="D100" s="19"/>
       <c r="E100" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F100" s="27"/>
       <c r="G100" s="27"/>
@@ -4298,7 +4298,7 @@
       <c r="C101" s="27"/>
       <c r="D101" s="19"/>
       <c r="E101" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F101" s="27"/>
       <c r="G101" s="27"/>
@@ -4327,7 +4327,7 @@
       <c r="C102" s="27"/>
       <c r="D102" s="19"/>
       <c r="E102" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F102" s="27"/>
       <c r="G102" s="27"/>
@@ -4356,7 +4356,7 @@
       <c r="C103" s="27"/>
       <c r="D103" s="19"/>
       <c r="E103" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F103" s="27"/>
       <c r="G103" s="27"/>
@@ -4385,7 +4385,7 @@
       <c r="C104" s="27"/>
       <c r="D104" s="19"/>
       <c r="E104" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F104" s="27"/>
       <c r="G104" s="27"/>
@@ -4414,7 +4414,7 @@
       <c r="C105" s="27"/>
       <c r="D105" s="19"/>
       <c r="E105" s="34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F105" s="27"/>
       <c r="G105" s="27"/>
@@ -6300,7 +6300,7 @@
         <v>zonmwpa:Institution</v>
       </c>
       <c r="B170" s="33" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C170" s="16"/>
       <c r="D170" s="16" t="s">
@@ -6332,12 +6332,12 @@
 PraktijkverpleegkundigenenPraktijkondersteuners-V&amp;VN</v>
       </c>
       <c r="B171" s="26" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C171" s="30"/>
       <c r="D171" s="26"/>
       <c r="E171" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F171" s="30"/>
       <c r="G171" s="30"/>
@@ -6362,12 +6362,12 @@
 Verenigingen-FMWV</v>
       </c>
       <c r="B172" s="26" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C172" s="30"/>
       <c r="D172" s="26"/>
       <c r="E172" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F172" s="30"/>
       <c r="G172" s="30"/>
@@ -6391,12 +6391,12 @@
         <v>zonmwpa:LandelijkeHuisartsenVereniging-LHV</v>
       </c>
       <c r="B173" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C173" s="30"/>
       <c r="D173" s="26"/>
       <c r="E173" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F173" s="30"/>
       <c r="G173" s="30"/>
@@ -6420,12 +6420,12 @@
         <v>zonmwpa:NederlandsHuisartsenGenootschap-NHG</v>
       </c>
       <c r="B174" s="26" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C174" s="30"/>
       <c r="D174" s="26"/>
       <c r="E174" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F174" s="30"/>
       <c r="G174" s="30"/>
@@ -6449,12 +6449,12 @@
         <v>zonmwpa:NederlandsOogheelkundigGezelschap-NOG</v>
       </c>
       <c r="B175" s="26" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C175" s="30"/>
       <c r="D175" s="26"/>
       <c r="E175" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F175" s="30"/>
       <c r="G175" s="30"/>
@@ -6478,12 +6478,12 @@
         <v>zonmwpa:NederlandscheInternistenVereeniging-NIV</v>
       </c>
       <c r="B176" s="26" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C176" s="30"/>
       <c r="D176" s="26"/>
       <c r="E176" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F176" s="30"/>
       <c r="G176" s="30"/>
@@ -6508,12 +6508,12 @@
 OrthopaedischeVereniging-NOV</v>
       </c>
       <c r="B177" s="26" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C177" s="30"/>
       <c r="D177" s="26"/>
       <c r="E177" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F177" s="30"/>
       <c r="G177" s="30"/>
@@ -6537,12 +6537,12 @@
         <v>zonmwpa:NederlandseGenetischeVereniging-NGV</v>
       </c>
       <c r="B178" s="26" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C178" s="30"/>
       <c r="D178" s="26"/>
       <c r="E178" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F178" s="30"/>
       <c r="G178" s="30"/>
@@ -6567,12 +6567,12 @@
 Celbiologie-NVvC</v>
       </c>
       <c r="B179" s="26" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C179" s="30"/>
       <c r="D179" s="26"/>
       <c r="E179" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F179" s="30"/>
       <c r="G179" s="30"/>
@@ -6597,12 +6597,12 @@
 vanArtsenvoorRevalidatieenPhysischeGeneeskunde</v>
       </c>
       <c r="B180" s="26" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C180" s="30"/>
       <c r="D180" s="26"/>
       <c r="E180" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F180" s="30"/>
       <c r="G180" s="30"/>
@@ -6627,12 +6627,12 @@
 vanBiochemieenMoleculaireBiologie-NVBMB</v>
       </c>
       <c r="B181" s="26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C181" s="30"/>
       <c r="D181" s="26"/>
       <c r="E181" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F181" s="30"/>
       <c r="G181" s="30"/>
@@ -6657,12 +6657,12 @@
 voorAllergologie-NVVA</v>
       </c>
       <c r="B182" s="26" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C182" s="30"/>
       <c r="D182" s="26"/>
       <c r="E182" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F182" s="30"/>
       <c r="G182" s="30"/>
@@ -6687,12 +6687,12 @@
 voorArbeids-enBedrijfsgeneeskunde-NVAB</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C183" s="30"/>
       <c r="D183" s="26"/>
       <c r="E183" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F183" s="30"/>
       <c r="G183" s="30"/>
@@ -6717,12 +6717,12 @@
 voorDuikgeneeskunde-NVD</v>
       </c>
       <c r="B184" s="26" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C184" s="30"/>
       <c r="D184" s="26"/>
       <c r="E184" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F184" s="30"/>
       <c r="G184" s="30"/>
@@ -6747,12 +6747,12 @@
 voorFysiologie-NVF</v>
       </c>
       <c r="B185" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C185" s="30"/>
       <c r="D185" s="26"/>
       <c r="E185" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F185" s="30"/>
       <c r="G185" s="30"/>
@@ -6777,12 +6777,12 @@
 voorGentherapie-NVGT</v>
       </c>
       <c r="B186" s="26" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C186" s="30"/>
       <c r="D186" s="26"/>
       <c r="E186" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F186" s="30"/>
       <c r="G186" s="30"/>
@@ -6807,12 +6807,12 @@
 voorHematologie-NVvH</v>
       </c>
       <c r="B187" s="26" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C187" s="30"/>
       <c r="D187" s="26"/>
       <c r="E187" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F187" s="30"/>
       <c r="G187" s="30"/>
@@ -6837,12 +6837,12 @@
 voorHumaneGenetica-NVHG</v>
       </c>
       <c r="B188" s="26" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C188" s="30"/>
       <c r="D188" s="26"/>
       <c r="E188" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F188" s="30"/>
       <c r="G188" s="30"/>
@@ -6867,12 +6867,12 @@
 voorImmunologie-NVVI</v>
       </c>
       <c r="B189" s="26" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C189" s="30"/>
       <c r="D189" s="26"/>
       <c r="E189" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F189" s="30"/>
       <c r="G189" s="30"/>
@@ -6897,12 +6897,12 @@
 voorKindergeneeskunde-NVK</v>
       </c>
       <c r="B190" s="26" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C190" s="30"/>
       <c r="D190" s="26"/>
       <c r="E190" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F190" s="30"/>
       <c r="G190" s="30"/>
@@ -6927,12 +6927,12 @@
 voorKlinischeChemieenLaboratoriumgeneeskunde-NVKC</v>
       </c>
       <c r="B191" s="26" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C191" s="30"/>
       <c r="D191" s="26"/>
       <c r="E191" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F191" s="30"/>
       <c r="G191" s="30"/>
@@ -6957,12 +6957,12 @@
 voorKlinischeFarmacologieenBiofarmacie</v>
       </c>
       <c r="B192" s="26" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C192" s="30"/>
       <c r="D192" s="26"/>
       <c r="E192" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F192" s="30"/>
       <c r="G192" s="30"/>
@@ -6987,12 +6987,12 @@
 voorKlinischeGeriatrie-NVKG</v>
       </c>
       <c r="B193" s="26" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C193" s="30"/>
       <c r="D193" s="26"/>
       <c r="E193" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F193" s="30"/>
       <c r="G193" s="30"/>
@@ -7017,12 +7017,12 @@
 voorMedischeMicrobiologie-NVMM</v>
       </c>
       <c r="B194" s="26" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C194" s="30"/>
       <c r="D194" s="26"/>
       <c r="E194" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F194" s="30"/>
       <c r="G194" s="30"/>
@@ -7047,12 +7047,12 @@
 voorMedischeOncologie-NVMO</v>
       </c>
       <c r="B195" s="26" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C195" s="30"/>
       <c r="D195" s="26"/>
       <c r="E195" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F195" s="30"/>
       <c r="G195" s="30"/>
@@ -7077,12 +7077,12 @@
 voorOncologie-NVvO</v>
       </c>
       <c r="B196" s="26" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C196" s="30"/>
       <c r="D196" s="26"/>
       <c r="E196" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F196" s="30"/>
       <c r="G196" s="30"/>
@@ -7107,12 +7107,12 @@
 voorParasitologie-NVP</v>
       </c>
       <c r="B197" s="26" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C197" s="30"/>
       <c r="D197" s="26"/>
       <c r="E197" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F197" s="30"/>
       <c r="G197" s="30"/>
@@ -7137,12 +7137,12 @@
 voorPathologie-NVVP</v>
       </c>
       <c r="B198" s="26" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C198" s="30"/>
       <c r="D198" s="26"/>
       <c r="E198" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F198" s="30"/>
       <c r="G198" s="30"/>
@@ -7167,12 +7167,12 @@
 voorProefdierkunde-NVP</v>
       </c>
       <c r="B199" s="26" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C199" s="30"/>
       <c r="D199" s="26"/>
       <c r="E199" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F199" s="30"/>
       <c r="G199" s="30"/>
@@ -7197,12 +7197,12 @@
 voorReumatologie-NVR</v>
       </c>
       <c r="B200" s="26" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C200" s="30"/>
       <c r="D200" s="26"/>
       <c r="E200" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F200" s="30"/>
       <c r="G200" s="30"/>
@@ -7227,12 +7227,12 @@
 enHeelkundevanhetHoofdHalsgebied</v>
       </c>
       <c r="B201" s="26" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C201" s="30"/>
       <c r="D201" s="26"/>
       <c r="E201" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F201" s="30"/>
       <c r="G201" s="30"/>
@@ -7257,12 +7257,12 @@
 Neuropathologie-NVVNP</v>
       </c>
       <c r="B202" s="26" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C202" s="30"/>
       <c r="D202" s="26"/>
       <c r="E202" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F202" s="30"/>
       <c r="G202" s="30"/>
@@ -7287,12 +7287,12 @@
 LongziektenenTuberculose-NVALT</v>
       </c>
       <c r="B203" s="26" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C203" s="30"/>
       <c r="D203" s="26"/>
       <c r="E203" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F203" s="30"/>
       <c r="G203" s="30"/>
@@ -7317,12 +7317,12 @@
 VerstandelijkGehandicapten</v>
       </c>
       <c r="B204" s="26" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C204" s="30"/>
       <c r="D204" s="26"/>
       <c r="E204" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F204" s="30"/>
       <c r="G204" s="30"/>
@@ -7346,12 +7346,12 @@
         <v>zonmwpa:NederlandseVerenigingvanDiëtisten</v>
       </c>
       <c r="B205" s="26" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C205" s="30"/>
       <c r="D205" s="26"/>
       <c r="E205" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F205" s="30"/>
       <c r="G205" s="30"/>
@@ -7376,12 +7376,12 @@
 Leverartsen-MDL</v>
       </c>
       <c r="B206" s="26" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C206" s="30"/>
       <c r="D206" s="26"/>
       <c r="E206" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F206" s="30"/>
       <c r="G206" s="30"/>
@@ -7406,12 +7406,12 @@
 -NVVN</v>
       </c>
       <c r="B207" s="26" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C207" s="30"/>
       <c r="D207" s="26"/>
       <c r="E207" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F207" s="30"/>
       <c r="G207" s="30"/>
@@ -7435,12 +7435,12 @@
         <v>zonmwpa:NederlandseVerenigingvanNeurologie-NVN</v>
       </c>
       <c r="B208" s="26" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C208" s="30"/>
       <c r="D208" s="26"/>
       <c r="E208" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F208" s="30"/>
       <c r="G208" s="30"/>
@@ -7465,12 +7465,12 @@
 Verzekeringsgeneeskunde-NVVG</v>
       </c>
       <c r="B209" s="26" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C209" s="30"/>
       <c r="D209" s="26"/>
       <c r="E209" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F209" s="30"/>
       <c r="G209" s="30"/>
@@ -7495,12 +7495,12 @@
 -NAV</v>
       </c>
       <c r="B210" s="26" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C210" s="30"/>
       <c r="D210" s="26"/>
       <c r="E210" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F210" s="30"/>
       <c r="G210" s="30"/>
@@ -7525,12 +7525,12 @@
 Venereologie-NVDV</v>
       </c>
       <c r="B211" s="26" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C211" s="30"/>
       <c r="D211" s="26"/>
       <c r="E211" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F211" s="30"/>
       <c r="G211" s="30"/>
@@ -7555,12 +7555,12 @@
 -NVvH</v>
       </c>
       <c r="B212" s="26" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C212" s="30"/>
       <c r="D212" s="26"/>
       <c r="E212" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F212" s="30"/>
       <c r="G212" s="30"/>
@@ -7585,12 +7585,12 @@
 Geneeskunde-NVNG</v>
       </c>
       <c r="B213" s="26" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C213" s="30"/>
       <c r="D213" s="26"/>
       <c r="E213" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F213" s="30"/>
       <c r="G213" s="30"/>
@@ -7615,12 +7615,12 @@
 Gynaecologie-NVOG</v>
       </c>
       <c r="B214" s="26" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C214" s="30"/>
       <c r="D214" s="26"/>
       <c r="E214" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F214" s="30"/>
       <c r="G214" s="30"/>
@@ -7644,12 +7644,12 @@
         <v>zonmwpa:NederlandseVerenigingvoorPlastischeenReconstructieveChirurgie-NVPC</v>
       </c>
       <c r="B215" s="26" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C215" s="30"/>
       <c r="D215" s="26"/>
       <c r="E215" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F215" s="30"/>
       <c r="G215" s="30"/>
@@ -7674,12 +7674,12 @@
 -NVVP</v>
       </c>
       <c r="B216" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C216" s="30"/>
       <c r="D216" s="26"/>
       <c r="E216" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F216" s="30"/>
       <c r="G216" s="30"/>
@@ -7704,12 +7704,12 @@
 -NVvR</v>
       </c>
       <c r="B217" s="26" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C217" s="30"/>
       <c r="D217" s="26"/>
       <c r="E217" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F217" s="30"/>
       <c r="G217" s="30"/>
@@ -7734,12 +7734,12 @@
 enOncologie-NVRO</v>
       </c>
       <c r="B218" s="26" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C218" s="30"/>
       <c r="D218" s="26"/>
       <c r="E218" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F218" s="30"/>
       <c r="G218" s="30"/>
@@ -7764,12 +7764,12 @@
 -NVT</v>
       </c>
       <c r="B219" s="26" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C219" s="30"/>
       <c r="D219" s="26"/>
       <c r="E219" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F219" s="30"/>
       <c r="G219" s="30"/>
@@ -7793,12 +7793,12 @@
         <v>zonmwpa:NederlandseVerenigingvoorUrologie-NVU</v>
       </c>
       <c r="B220" s="26" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C220" s="30"/>
       <c r="D220" s="26"/>
       <c r="E220" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F220" s="30"/>
       <c r="G220" s="30"/>
@@ -7823,12 +7823,12 @@
 Ouderengeneeskunde-Verenso</v>
       </c>
       <c r="B221" s="26" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C221" s="30"/>
       <c r="D221" s="26"/>
       <c r="E221" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F221" s="30"/>
       <c r="G221" s="30"/>
@@ -7852,12 +7852,12 @@
         <v>zonmwpa:VerenigingvanEpidemiologie-VvE</v>
       </c>
       <c r="B222" s="26" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C222" s="30"/>
       <c r="D222" s="26"/>
       <c r="E222" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F222" s="30"/>
       <c r="G222" s="30"/>
@@ -7882,12 +7882,12 @@
 WetenschappelijkeOnderzoekers-V.M.W.O.</v>
       </c>
       <c r="B223" s="26" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C223" s="30"/>
       <c r="D223" s="26"/>
       <c r="E223" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F223" s="30"/>
       <c r="G223" s="30"/>
@@ -7912,12 +7912,12 @@
 InformatieverwerkingindeZorg-VMBI</v>
       </c>
       <c r="B224" s="26" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C224" s="30"/>
       <c r="D224" s="26"/>
       <c r="E224" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F224" s="30"/>
       <c r="G224" s="30"/>
@@ -7942,12 +7942,12 @@
 Sportgeneeskunde</v>
       </c>
       <c r="B225" s="26" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C225" s="30"/>
       <c r="D225" s="26"/>
       <c r="E225" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F225" s="30"/>
       <c r="G225" s="30"/>
@@ -7971,12 +7971,12 @@
         <v>zonmwpa:VerenigingvoorInfectieziekten-VIZ</v>
       </c>
       <c r="B226" s="26" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C226" s="30"/>
       <c r="D226" s="26"/>
       <c r="E226" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F226" s="30"/>
       <c r="G226" s="30"/>
@@ -8000,12 +8000,12 @@
         <v>zonmwpa:Otherinstitution</v>
       </c>
       <c r="B227" s="31" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C227" s="30"/>
       <c r="D227" s="26"/>
       <c r="E227" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F227" s="30"/>
       <c r="G227" s="30"/>
@@ -8026,14 +8026,14 @@
     <row r="228" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="16" t="str">
         <f t="shared" ref="A228:A232" si="3">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B228," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
-        <v>zonmwpa:FocusAreas</v>
-      </c>
-      <c r="B228" s="16" t="s">
-        <v>182</v>
+        <v>zonmwpa:FocusArea</v>
+      </c>
+      <c r="B228" s="33" t="s">
+        <v>293</v>
       </c>
       <c r="C228" s="16"/>
-      <c r="D228" s="16" t="s">
-        <v>183</v>
+      <c r="D228" s="33" t="s">
+        <v>294</v>
       </c>
       <c r="E228" s="17"/>
       <c r="F228" s="16" t="s">
@@ -8060,12 +8060,12 @@
         <v>zonmwpa:Predictivediagnosticsandtreatment</v>
       </c>
       <c r="B229" s="31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C229" s="30"/>
       <c r="D229" s="26"/>
-      <c r="E229" s="30" t="s">
-        <v>184</v>
+      <c r="E229" s="34" t="s">
+        <v>182</v>
       </c>
       <c r="F229" s="30"/>
       <c r="G229" s="30"/>
@@ -8089,12 +8089,12 @@
         <v>zonmwpa:Careandprevention</v>
       </c>
       <c r="B230" s="31" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C230" s="30"/>
       <c r="D230" s="26"/>
       <c r="E230" s="30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F230" s="30"/>
       <c r="G230" s="30"/>
@@ -8118,12 +8118,12 @@
         <v>zonmwpa:Effectsonsociety</v>
       </c>
       <c r="B231" s="31" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C231" s="30"/>
       <c r="D231" s="26"/>
       <c r="E231" s="30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F231" s="30"/>
       <c r="G231" s="30"/>
@@ -8147,12 +8147,12 @@
         <v>zonmwpa:OtherFocusArea</v>
       </c>
       <c r="B232" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C232" s="30"/>
       <c r="D232" s="26"/>
       <c r="E232" s="30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F232" s="30"/>
       <c r="G232" s="30"/>
@@ -8176,11 +8176,11 @@
         <v>zonmwpa:Theme</v>
       </c>
       <c r="B233" s="33" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C233" s="16"/>
-      <c r="D233" s="16" t="s">
-        <v>186</v>
+      <c r="D233" s="33" t="s">
+        <v>295</v>
       </c>
       <c r="E233" s="17"/>
       <c r="F233" s="16" t="s">
@@ -8207,12 +8207,12 @@
         <v>zonmwpa:Treatment</v>
       </c>
       <c r="B234" s="31" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C234" s="30"/>
       <c r="D234" s="26"/>
       <c r="E234" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F234" s="30"/>
       <c r="G234" s="30"/>
@@ -8236,12 +8236,12 @@
         <v>zonmwpa:Diagnosticsofinfection</v>
       </c>
       <c r="B235" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C235" s="30"/>
       <c r="D235" s="26"/>
       <c r="E235" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F235" s="30"/>
       <c r="G235" s="30"/>
@@ -8265,12 +8265,12 @@
         <v>zonmwpa:Riskanalysisandprognostics</v>
       </c>
       <c r="B236" s="31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C236" s="30"/>
       <c r="D236" s="26"/>
       <c r="E236" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F236" s="30"/>
       <c r="G236" s="30"/>
@@ -8294,12 +8294,12 @@
         <v>zonmwpa:Virus-immunity-immuneresponseandpathogenesis</v>
       </c>
       <c r="B237" s="31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C237" s="30"/>
       <c r="D237" s="26"/>
       <c r="E237" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F237" s="30"/>
       <c r="G237" s="30"/>
@@ -8323,12 +8323,12 @@
         <v>zonmwpa:Clinicaltreatment</v>
       </c>
       <c r="B238" s="31" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C238" s="30"/>
       <c r="D238" s="26"/>
       <c r="E238" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F238" s="30"/>
       <c r="G238" s="30"/>
@@ -8352,12 +8352,12 @@
         <v>zonmwpa:Animalfreeinnovations</v>
       </c>
       <c r="B239" s="31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C239" s="30"/>
       <c r="D239" s="26"/>
       <c r="E239" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F239" s="30"/>
       <c r="G239" s="30"/>
@@ -8381,12 +8381,12 @@
         <v>zonmwpa:Organisationofcareandprevention</v>
       </c>
       <c r="B240" s="31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C240" s="30"/>
       <c r="D240" s="26"/>
       <c r="E240" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F240" s="30"/>
       <c r="G240" s="30"/>
@@ -8410,12 +8410,12 @@
         <v>zonmwpa:Careandpreventionforvulnerablecitizens</v>
       </c>
       <c r="B241" s="31" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C241" s="30"/>
       <c r="D241" s="26"/>
       <c r="E241" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F241" s="30"/>
       <c r="G241" s="30"/>
@@ -8439,12 +8439,12 @@
         <v>zonmwpa:Transmissionandepidemiology</v>
       </c>
       <c r="B242" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C242" s="30"/>
       <c r="D242" s="26"/>
       <c r="E242" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F242" s="30"/>
       <c r="G242" s="30"/>
@@ -8468,12 +8468,12 @@
         <v>zonmwpa:Palliativecare</v>
       </c>
       <c r="B243" s="31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C243" s="30"/>
       <c r="D243" s="26"/>
       <c r="E243" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F243" s="30"/>
       <c r="G243" s="30"/>
@@ -8497,12 +8497,12 @@
         <v>zonmwpa:Impactofmeasuresorstrategies</v>
       </c>
       <c r="B244" s="31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C244" s="30"/>
       <c r="D244" s="26"/>
       <c r="E244" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F244" s="30"/>
       <c r="G244" s="30"/>
@@ -8526,12 +8526,12 @@
         <v>zonmwpa:Resilienceofsociety</v>
       </c>
       <c r="B245" s="31" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C245" s="30"/>
       <c r="D245" s="26"/>
       <c r="E245" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F245" s="30"/>
       <c r="G245" s="30"/>
@@ -8555,12 +8555,12 @@
         <v>zonmwpa:Economicresilience</v>
       </c>
       <c r="B246" s="31" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C246" s="30"/>
       <c r="D246" s="26"/>
       <c r="E246" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F246" s="30"/>
       <c r="G246" s="30"/>
@@ -8584,12 +8584,12 @@
         <v>zonmwpa:OtherTheme</v>
       </c>
       <c r="B247" s="31" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C247" s="30"/>
       <c r="D247" s="26"/>
       <c r="E247" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F247" s="30"/>
       <c r="G247" s="30"/>
@@ -8613,11 +8613,11 @@
         <v>zonmwpa:Province</v>
       </c>
       <c r="B248" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C248" s="16"/>
       <c r="D248" s="16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E248" s="17"/>
       <c r="F248" s="16" t="s">
@@ -8644,12 +8644,12 @@
         <v>zonmwpa:Drenthe</v>
       </c>
       <c r="B249" s="26" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C249" s="30"/>
       <c r="D249" s="26"/>
       <c r="E249" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F249" s="30"/>
       <c r="G249" s="30"/>
@@ -8673,12 +8673,12 @@
         <v>zonmwpa:Flevoland</v>
       </c>
       <c r="B250" s="26" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C250" s="30"/>
       <c r="D250" s="26"/>
       <c r="E250" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F250" s="30"/>
       <c r="G250" s="30"/>
@@ -8702,12 +8702,12 @@
         <v>zonmwpa:Friesland</v>
       </c>
       <c r="B251" s="26" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C251" s="30"/>
       <c r="D251" s="26"/>
       <c r="E251" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F251" s="30"/>
       <c r="G251" s="30"/>
@@ -8731,12 +8731,12 @@
         <v>zonmwpa:Gelderland</v>
       </c>
       <c r="B252" s="26" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C252" s="30"/>
       <c r="D252" s="26"/>
       <c r="E252" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F252" s="30"/>
       <c r="G252" s="30"/>
@@ -8760,12 +8760,12 @@
         <v>zonmwpa:Groningen</v>
       </c>
       <c r="B253" s="26" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C253" s="30"/>
       <c r="D253" s="26"/>
       <c r="E253" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F253" s="30"/>
       <c r="G253" s="30"/>
@@ -8789,12 +8789,12 @@
         <v>zonmwpa:Limburg</v>
       </c>
       <c r="B254" s="26" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C254" s="30"/>
       <c r="D254" s="26"/>
       <c r="E254" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F254" s="30"/>
       <c r="G254" s="30"/>
@@ -8818,12 +8818,12 @@
         <v>zonmwpa:Noord-Brabant</v>
       </c>
       <c r="B255" s="26" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C255" s="30"/>
       <c r="D255" s="26"/>
       <c r="E255" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F255" s="30"/>
       <c r="G255" s="30"/>
@@ -8847,12 +8847,12 @@
         <v>zonmwpa:Noord-Holland</v>
       </c>
       <c r="B256" s="26" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C256" s="30"/>
       <c r="D256" s="26"/>
       <c r="E256" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F256" s="30"/>
       <c r="G256" s="30"/>
@@ -8876,12 +8876,12 @@
         <v>zonmwpa:Overijssel</v>
       </c>
       <c r="B257" s="26" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C257" s="30"/>
       <c r="D257" s="26"/>
       <c r="E257" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F257" s="30"/>
       <c r="G257" s="30"/>
@@ -8905,12 +8905,12 @@
         <v>zonmwpa:Utrecht</v>
       </c>
       <c r="B258" s="26" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C258" s="30"/>
       <c r="D258" s="26"/>
       <c r="E258" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F258" s="30"/>
       <c r="G258" s="30"/>
@@ -8934,12 +8934,12 @@
         <v>zonmwpa:Zeeland</v>
       </c>
       <c r="B259" s="26" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C259" s="30"/>
       <c r="D259" s="26"/>
       <c r="E259" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F259" s="30"/>
       <c r="G259" s="30"/>
@@ -8963,12 +8963,12 @@
         <v>zonmwpa:Zuid-Holland</v>
       </c>
       <c r="B260" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C260" s="30"/>
       <c r="D260" s="26"/>
       <c r="E260" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F260" s="30"/>
       <c r="G260" s="30"/>
@@ -8992,12 +8992,12 @@
         <v>zonmwpa:OtherProvince</v>
       </c>
       <c r="B261" s="31" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C261" s="30"/>
       <c r="D261" s="26"/>
       <c r="E261" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F261" s="30"/>
       <c r="G261" s="30"/>

</xml_diff>

<commit_message>
trying to eliminate icky chars
</commit_message>
<xml_diff>
--- a/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
+++ b/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/fair-data-collective/zonmw-project-admin/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381F6DCB-7C4D-DD46-8A0E-03CB54C7180F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849CBF44-9781-1040-AA43-323DB0F54247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="46900" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-termilogy" sheetId="1" r:id="rId1"/>
@@ -971,9 +971,6 @@
     <t>zonmwpa:TypeOfCollection</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>2020-10-30T06:55:00+00:00</t>
   </si>
   <si>
@@ -987,6 +984,9 @@
   </si>
   <si>
     <t>This is a set of controlled terms for the Theme category.</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1204,6 +1204,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1424,8 +1425,8 @@
   </sheetPr>
   <dimension ref="A1:T1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="D234" sqref="D234"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1659,7 +1660,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1685,9 +1686,9 @@
         <v>17</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>291</v>
-      </c>
-      <c r="C10" s="3"/>
+        <v>290</v>
+      </c>
+      <c r="C10" s="38"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1711,9 +1712,9 @@
         <v>18</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>292</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>291</v>
+      </c>
+      <c r="C11" s="37"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1928,7 +1929,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="str">
-        <f t="shared" ref="A20:A169" si="0">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B20," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" ref="A20" si="0">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B20," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
         <v>zonmwpa:StudyArea</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -1959,7 +1960,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B21," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
         <v>zonmwpa:Township</v>
       </c>
       <c r="B21" s="20" t="s">
@@ -1988,7 +1989,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A22:A85" si="1">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B22," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
         <v>zonmwpa:Rural</v>
       </c>
       <c r="B22" s="26" t="s">
@@ -2017,7 +2018,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Multiplemunicipalities</v>
       </c>
       <c r="B23" s="26" t="s">
@@ -2046,7 +2047,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Provincial</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -2075,7 +2076,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Regional</v>
       </c>
       <c r="B25" s="26" t="s">
@@ -2104,7 +2105,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Neighbourhood</v>
       </c>
       <c r="B26" s="26" t="s">
@@ -2133,7 +2134,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:OtherStudyArea</v>
       </c>
       <c r="B27" s="26" t="s">
@@ -2162,7 +2163,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:SizeOfCollection</v>
       </c>
       <c r="B28" s="14" t="s">
@@ -2193,7 +2194,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Under10</v>
       </c>
       <c r="B29" s="26" t="s">
@@ -2222,7 +2223,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:10-100</v>
       </c>
       <c r="B30" s="19" t="s">
@@ -2251,7 +2252,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:100-1000</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2280,7 +2281,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:1000-10.000</v>
       </c>
       <c r="B32" s="19" t="s">
@@ -2309,7 +2310,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:10.000-100.000</v>
       </c>
       <c r="B33" s="19" t="s">
@@ -2338,7 +2339,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:100.000-1.000.000</v>
       </c>
       <c r="B34" s="19" t="s">
@@ -2367,7 +2368,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:1.000.000-10.000.000</v>
       </c>
       <c r="B35" s="19" t="s">
@@ -2396,7 +2397,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:10.000.000-100.000.000</v>
       </c>
       <c r="B36" s="19" t="s">
@@ -2425,7 +2426,7 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:100.000.000-1.000.000.000</v>
       </c>
       <c r="B37" s="19" t="s">
@@ -2454,7 +2455,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:OtherSizeOfCollection</v>
       </c>
       <c r="B38" s="26" t="s">
@@ -2483,7 +2484,7 @@
     </row>
     <row r="39" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Service</v>
       </c>
       <c r="B39" s="33" t="s">
@@ -2514,7 +2515,7 @@
     </row>
     <row r="40" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:BSL-2laboratoriesavailable</v>
       </c>
       <c r="B40" s="19" t="s">
@@ -2543,7 +2544,7 @@
     </row>
     <row r="41" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:BSL-3laboratoriesavailable</v>
       </c>
       <c r="B41" s="19" t="s">
@@ -2572,7 +2573,7 @@
     </row>
     <row r="42" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:MemberCOVID-19Network</v>
       </c>
       <c r="B42" s="26" t="s">
@@ -2601,7 +2602,7 @@
     </row>
     <row r="43" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:AntibodyDevelopment</v>
       </c>
       <c r="B43" s="19" t="s">
@@ -2630,7 +2631,7 @@
     </row>
     <row r="44" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:LaboratoriesdoingPCR-baseddiagnosis</v>
       </c>
       <c r="B44" s="19" t="s">
@@ -2659,7 +2660,7 @@
     </row>
     <row r="45" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Proteomicsstudiesincludingproteinengineeringandproteininteractions</v>
       </c>
       <c r="B45" s="19" t="s">
@@ -2688,7 +2689,7 @@
     </row>
     <row r="46" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Screeningtoolsforsearchingvirusproteasesinhibitors</v>
       </c>
       <c r="B46" s="19" t="s">
@@ -2717,7 +2718,7 @@
     </row>
     <row r="47" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:AnimalTestingFacility</v>
       </c>
       <c r="B47" s="19" t="s">
@@ -2746,7 +2747,7 @@
     </row>
     <row r="48" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Abilitytosetupclinicaltrials</v>
       </c>
       <c r="B48" s="19" t="s">
@@ -2775,7 +2776,7 @@
     </row>
     <row r="49" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:VirusSequencingFacility</v>
       </c>
       <c r="B49" s="19" t="s">
@@ -2804,7 +2805,7 @@
     </row>
     <row r="50" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:OtherServices</v>
       </c>
       <c r="B50" s="26" t="s">
@@ -2833,7 +2834,7 @@
     </row>
     <row r="51" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:TypeOfMaterial</v>
       </c>
       <c r="B51" s="33" t="s">
@@ -2864,7 +2865,7 @@
     </row>
     <row r="52" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:BuffyCoat</v>
       </c>
       <c r="B52" s="19" t="s">
@@ -2893,7 +2894,7 @@
     </row>
     <row r="53" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:cDNADivmRNA</v>
       </c>
       <c r="B53" s="19" t="s">
@@ -2922,7 +2923,7 @@
     </row>
     <row r="54" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Celllines</v>
       </c>
       <c r="B54" s="19" t="s">
@@ -2951,7 +2952,7 @@
     </row>
     <row r="55" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:DNA</v>
       </c>
       <c r="B55" s="19" t="s">
@@ -2980,7 +2981,7 @@
     </row>
     <row r="56" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Faeces</v>
       </c>
       <c r="B56" s="19" t="s">
@@ -3009,7 +3010,7 @@
     </row>
     <row r="57" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:microRNA</v>
       </c>
       <c r="B57" s="19" t="s">
@@ -3038,7 +3039,7 @@
     </row>
     <row r="58" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Nasalswab</v>
       </c>
       <c r="B58" s="19" t="s">
@@ -3067,7 +3068,7 @@
     </row>
     <row r="59" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Notavailable</v>
       </c>
       <c r="B59" s="19" t="s">
@@ -3096,7 +3097,7 @@
     </row>
     <row r="60" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Pathogen</v>
       </c>
       <c r="B60" s="19" t="s">
@@ -3125,7 +3126,7 @@
     </row>
     <row r="61" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Peripheralbloodcells</v>
       </c>
       <c r="B61" s="19" t="s">
@@ -3154,7 +3155,7 @@
     </row>
     <row r="62" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Plasma</v>
       </c>
       <c r="B62" s="19" t="s">
@@ -3183,7 +3184,7 @@
     </row>
     <row r="63" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:RNA</v>
       </c>
       <c r="B63" s="19" t="s">
@@ -3212,7 +3213,7 @@
     </row>
     <row r="64" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Saliva</v>
       </c>
       <c r="B64" s="19" t="s">
@@ -3241,7 +3242,7 @@
     </row>
     <row r="65" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Serum</v>
       </c>
       <c r="B65" s="19" t="s">
@@ -3270,7 +3271,7 @@
     </row>
     <row r="66" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Throatswab</v>
       </c>
       <c r="B66" s="19" t="s">
@@ -3299,7 +3300,7 @@
     </row>
     <row r="67" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Tissue-cryopreserved</v>
       </c>
       <c r="B67" s="19" t="s">
@@ -3328,7 +3329,7 @@
     </row>
     <row r="68" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Tissue-paraffinpreserved</v>
       </c>
       <c r="B68" s="19" t="s">
@@ -3357,7 +3358,7 @@
     </row>
     <row r="69" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Tissue-stainedsectionsDivslides</v>
       </c>
       <c r="B69" s="19" t="s">
@@ -3386,7 +3387,7 @@
     </row>
     <row r="70" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Urine</v>
       </c>
       <c r="B70" s="19" t="s">
@@ -3415,7 +3416,7 @@
     </row>
     <row r="71" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:WholeBlood</v>
       </c>
       <c r="B71" s="19" t="s">
@@ -3444,7 +3445,7 @@
     </row>
     <row r="72" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:OtherTypesOfMaterial</v>
       </c>
       <c r="B72" s="26" t="s">
@@ -3473,7 +3474,7 @@
     </row>
     <row r="73" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:TypeOfData</v>
       </c>
       <c r="B73" s="33" t="s">
@@ -3504,7 +3505,7 @@
     </row>
     <row r="74" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Antibodiestiter-IgMandIgG</v>
       </c>
       <c r="B74" s="19" t="s">
@@ -3533,7 +3534,7 @@
     </row>
     <row r="75" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Biologicalsamples</v>
       </c>
       <c r="B75" s="19" t="s">
@@ -3562,7 +3563,7 @@
     </row>
     <row r="76" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Bloodcountandotherlabresultsespeciallyatthemomentofhospitaladmission</v>
       </c>
       <c r="B76" s="19" t="s">
@@ -3591,7 +3592,7 @@
     </row>
     <row r="77" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Dataonclinicalsymptoms</v>
       </c>
       <c r="B77" s="19" t="s">
@@ -3620,7 +3621,7 @@
     </row>
     <row r="78" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:CTimagingoflungs-alternativelyXray</v>
       </c>
       <c r="B78" s="19" t="s">
@@ -3649,7 +3650,7 @@
     </row>
     <row r="79" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Dataondiseasedurationanddiseaseoutcome</v>
       </c>
       <c r="B79" s="19" t="s">
@@ -3678,7 +3679,7 @@
     </row>
     <row r="80" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Genealogicalrecords</v>
       </c>
       <c r="B80" s="19" t="s">
@@ -3707,7 +3708,7 @@
     </row>
     <row r="81" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Imagingdata</v>
       </c>
       <c r="B81" s="19" t="s">
@@ -3736,7 +3737,7 @@
     </row>
     <row r="82" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Medicalrecords</v>
       </c>
       <c r="B82" s="19" t="s">
@@ -3765,7 +3766,7 @@
     </row>
     <row r="83" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Nationalregistries</v>
       </c>
       <c r="B83" s="19" t="s">
@@ -3794,7 +3795,7 @@
     </row>
     <row r="84" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:PhysiologicalDivBiochemicalmeasurements</v>
       </c>
       <c r="B84" s="19" t="s">
@@ -3823,7 +3824,7 @@
     </row>
     <row r="85" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Surveydata</v>
       </c>
       <c r="B85" s="19" t="s">
@@ -3852,7 +3853,7 @@
     </row>
     <row r="86" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A86:A149" si="2">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B86," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
         <v>zonmwpa:Treatmentprotocol-typesofdrugsused</v>
       </c>
       <c r="B86" s="19" t="s">
@@ -3881,7 +3882,7 @@
     </row>
     <row r="87" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Notavailable</v>
       </c>
       <c r="B87" s="19" t="s">
@@ -3910,7 +3911,7 @@
     </row>
     <row r="88" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:OtherTypesOfData</v>
       </c>
       <c r="B88" s="26" t="s">
@@ -3939,7 +3940,7 @@
     </row>
     <row r="89" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:TypeOfCollection</v>
       </c>
       <c r="B89" s="33" t="s">
@@ -3970,7 +3971,7 @@
     </row>
     <row r="90" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Birthcohort</v>
       </c>
       <c r="B90" s="19" t="s">
@@ -3999,7 +4000,7 @@
     </row>
     <row r="91" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Case-Control</v>
       </c>
       <c r="B91" s="19" t="s">
@@ -4028,7 +4029,7 @@
     </row>
     <row r="92" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Cohort</v>
       </c>
       <c r="B92" s="19" t="s">
@@ -4057,7 +4058,7 @@
     </row>
     <row r="93" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Cross-sectional</v>
       </c>
       <c r="B93" s="19" t="s">
@@ -4086,7 +4087,7 @@
     </row>
     <row r="94" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Diseasespecific</v>
       </c>
       <c r="B94" s="19" t="s">
@@ -4115,7 +4116,7 @@
     </row>
     <row r="95" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Hospital</v>
       </c>
       <c r="B95" s="19" t="s">
@@ -4144,7 +4145,7 @@
     </row>
     <row r="96" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Imagecollection</v>
       </c>
       <c r="B96" s="19" t="s">
@@ -4173,7 +4174,7 @@
     </row>
     <row r="97" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Longitudinal</v>
       </c>
       <c r="B97" s="19" t="s">
@@ -4202,7 +4203,7 @@
     </row>
     <row r="98" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Non-human</v>
       </c>
       <c r="B98" s="19" t="s">
@@ -4231,7 +4232,7 @@
     </row>
     <row r="99" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:OtherTypeofCollection</v>
       </c>
       <c r="B99" s="26" t="s">
@@ -4260,7 +4261,7 @@
     </row>
     <row r="100" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Population-based</v>
       </c>
       <c r="B100" s="19" t="s">
@@ -4289,7 +4290,7 @@
     </row>
     <row r="101" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Prospectivestudy</v>
       </c>
       <c r="B101" s="19" t="s">
@@ -4318,7 +4319,7 @@
     </row>
     <row r="102" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Qualitycontrol</v>
       </c>
       <c r="B102" s="19" t="s">
@@ -4347,7 +4348,7 @@
     </row>
     <row r="103" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Rarediseasecollection</v>
       </c>
       <c r="B103" s="19" t="s">
@@ -4376,7 +4377,7 @@
     </row>
     <row r="104" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Samplecollection</v>
       </c>
       <c r="B104" s="19" t="s">
@@ -4405,7 +4406,7 @@
     </row>
     <row r="105" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Twin-study</v>
       </c>
       <c r="B105" s="19" t="s">
@@ -4434,7 +4435,7 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106" s="13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Population</v>
       </c>
       <c r="B106" s="14" t="s">
@@ -4465,7 +4466,7 @@
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Populationwide</v>
       </c>
       <c r="B107" s="19" t="s">
@@ -4494,7 +4495,7 @@
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A108" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Neonates</v>
       </c>
       <c r="B108" s="19" t="s">
@@ -4523,7 +4524,7 @@
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A109" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Children-0-18years</v>
       </c>
       <c r="B109" s="19" t="s">
@@ -4552,7 +4553,7 @@
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A110" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Primaryschoolchildren-4-12years</v>
       </c>
       <c r="B110" s="19" t="s">
@@ -4581,7 +4582,7 @@
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A111" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Teenager-12-18years</v>
       </c>
       <c r="B111" s="19" t="s">
@@ -4610,7 +4611,7 @@
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A112" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Youngpeople-16-27years</v>
       </c>
       <c r="B112" s="19" t="s">
@@ -4639,7 +4640,7 @@
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Youngadults18-21years</v>
       </c>
       <c r="B113" s="19" t="s">
@@ -4668,7 +4669,7 @@
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Adults-18-65years</v>
       </c>
       <c r="B114" s="19" t="s">
@@ -4697,7 +4698,7 @@
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Elderly-65plus</v>
       </c>
       <c r="B115" s="19" t="s">
@@ -4726,7 +4727,7 @@
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Vulnerableelderly</v>
       </c>
       <c r="B116" s="19" t="s">
@@ -4755,7 +4756,7 @@
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Pregnantwomen</v>
       </c>
       <c r="B117" s="19" t="s">
@@ -4784,7 +4785,7 @@
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Peoplewithaspecificethnicbackground</v>
       </c>
       <c r="B118" s="19" t="s">
@@ -4813,7 +4814,7 @@
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Peoplewithamigrationbackground</v>
       </c>
       <c r="B119" s="19" t="s">
@@ -4842,7 +4843,7 @@
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Peoplewithachronicillness</v>
       </c>
       <c r="B120" s="19" t="s">
@@ -4871,7 +4872,7 @@
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Peoplewithaphysicaldisability</v>
       </c>
       <c r="B121" s="19" t="s">
@@ -4900,7 +4901,7 @@
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A122" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Mentallychallengedpeople</v>
       </c>
       <c r="B122" s="19" t="s">
@@ -4929,7 +4930,7 @@
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Peoplewithararecondition</v>
       </c>
       <c r="B123" s="19" t="s">
@@ -4958,7 +4959,7 @@
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A124" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Peoplewithalowsocio-economicstatus</v>
       </c>
       <c r="B124" s="19" t="s">
@@ -4987,7 +4988,7 @@
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A125" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Workingpeople</v>
       </c>
       <c r="B125" s="19" t="s">
@@ -5016,7 +5017,7 @@
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A126" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Topathletes</v>
       </c>
       <c r="B126" s="26" t="s">
@@ -5045,7 +5046,7 @@
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Men</v>
       </c>
       <c r="B127" s="19" t="s">
@@ -5074,7 +5075,7 @@
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Women</v>
       </c>
       <c r="B128" s="19" t="s">
@@ -5103,7 +5104,7 @@
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A129" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:OtherPopulation</v>
       </c>
       <c r="B129" s="26" t="s">
@@ -5132,7 +5133,7 @@
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A130" s="13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:CareProcessPhase</v>
       </c>
       <c r="B130" s="14" t="s">
@@ -5163,7 +5164,7 @@
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Prevention</v>
       </c>
       <c r="B131" s="19" t="s">
@@ -5192,7 +5193,7 @@
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A132" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Diagnosis</v>
       </c>
       <c r="B132" s="19" t="s">
@@ -5221,7 +5222,7 @@
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A133" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Therapy</v>
       </c>
       <c r="B133" s="19" t="s">
@@ -5250,7 +5251,7 @@
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A134" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Follow-up</v>
       </c>
       <c r="B134" s="19" t="s">
@@ -5279,7 +5280,7 @@
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A135" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Aftercare</v>
       </c>
       <c r="B135" s="19" t="s">
@@ -5308,7 +5309,7 @@
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A136" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Palliative</v>
       </c>
       <c r="B136" s="19" t="s">
@@ -5337,7 +5338,7 @@
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A137" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Information</v>
       </c>
       <c r="B137" s="19" t="s">
@@ -5366,8 +5367,8 @@
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A138" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>zonmwpa:Earlydetection&amp;screening</v>
+        <f t="shared" si="2"/>
+        <v>zonmwpa:Earlydetection-screening</v>
       </c>
       <c r="B138" s="19" t="s">
         <v>150</v>
@@ -5395,7 +5396,7 @@
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A139" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Organizationofcare</v>
       </c>
       <c r="B139" s="19" t="s">
@@ -5424,7 +5425,7 @@
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A140" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:OtherCareProcessPhase</v>
       </c>
       <c r="B140" s="26" t="s">
@@ -5453,7 +5454,7 @@
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A141" s="13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Setting</v>
       </c>
       <c r="B141" s="14" t="s">
@@ -5484,7 +5485,7 @@
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A142" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Primarycare</v>
       </c>
       <c r="B142" s="19" t="s">
@@ -5513,7 +5514,7 @@
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A143" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Second-linecare</v>
       </c>
       <c r="B143" s="19" t="s">
@@ -5542,7 +5543,7 @@
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A144" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Prevention</v>
       </c>
       <c r="B144" s="19" t="s">
@@ -5571,7 +5572,7 @@
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A145" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Healthcareinstitution</v>
       </c>
       <c r="B145" s="19" t="s">
@@ -5600,7 +5601,7 @@
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A146" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Cattle</v>
       </c>
       <c r="B146" s="19" t="s">
@@ -5629,7 +5630,7 @@
     </row>
     <row r="147" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A147" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Transmural</v>
       </c>
       <c r="B147" s="19" t="s">
@@ -5658,7 +5659,7 @@
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A148" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Nursinghomecare</v>
       </c>
       <c r="B148" s="19" t="s">
@@ -5687,7 +5688,7 @@
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A149" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Hospitalcare</v>
       </c>
       <c r="B149" s="19" t="s">
@@ -5716,7 +5717,7 @@
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A150" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A150:A213" si="3">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B150," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
         <v>zonmwpa:Homecare</v>
       </c>
       <c r="B150" s="19" t="s">
@@ -5745,7 +5746,7 @@
     </row>
     <row r="151" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A151" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Education-schoolandupbringing</v>
       </c>
       <c r="B151" s="19" t="s">
@@ -5774,7 +5775,7 @@
     </row>
     <row r="152" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A152" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:WorkandIncome</v>
       </c>
       <c r="B152" s="26" t="s">
@@ -5803,7 +5804,7 @@
     </row>
     <row r="153" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A153" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Neighbourhood</v>
       </c>
       <c r="B153" s="19" t="s">
@@ -5832,7 +5833,7 @@
     </row>
     <row r="154" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A154" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Care</v>
       </c>
       <c r="B154" s="19" t="s">
@@ -5861,8 +5862,8 @@
     </row>
     <row r="155" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A155" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>zonmwpa:Earlydetection&amp;screening</v>
+        <f t="shared" si="3"/>
+        <v>zonmwpa:Earlydetection-screening</v>
       </c>
       <c r="B155" s="19" t="s">
         <v>150</v>
@@ -5890,7 +5891,7 @@
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A156" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Justice</v>
       </c>
       <c r="B156" s="19" t="s">
@@ -5919,7 +5920,7 @@
     </row>
     <row r="157" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A157" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Socialdomain</v>
       </c>
       <c r="B157" s="19" t="s">
@@ -5948,7 +5949,7 @@
     </row>
     <row r="158" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A158" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Youth</v>
       </c>
       <c r="B158" s="19" t="s">
@@ -5977,7 +5978,7 @@
     </row>
     <row r="159" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A159" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:SocialSupport</v>
       </c>
       <c r="B159" s="19" t="s">
@@ -6006,7 +6007,7 @@
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A160" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:SportDivhealthDivwellness</v>
       </c>
       <c r="B160" s="19" t="s">
@@ -6035,7 +6036,7 @@
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A161" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Disabledcare</v>
       </c>
       <c r="B161" s="19" t="s">
@@ -6064,7 +6065,7 @@
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A162" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Long-termmentalhealthcare</v>
       </c>
       <c r="B162" s="26" t="s">
@@ -6093,7 +6094,7 @@
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A163" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Youth-healthcare</v>
       </c>
       <c r="B163" s="26" t="s">
@@ -6122,7 +6123,7 @@
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A164" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Generalpractitionercare</v>
       </c>
       <c r="B164" s="19" t="s">
@@ -6151,7 +6152,7 @@
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A165" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Elderlycare</v>
       </c>
       <c r="B165" s="19" t="s">
@@ -6180,7 +6181,7 @@
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A166" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:ClientsandDivorpatientorganization</v>
       </c>
       <c r="B166" s="19" t="s">
@@ -6209,7 +6210,7 @@
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A167" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Measuringinstrument</v>
       </c>
       <c r="B167" s="19" t="s">
@@ -6238,7 +6239,7 @@
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A168" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Experimentalgarden</v>
       </c>
       <c r="B168" s="19" t="s">
@@ -6267,7 +6268,7 @@
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A169" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:OtherSetting</v>
       </c>
       <c r="B169" s="26" t="s">
@@ -6296,7 +6297,7 @@
     </row>
     <row r="170" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="16" t="str">
-        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B170," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Institution</v>
       </c>
       <c r="B170" s="33" t="s">
@@ -6327,9 +6328,9 @@
     </row>
     <row r="171" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="26" t="str">
-        <f t="shared" ref="A171" si="1">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B171," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Beroepsvereniging
-PraktijkverpleegkundigenenPraktijkondersteuners-V&amp;VN</v>
+PraktijkverpleegkundigenenPraktijkondersteuners-V-VN</v>
       </c>
       <c r="B171" s="26" t="s">
         <v>202</v>
@@ -6357,7 +6358,7 @@
     </row>
     <row r="172" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="26" t="str">
-        <f t="shared" ref="A172:A227" si="2">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B172," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="3"/>
         <v>zonmwpa:FederatievanMedischWetenschappelijke
 Verenigingen-FMWV</v>
       </c>
@@ -6387,7 +6388,7 @@
     </row>
     <row r="173" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:LandelijkeHuisartsenVereniging-LHV</v>
       </c>
       <c r="B173" s="26" t="s">
@@ -6416,7 +6417,7 @@
     </row>
     <row r="174" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandsHuisartsenGenootschap-NHG</v>
       </c>
       <c r="B174" s="26" t="s">
@@ -6445,7 +6446,7 @@
     </row>
     <row r="175" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandsOogheelkundigGezelschap-NOG</v>
       </c>
       <c r="B175" s="26" t="s">
@@ -6474,7 +6475,7 @@
     </row>
     <row r="176" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandscheInternistenVereeniging-NIV</v>
       </c>
       <c r="B176" s="26" t="s">
@@ -6503,7 +6504,7 @@
     </row>
     <row r="177" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Nederlandse
 OrthopaedischeVereniging-NOV</v>
       </c>
@@ -6533,7 +6534,7 @@
     </row>
     <row r="178" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseGenetischeVereniging-NGV</v>
       </c>
       <c r="B178" s="26" t="s">
@@ -6562,7 +6563,7 @@
     </row>
     <row r="179" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 Celbiologie-NVvC</v>
       </c>
@@ -6592,7 +6593,7 @@
     </row>
     <row r="180" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 vanArtsenvoorRevalidatieenPhysischeGeneeskunde</v>
       </c>
@@ -6622,7 +6623,7 @@
     </row>
     <row r="181" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 vanBiochemieenMoleculaireBiologie-NVBMB</v>
       </c>
@@ -6652,7 +6653,7 @@
     </row>
     <row r="182" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorAllergologie-NVVA</v>
       </c>
@@ -6682,7 +6683,7 @@
     </row>
     <row r="183" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorArbeids-enBedrijfsgeneeskunde-NVAB</v>
       </c>
@@ -6712,7 +6713,7 @@
     </row>
     <row r="184" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorDuikgeneeskunde-NVD</v>
       </c>
@@ -6742,7 +6743,7 @@
     </row>
     <row r="185" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorFysiologie-NVF</v>
       </c>
@@ -6772,7 +6773,7 @@
     </row>
     <row r="186" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorGentherapie-NVGT</v>
       </c>
@@ -6802,7 +6803,7 @@
     </row>
     <row r="187" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorHematologie-NVvH</v>
       </c>
@@ -6832,7 +6833,7 @@
     </row>
     <row r="188" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorHumaneGenetica-NVHG</v>
       </c>
@@ -6862,7 +6863,7 @@
     </row>
     <row r="189" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorImmunologie-NVVI</v>
       </c>
@@ -6892,7 +6893,7 @@
     </row>
     <row r="190" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorKindergeneeskunde-NVK</v>
       </c>
@@ -6922,7 +6923,7 @@
     </row>
     <row r="191" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorKlinischeChemieenLaboratoriumgeneeskunde-NVKC</v>
       </c>
@@ -6952,7 +6953,7 @@
     </row>
     <row r="192" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorKlinischeFarmacologieenBiofarmacie</v>
       </c>
@@ -6982,7 +6983,7 @@
     </row>
     <row r="193" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorKlinischeGeriatrie-NVKG</v>
       </c>
@@ -7012,7 +7013,7 @@
     </row>
     <row r="194" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorMedischeMicrobiologie-NVMM</v>
       </c>
@@ -7042,7 +7043,7 @@
     </row>
     <row r="195" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorMedischeOncologie-NVMO</v>
       </c>
@@ -7072,7 +7073,7 @@
     </row>
     <row r="196" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorOncologie-NVvO</v>
       </c>
@@ -7102,7 +7103,7 @@
     </row>
     <row r="197" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorParasitologie-NVP</v>
       </c>
@@ -7132,7 +7133,7 @@
     </row>
     <row r="198" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorPathologie-NVVP</v>
       </c>
@@ -7162,7 +7163,7 @@
     </row>
     <row r="199" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorProefdierkunde-NVP</v>
       </c>
@@ -7192,7 +7193,7 @@
     </row>
     <row r="200" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVereniging
 voorReumatologie-NVR</v>
       </c>
@@ -7222,7 +7223,7 @@
     </row>
     <row r="201" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingKeel-Neus-Oorheelkunde
 enHeelkundevanhetHoofdHalsgebied</v>
       </c>
@@ -7252,7 +7253,7 @@
     </row>
     <row r="202" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingv.
 Neuropathologie-NVVNP</v>
       </c>
@@ -7282,7 +7283,7 @@
     </row>
     <row r="203" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvanArtsenvoor
 LongziektenenTuberculose-NVALT</v>
       </c>
@@ -7312,7 +7313,7 @@
     </row>
     <row r="204" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvanArtsenvoor
 VerstandelijkGehandicapten</v>
       </c>
@@ -7342,10 +7343,10 @@
     </row>
     <row r="205" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>zonmwpa:NederlandseVerenigingvanDiëtisten</v>
-      </c>
-      <c r="B205" s="26" t="s">
+        <f t="shared" si="3"/>
+        <v>zonmwpa:NederlandseVerenigingvanDietisten</v>
+      </c>
+      <c r="B205" s="31" t="s">
         <v>236</v>
       </c>
       <c r="C205" s="30"/>
@@ -7371,8 +7372,8 @@
     </row>
     <row r="206" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>zonmwpa:NederlandseVerenigingvanMaag--Darm-en
+        <f t="shared" si="3"/>
+        <v>zonmwpa:NederlandseVerenigingvanMaag-Darm-en
 Leverartsen-MDL</v>
       </c>
       <c r="B206" s="26" t="s">
@@ -7401,7 +7402,7 @@
     </row>
     <row r="207" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvanNeurochirurgen
 -NVVN</v>
       </c>
@@ -7431,7 +7432,7 @@
     </row>
     <row r="208" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvanNeurologie-NVN</v>
       </c>
       <c r="B208" s="26" t="s">
@@ -7460,7 +7461,7 @@
     </row>
     <row r="209" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoor
 Verzekeringsgeneeskunde-NVVG</v>
       </c>
@@ -7490,7 +7491,7 @@
     </row>
     <row r="210" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorAnesthesiologie
 -NAV</v>
       </c>
@@ -7520,7 +7521,7 @@
     </row>
     <row r="211" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorDermatologieen
 Venereologie-NVDV</v>
       </c>
@@ -7550,7 +7551,7 @@
     </row>
     <row r="212" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorHeelkunde
 -NVvH</v>
       </c>
@@ -7580,7 +7581,7 @@
     </row>
     <row r="213" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorNucleaire
 Geneeskunde-NVNG</v>
       </c>
@@ -7610,7 +7611,7 @@
     </row>
     <row r="214" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A214:A261" si="4">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B214," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
         <v>zonmwpa:NederlandseVerenigingvoorObstetrieen
 Gynaecologie-NVOG</v>
       </c>
@@ -7640,7 +7641,7 @@
     </row>
     <row r="215" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:NederlandseVerenigingvoorPlastischeenReconstructieveChirurgie-NVPC</v>
       </c>
       <c r="B215" s="26" t="s">
@@ -7669,7 +7670,7 @@
     </row>
     <row r="216" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:NederlandseVerenigingvoorPsychiatrie
 -NVVP</v>
       </c>
@@ -7699,7 +7700,7 @@
     </row>
     <row r="217" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:NederlandseVerenigingvoorRadiologie
 -NVvR</v>
       </c>
@@ -7729,7 +7730,7 @@
     </row>
     <row r="218" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:NederlandseVerenigingvoorRadiotherapie
 enOncologie-NVRO</v>
       </c>
@@ -7759,7 +7760,7 @@
     </row>
     <row r="219" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:NederlandseVerenigingvoorThoraxchirurgie
 -NVT</v>
       </c>
@@ -7789,7 +7790,7 @@
     </row>
     <row r="220" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:NederlandseVerenigingvoorUrologie-NVU</v>
       </c>
       <c r="B220" s="26" t="s">
@@ -7818,7 +7819,7 @@
     </row>
     <row r="221" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:VerenigingSpecialistenin
 Ouderengeneeskunde-Verenso</v>
       </c>
@@ -7848,7 +7849,7 @@
     </row>
     <row r="222" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:VerenigingvanEpidemiologie-VvE</v>
       </c>
       <c r="B222" s="26" t="s">
@@ -7877,7 +7878,7 @@
     </row>
     <row r="223" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:VerenigingvanMedisch
 WetenschappelijkeOnderzoekers-V.M.W.O.</v>
       </c>
@@ -7907,7 +7908,7 @@
     </row>
     <row r="224" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Verenigingvoor
 InformatieverwerkingindeZorg-VMBI</v>
       </c>
@@ -7937,7 +7938,7 @@
     </row>
     <row r="225" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Verenigingvoor
 Sportgeneeskunde</v>
       </c>
@@ -7967,7 +7968,7 @@
     </row>
     <row r="226" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:VerenigingvoorInfectieziekten-VIZ</v>
       </c>
       <c r="B226" s="26" t="s">
@@ -7996,7 +7997,7 @@
     </row>
     <row r="227" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="26" t="str">
-        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B227," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Otherinstitution</v>
       </c>
       <c r="B227" s="31" t="s">
@@ -8025,15 +8026,15 @@
     </row>
     <row r="228" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="16" t="str">
-        <f t="shared" ref="A228:A232" si="3">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B228," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="4"/>
         <v>zonmwpa:FocusArea</v>
       </c>
       <c r="B228" s="33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C228" s="16"/>
       <c r="D228" s="33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E228" s="17"/>
       <c r="F228" s="16" t="s">
@@ -8056,7 +8057,7 @@
     </row>
     <row r="229" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Predictivediagnosticsandtreatment</v>
       </c>
       <c r="B229" s="31" t="s">
@@ -8085,7 +8086,7 @@
     </row>
     <row r="230" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Careandprevention</v>
       </c>
       <c r="B230" s="31" t="s">
@@ -8114,7 +8115,7 @@
     </row>
     <row r="231" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A231" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Effectsonsociety</v>
       </c>
       <c r="B231" s="31" t="s">
@@ -8143,7 +8144,7 @@
     </row>
     <row r="232" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:OtherFocusArea</v>
       </c>
       <c r="B232" s="31" t="s">
@@ -8172,7 +8173,7 @@
     </row>
     <row r="233" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A233" s="16" t="str">
-        <f t="shared" ref="A233:A242" si="4">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B233," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Theme</v>
       </c>
       <c r="B233" s="33" t="s">
@@ -8180,7 +8181,7 @@
       </c>
       <c r="C233" s="16"/>
       <c r="D233" s="33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E233" s="17"/>
       <c r="F233" s="16" t="s">
@@ -8464,7 +8465,7 @@
     </row>
     <row r="243" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A243" s="26" t="str">
-        <f t="shared" ref="A243:A247" si="5">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B243," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Palliativecare</v>
       </c>
       <c r="B243" s="31" t="s">
@@ -8493,7 +8494,7 @@
     </row>
     <row r="244" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A244" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Impactofmeasuresorstrategies</v>
       </c>
       <c r="B244" s="31" t="s">
@@ -8522,7 +8523,7 @@
     </row>
     <row r="245" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A245" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Resilienceofsociety</v>
       </c>
       <c r="B245" s="31" t="s">
@@ -8551,7 +8552,7 @@
     </row>
     <row r="246" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A246" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Economicresilience</v>
       </c>
       <c r="B246" s="31" t="s">
@@ -8580,7 +8581,7 @@
     </row>
     <row r="247" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A247" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:OtherTheme</v>
       </c>
       <c r="B247" s="31" t="s">
@@ -8609,7 +8610,7 @@
     </row>
     <row r="248" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A248" s="16" t="str">
-        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B248," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Province</v>
       </c>
       <c r="B248" s="16" t="s">
@@ -8640,7 +8641,7 @@
     </row>
     <row r="249" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A249" s="26" t="str">
-        <f t="shared" ref="A249:A253" si="6">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B249," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Drenthe</v>
       </c>
       <c r="B249" s="26" t="s">
@@ -8669,7 +8670,7 @@
     </row>
     <row r="250" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A250" s="26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Flevoland</v>
       </c>
       <c r="B250" s="26" t="s">
@@ -8698,7 +8699,7 @@
     </row>
     <row r="251" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A251" s="26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Friesland</v>
       </c>
       <c r="B251" s="26" t="s">
@@ -8727,7 +8728,7 @@
     </row>
     <row r="252" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A252" s="26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Gelderland</v>
       </c>
       <c r="B252" s="26" t="s">
@@ -8756,7 +8757,7 @@
     </row>
     <row r="253" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A253" s="26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Groningen</v>
       </c>
       <c r="B253" s="26" t="s">
@@ -8785,7 +8786,7 @@
     </row>
     <row r="254" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A254" s="26" t="str">
-        <f t="shared" ref="A254:A261" si="7">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B254," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"))</f>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Limburg</v>
       </c>
       <c r="B254" s="26" t="s">
@@ -8814,7 +8815,7 @@
     </row>
     <row r="255" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A255" s="26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Noord-Brabant</v>
       </c>
       <c r="B255" s="26" t="s">
@@ -8843,7 +8844,7 @@
     </row>
     <row r="256" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A256" s="26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Noord-Holland</v>
       </c>
       <c r="B256" s="26" t="s">
@@ -8872,7 +8873,7 @@
     </row>
     <row r="257" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A257" s="26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Overijssel</v>
       </c>
       <c r="B257" s="26" t="s">
@@ -8901,7 +8902,7 @@
     </row>
     <row r="258" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A258" s="26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Utrecht</v>
       </c>
       <c r="B258" s="26" t="s">
@@ -8930,7 +8931,7 @@
     </row>
     <row r="259" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A259" s="26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Zeeland</v>
       </c>
       <c r="B259" s="26" t="s">
@@ -8959,7 +8960,7 @@
     </row>
     <row r="260" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A260" s="26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:Zuid-Holland</v>
       </c>
       <c r="B260" s="26" t="s">
@@ -8988,7 +8989,7 @@
     </row>
     <row r="261" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A261" s="26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>zonmwpa:OtherProvince</v>
       </c>
       <c r="B261" s="31" t="s">

</xml_diff>

<commit_message>
still clearing bad chars stuff
\u000A (line feed) this time
</commit_message>
<xml_diff>
--- a/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
+++ b/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/fair-data-collective/zonmw-project-admin/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849CBF44-9781-1040-AA43-323DB0F54247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB2D2FC-59CD-5A4F-94DB-451CB6A049B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="46900" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="295">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -971,12 +971,6 @@
     <t>zonmwpa:TypeOfCollection</t>
   </si>
   <si>
-    <t>2020-10-30T06:55:00+00:00</t>
-  </si>
-  <si>
-    <t>2020-10-30T06:55:00+00:01</t>
-  </si>
-  <si>
     <t>Focus Area</t>
   </si>
   <si>
@@ -986,7 +980,10 @@
     <t>This is a set of controlled terms for the Theme category.</t>
   </si>
   <si>
-    <t>1.1.0</t>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>2020-10-30T13:43:00+00:00</t>
   </si>
 </sst>
 </file>
@@ -1425,8 +1422,8 @@
   </sheetPr>
   <dimension ref="A1:T1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1660,7 +1657,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1686,7 +1683,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="3"/>
@@ -1712,7 +1709,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="3"/>
@@ -1929,7 +1926,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="str">
-        <f t="shared" ref="A20" si="0">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B20," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
+        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B20," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
         <v>zonmwpa:StudyArea</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -1989,7 +1986,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="str">
-        <f t="shared" ref="A22:A85" si="1">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B22," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
+        <f t="shared" ref="A22:A84" si="0">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B22," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
         <v>zonmwpa:Rural</v>
       </c>
       <c r="B22" s="26" t="s">
@@ -2018,7 +2015,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Multiplemunicipalities</v>
       </c>
       <c r="B23" s="26" t="s">
@@ -2047,7 +2044,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Provincial</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -2076,7 +2073,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Regional</v>
       </c>
       <c r="B25" s="26" t="s">
@@ -2105,7 +2102,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Neighbourhood</v>
       </c>
       <c r="B26" s="26" t="s">
@@ -2134,7 +2131,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:OtherStudyArea</v>
       </c>
       <c r="B27" s="26" t="s">
@@ -2163,7 +2160,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:SizeOfCollection</v>
       </c>
       <c r="B28" s="14" t="s">
@@ -2194,7 +2191,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Under10</v>
       </c>
       <c r="B29" s="26" t="s">
@@ -2223,7 +2220,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:10-100</v>
       </c>
       <c r="B30" s="19" t="s">
@@ -2252,7 +2249,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:100-1000</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2281,7 +2278,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:1000-10.000</v>
       </c>
       <c r="B32" s="19" t="s">
@@ -2310,7 +2307,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:10.000-100.000</v>
       </c>
       <c r="B33" s="19" t="s">
@@ -2339,7 +2336,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:100.000-1.000.000</v>
       </c>
       <c r="B34" s="19" t="s">
@@ -2368,7 +2365,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:1.000.000-10.000.000</v>
       </c>
       <c r="B35" s="19" t="s">
@@ -2397,7 +2394,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:10.000.000-100.000.000</v>
       </c>
       <c r="B36" s="19" t="s">
@@ -2426,7 +2423,7 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:100.000.000-1.000.000.000</v>
       </c>
       <c r="B37" s="19" t="s">
@@ -2455,7 +2452,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:OtherSizeOfCollection</v>
       </c>
       <c r="B38" s="26" t="s">
@@ -2484,7 +2481,7 @@
     </row>
     <row r="39" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Service</v>
       </c>
       <c r="B39" s="33" t="s">
@@ -2515,7 +2512,7 @@
     </row>
     <row r="40" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:BSL-2laboratoriesavailable</v>
       </c>
       <c r="B40" s="19" t="s">
@@ -2544,7 +2541,7 @@
     </row>
     <row r="41" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:BSL-3laboratoriesavailable</v>
       </c>
       <c r="B41" s="19" t="s">
@@ -2573,7 +2570,7 @@
     </row>
     <row r="42" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:MemberCOVID-19Network</v>
       </c>
       <c r="B42" s="26" t="s">
@@ -2602,7 +2599,7 @@
     </row>
     <row r="43" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:AntibodyDevelopment</v>
       </c>
       <c r="B43" s="19" t="s">
@@ -2631,7 +2628,7 @@
     </row>
     <row r="44" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:LaboratoriesdoingPCR-baseddiagnosis</v>
       </c>
       <c r="B44" s="19" t="s">
@@ -2660,7 +2657,7 @@
     </row>
     <row r="45" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Proteomicsstudiesincludingproteinengineeringandproteininteractions</v>
       </c>
       <c r="B45" s="19" t="s">
@@ -2689,7 +2686,7 @@
     </row>
     <row r="46" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Screeningtoolsforsearchingvirusproteasesinhibitors</v>
       </c>
       <c r="B46" s="19" t="s">
@@ -2718,7 +2715,7 @@
     </row>
     <row r="47" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:AnimalTestingFacility</v>
       </c>
       <c r="B47" s="19" t="s">
@@ -2747,7 +2744,7 @@
     </row>
     <row r="48" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Abilitytosetupclinicaltrials</v>
       </c>
       <c r="B48" s="19" t="s">
@@ -2776,7 +2773,7 @@
     </row>
     <row r="49" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:VirusSequencingFacility</v>
       </c>
       <c r="B49" s="19" t="s">
@@ -2805,7 +2802,7 @@
     </row>
     <row r="50" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:OtherServices</v>
       </c>
       <c r="B50" s="26" t="s">
@@ -2834,7 +2831,7 @@
     </row>
     <row r="51" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:TypeOfMaterial</v>
       </c>
       <c r="B51" s="33" t="s">
@@ -2865,7 +2862,7 @@
     </row>
     <row r="52" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:BuffyCoat</v>
       </c>
       <c r="B52" s="19" t="s">
@@ -2894,7 +2891,7 @@
     </row>
     <row r="53" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:cDNADivmRNA</v>
       </c>
       <c r="B53" s="19" t="s">
@@ -2923,7 +2920,7 @@
     </row>
     <row r="54" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Celllines</v>
       </c>
       <c r="B54" s="19" t="s">
@@ -2952,7 +2949,7 @@
     </row>
     <row r="55" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:DNA</v>
       </c>
       <c r="B55" s="19" t="s">
@@ -2981,7 +2978,7 @@
     </row>
     <row r="56" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Faeces</v>
       </c>
       <c r="B56" s="19" t="s">
@@ -3010,7 +3007,7 @@
     </row>
     <row r="57" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:microRNA</v>
       </c>
       <c r="B57" s="19" t="s">
@@ -3039,7 +3036,7 @@
     </row>
     <row r="58" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Nasalswab</v>
       </c>
       <c r="B58" s="19" t="s">
@@ -3068,7 +3065,7 @@
     </row>
     <row r="59" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Notavailable</v>
       </c>
       <c r="B59" s="19" t="s">
@@ -3097,7 +3094,7 @@
     </row>
     <row r="60" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Pathogen</v>
       </c>
       <c r="B60" s="19" t="s">
@@ -3126,7 +3123,7 @@
     </row>
     <row r="61" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Peripheralbloodcells</v>
       </c>
       <c r="B61" s="19" t="s">
@@ -3155,7 +3152,7 @@
     </row>
     <row r="62" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Plasma</v>
       </c>
       <c r="B62" s="19" t="s">
@@ -3184,7 +3181,7 @@
     </row>
     <row r="63" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:RNA</v>
       </c>
       <c r="B63" s="19" t="s">
@@ -3213,7 +3210,7 @@
     </row>
     <row r="64" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Saliva</v>
       </c>
       <c r="B64" s="19" t="s">
@@ -3242,7 +3239,7 @@
     </row>
     <row r="65" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Serum</v>
       </c>
       <c r="B65" s="19" t="s">
@@ -3271,7 +3268,7 @@
     </row>
     <row r="66" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Throatswab</v>
       </c>
       <c r="B66" s="19" t="s">
@@ -3300,7 +3297,7 @@
     </row>
     <row r="67" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Tissue-cryopreserved</v>
       </c>
       <c r="B67" s="19" t="s">
@@ -3329,7 +3326,7 @@
     </row>
     <row r="68" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Tissue-paraffinpreserved</v>
       </c>
       <c r="B68" s="19" t="s">
@@ -3358,7 +3355,7 @@
     </row>
     <row r="69" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Tissue-stainedsectionsDivslides</v>
       </c>
       <c r="B69" s="19" t="s">
@@ -3387,7 +3384,7 @@
     </row>
     <row r="70" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Urine</v>
       </c>
       <c r="B70" s="19" t="s">
@@ -3416,7 +3413,7 @@
     </row>
     <row r="71" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:WholeBlood</v>
       </c>
       <c r="B71" s="19" t="s">
@@ -3445,7 +3442,7 @@
     </row>
     <row r="72" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:OtherTypesOfMaterial</v>
       </c>
       <c r="B72" s="26" t="s">
@@ -3474,7 +3471,7 @@
     </row>
     <row r="73" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:TypeOfData</v>
       </c>
       <c r="B73" s="33" t="s">
@@ -3505,7 +3502,7 @@
     </row>
     <row r="74" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Antibodiestiter-IgMandIgG</v>
       </c>
       <c r="B74" s="19" t="s">
@@ -3534,7 +3531,7 @@
     </row>
     <row r="75" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Biologicalsamples</v>
       </c>
       <c r="B75" s="19" t="s">
@@ -3563,7 +3560,7 @@
     </row>
     <row r="76" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Bloodcountandotherlabresultsespeciallyatthemomentofhospitaladmission</v>
       </c>
       <c r="B76" s="19" t="s">
@@ -3592,7 +3589,7 @@
     </row>
     <row r="77" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Dataonclinicalsymptoms</v>
       </c>
       <c r="B77" s="19" t="s">
@@ -3621,7 +3618,7 @@
     </row>
     <row r="78" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:CTimagingoflungs-alternativelyXray</v>
       </c>
       <c r="B78" s="19" t="s">
@@ -3650,7 +3647,7 @@
     </row>
     <row r="79" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Dataondiseasedurationanddiseaseoutcome</v>
       </c>
       <c r="B79" s="19" t="s">
@@ -3679,7 +3676,7 @@
     </row>
     <row r="80" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Genealogicalrecords</v>
       </c>
       <c r="B80" s="19" t="s">
@@ -3708,7 +3705,7 @@
     </row>
     <row r="81" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Imagingdata</v>
       </c>
       <c r="B81" s="19" t="s">
@@ -3737,7 +3734,7 @@
     </row>
     <row r="82" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Medicalrecords</v>
       </c>
       <c r="B82" s="19" t="s">
@@ -3766,7 +3763,7 @@
     </row>
     <row r="83" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:Nationalregistries</v>
       </c>
       <c r="B83" s="19" t="s">
@@ -3795,7 +3792,7 @@
     </row>
     <row r="84" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>zonmwpa:PhysiologicalDivBiochemicalmeasurements</v>
       </c>
       <c r="B84" s="19" t="s">
@@ -3824,7 +3821,7 @@
     </row>
     <row r="85" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A85:A111" si="1">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B85," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
         <v>zonmwpa:Surveydata</v>
       </c>
       <c r="B85" s="19" t="s">
@@ -3853,7 +3850,7 @@
     </row>
     <row r="86" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="19" t="str">
-        <f t="shared" ref="A86:A149" si="2">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B86," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Treatmentprotocol-typesofdrugsused</v>
       </c>
       <c r="B86" s="19" t="s">
@@ -3882,7 +3879,7 @@
     </row>
     <row r="87" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Notavailable</v>
       </c>
       <c r="B87" s="19" t="s">
@@ -3911,7 +3908,7 @@
     </row>
     <row r="88" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:OtherTypesOfData</v>
       </c>
       <c r="B88" s="26" t="s">
@@ -3940,7 +3937,7 @@
     </row>
     <row r="89" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:TypeOfCollection</v>
       </c>
       <c r="B89" s="33" t="s">
@@ -3971,7 +3968,7 @@
     </row>
     <row r="90" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Birthcohort</v>
       </c>
       <c r="B90" s="19" t="s">
@@ -4000,7 +3997,7 @@
     </row>
     <row r="91" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Case-Control</v>
       </c>
       <c r="B91" s="19" t="s">
@@ -4029,7 +4026,7 @@
     </row>
     <row r="92" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Cohort</v>
       </c>
       <c r="B92" s="19" t="s">
@@ -4058,7 +4055,7 @@
     </row>
     <row r="93" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Cross-sectional</v>
       </c>
       <c r="B93" s="19" t="s">
@@ -4087,7 +4084,7 @@
     </row>
     <row r="94" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Diseasespecific</v>
       </c>
       <c r="B94" s="19" t="s">
@@ -4116,7 +4113,7 @@
     </row>
     <row r="95" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Hospital</v>
       </c>
       <c r="B95" s="19" t="s">
@@ -4145,7 +4142,7 @@
     </row>
     <row r="96" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Imagecollection</v>
       </c>
       <c r="B96" s="19" t="s">
@@ -4174,7 +4171,7 @@
     </row>
     <row r="97" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Longitudinal</v>
       </c>
       <c r="B97" s="19" t="s">
@@ -4203,7 +4200,7 @@
     </row>
     <row r="98" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Non-human</v>
       </c>
       <c r="B98" s="19" t="s">
@@ -4232,7 +4229,7 @@
     </row>
     <row r="99" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:OtherTypeofCollection</v>
       </c>
       <c r="B99" s="26" t="s">
@@ -4261,7 +4258,7 @@
     </row>
     <row r="100" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Population-based</v>
       </c>
       <c r="B100" s="19" t="s">
@@ -4290,7 +4287,7 @@
     </row>
     <row r="101" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Prospectivestudy</v>
       </c>
       <c r="B101" s="19" t="s">
@@ -4319,7 +4316,7 @@
     </row>
     <row r="102" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Qualitycontrol</v>
       </c>
       <c r="B102" s="19" t="s">
@@ -4348,7 +4345,7 @@
     </row>
     <row r="103" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Rarediseasecollection</v>
       </c>
       <c r="B103" s="19" t="s">
@@ -4377,7 +4374,7 @@
     </row>
     <row r="104" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Samplecollection</v>
       </c>
       <c r="B104" s="19" t="s">
@@ -4406,7 +4403,7 @@
     </row>
     <row r="105" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Twin-study</v>
       </c>
       <c r="B105" s="19" t="s">
@@ -4435,7 +4432,7 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Population</v>
       </c>
       <c r="B106" s="14" t="s">
@@ -4466,7 +4463,7 @@
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Populationwide</v>
       </c>
       <c r="B107" s="19" t="s">
@@ -4495,7 +4492,7 @@
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A108" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Neonates</v>
       </c>
       <c r="B108" s="19" t="s">
@@ -4524,7 +4521,7 @@
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A109" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Children-0-18years</v>
       </c>
       <c r="B109" s="19" t="s">
@@ -4553,7 +4550,7 @@
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A110" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Primaryschoolchildren-4-12years</v>
       </c>
       <c r="B110" s="19" t="s">
@@ -4582,7 +4579,7 @@
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A111" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zonmwpa:Teenager-12-18years</v>
       </c>
       <c r="B111" s="19" t="s">
@@ -4611,7 +4608,7 @@
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A112" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B112," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
         <v>zonmwpa:Youngpeople-16-27years</v>
       </c>
       <c r="B112" s="19" t="s">
@@ -4640,7 +4637,7 @@
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A113:A176" si="2">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B113," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
         <v>zonmwpa:Youngadults18-21years</v>
       </c>
       <c r="B113" s="19" t="s">
@@ -5717,7 +5714,7 @@
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A150" s="19" t="str">
-        <f t="shared" ref="A150:A213" si="3">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B150," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Homecare</v>
       </c>
       <c r="B150" s="19" t="s">
@@ -5746,7 +5743,7 @@
     </row>
     <row r="151" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A151" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Education-schoolandupbringing</v>
       </c>
       <c r="B151" s="19" t="s">
@@ -5775,7 +5772,7 @@
     </row>
     <row r="152" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A152" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:WorkandIncome</v>
       </c>
       <c r="B152" s="26" t="s">
@@ -5804,7 +5801,7 @@
     </row>
     <row r="153" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A153" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Neighbourhood</v>
       </c>
       <c r="B153" s="19" t="s">
@@ -5833,7 +5830,7 @@
     </row>
     <row r="154" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A154" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Care</v>
       </c>
       <c r="B154" s="19" t="s">
@@ -5862,7 +5859,7 @@
     </row>
     <row r="155" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A155" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Earlydetection-screening</v>
       </c>
       <c r="B155" s="19" t="s">
@@ -5891,7 +5888,7 @@
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A156" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Justice</v>
       </c>
       <c r="B156" s="19" t="s">
@@ -5920,7 +5917,7 @@
     </row>
     <row r="157" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A157" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Socialdomain</v>
       </c>
       <c r="B157" s="19" t="s">
@@ -5949,7 +5946,7 @@
     </row>
     <row r="158" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A158" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Youth</v>
       </c>
       <c r="B158" s="19" t="s">
@@ -5978,7 +5975,7 @@
     </row>
     <row r="159" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A159" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:SocialSupport</v>
       </c>
       <c r="B159" s="19" t="s">
@@ -6007,7 +6004,7 @@
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A160" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:SportDivhealthDivwellness</v>
       </c>
       <c r="B160" s="19" t="s">
@@ -6036,7 +6033,7 @@
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A161" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Disabledcare</v>
       </c>
       <c r="B161" s="19" t="s">
@@ -6065,7 +6062,7 @@
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A162" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Long-termmentalhealthcare</v>
       </c>
       <c r="B162" s="26" t="s">
@@ -6094,7 +6091,7 @@
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A163" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Youth-healthcare</v>
       </c>
       <c r="B163" s="26" t="s">
@@ -6123,7 +6120,7 @@
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A164" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Generalpractitionercare</v>
       </c>
       <c r="B164" s="19" t="s">
@@ -6152,7 +6149,7 @@
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A165" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Elderlycare</v>
       </c>
       <c r="B165" s="19" t="s">
@@ -6181,7 +6178,7 @@
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A166" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:ClientsandDivorpatientorganization</v>
       </c>
       <c r="B166" s="19" t="s">
@@ -6210,7 +6207,7 @@
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A167" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Measuringinstrument</v>
       </c>
       <c r="B167" s="19" t="s">
@@ -6239,7 +6236,7 @@
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A168" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Experimentalgarden</v>
       </c>
       <c r="B168" s="19" t="s">
@@ -6268,7 +6265,7 @@
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A169" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:OtherSetting</v>
       </c>
       <c r="B169" s="26" t="s">
@@ -6297,7 +6294,7 @@
     </row>
     <row r="170" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Institution</v>
       </c>
       <c r="B170" s="33" t="s">
@@ -6328,7 +6325,7 @@
     </row>
     <row r="171" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:Beroepsvereniging
 PraktijkverpleegkundigenenPraktijkondersteuners-V-VN</v>
       </c>
@@ -6358,7 +6355,7 @@
     </row>
     <row r="172" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:FederatievanMedischWetenschappelijke
 Verenigingen-FMWV</v>
       </c>
@@ -6388,7 +6385,7 @@
     </row>
     <row r="173" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:LandelijkeHuisartsenVereniging-LHV</v>
       </c>
       <c r="B173" s="26" t="s">
@@ -6417,7 +6414,7 @@
     </row>
     <row r="174" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:NederlandsHuisartsenGenootschap-NHG</v>
       </c>
       <c r="B174" s="26" t="s">
@@ -6446,7 +6443,7 @@
     </row>
     <row r="175" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:NederlandsOogheelkundigGezelschap-NOG</v>
       </c>
       <c r="B175" s="26" t="s">
@@ -6475,7 +6472,7 @@
     </row>
     <row r="176" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>zonmwpa:NederlandscheInternistenVereeniging-NIV</v>
       </c>
       <c r="B176" s="26" t="s">
@@ -6504,7 +6501,7 @@
     </row>
     <row r="177" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A177:A240" si="3">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B177," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
         <v>zonmwpa:Nederlandse
 OrthopaedischeVereniging-NOV</v>
       </c>
@@ -7344,7 +7341,7 @@
     <row r="205" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvanDietisten</v>
+        <v>zonmwpa:NederlandseVerenigingvanDiëtisten</v>
       </c>
       <c r="B205" s="31" t="s">
         <v>236</v>
@@ -7611,7 +7608,7 @@
     </row>
     <row r="214" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="26" t="str">
-        <f t="shared" ref="A214:A261" si="4">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B214," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorObstetrieen
 Gynaecologie-NVOG</v>
       </c>
@@ -7641,7 +7638,7 @@
     </row>
     <row r="215" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorPlastischeenReconstructieveChirurgie-NVPC</v>
       </c>
       <c r="B215" s="26" t="s">
@@ -7670,7 +7667,7 @@
     </row>
     <row r="216" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorPsychiatrie
 -NVVP</v>
       </c>
@@ -7700,7 +7697,7 @@
     </row>
     <row r="217" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorRadiologie
 -NVvR</v>
       </c>
@@ -7730,7 +7727,7 @@
     </row>
     <row r="218" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorRadiotherapie
 enOncologie-NVRO</v>
       </c>
@@ -7760,7 +7757,7 @@
     </row>
     <row r="219" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorThoraxchirurgie
 -NVT</v>
       </c>
@@ -7790,7 +7787,7 @@
     </row>
     <row r="220" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorUrologie-NVU</v>
       </c>
       <c r="B220" s="26" t="s">
@@ -7819,7 +7816,7 @@
     </row>
     <row r="221" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:VerenigingSpecialistenin
 Ouderengeneeskunde-Verenso</v>
       </c>
@@ -7849,7 +7846,7 @@
     </row>
     <row r="222" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:VerenigingvanEpidemiologie-VvE</v>
       </c>
       <c r="B222" s="26" t="s">
@@ -7878,7 +7875,7 @@
     </row>
     <row r="223" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:VerenigingvanMedisch
 WetenschappelijkeOnderzoekers-V.M.W.O.</v>
       </c>
@@ -7908,7 +7905,7 @@
     </row>
     <row r="224" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Verenigingvoor
 InformatieverwerkingindeZorg-VMBI</v>
       </c>
@@ -7938,7 +7935,7 @@
     </row>
     <row r="225" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Verenigingvoor
 Sportgeneeskunde</v>
       </c>
@@ -7968,7 +7965,7 @@
     </row>
     <row r="226" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:VerenigingvoorInfectieziekten-VIZ</v>
       </c>
       <c r="B226" s="26" t="s">
@@ -7997,7 +7994,7 @@
     </row>
     <row r="227" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Otherinstitution</v>
       </c>
       <c r="B227" s="31" t="s">
@@ -8026,15 +8023,15 @@
     </row>
     <row r="228" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:FocusArea</v>
       </c>
       <c r="B228" s="33" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C228" s="16"/>
       <c r="D228" s="33" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E228" s="17"/>
       <c r="F228" s="16" t="s">
@@ -8057,7 +8054,7 @@
     </row>
     <row r="229" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Predictivediagnosticsandtreatment</v>
       </c>
       <c r="B229" s="31" t="s">
@@ -8086,7 +8083,7 @@
     </row>
     <row r="230" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Careandprevention</v>
       </c>
       <c r="B230" s="31" t="s">
@@ -8115,7 +8112,7 @@
     </row>
     <row r="231" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A231" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Effectsonsociety</v>
       </c>
       <c r="B231" s="31" t="s">
@@ -8144,7 +8141,7 @@
     </row>
     <row r="232" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:OtherFocusArea</v>
       </c>
       <c r="B232" s="31" t="s">
@@ -8173,7 +8170,7 @@
     </row>
     <row r="233" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A233" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Theme</v>
       </c>
       <c r="B233" s="33" t="s">
@@ -8181,7 +8178,7 @@
       </c>
       <c r="C233" s="16"/>
       <c r="D233" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E233" s="17"/>
       <c r="F233" s="16" t="s">
@@ -8204,7 +8201,7 @@
     </row>
     <row r="234" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Treatment</v>
       </c>
       <c r="B234" s="31" t="s">
@@ -8233,7 +8230,7 @@
     </row>
     <row r="235" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A235" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Diagnosticsofinfection</v>
       </c>
       <c r="B235" s="31" t="s">
@@ -8262,7 +8259,7 @@
     </row>
     <row r="236" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A236" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Riskanalysisandprognostics</v>
       </c>
       <c r="B236" s="31" t="s">
@@ -8291,7 +8288,7 @@
     </row>
     <row r="237" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A237" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Virus-immunity-immuneresponseandpathogenesis</v>
       </c>
       <c r="B237" s="31" t="s">
@@ -8320,7 +8317,7 @@
     </row>
     <row r="238" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A238" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Clinicaltreatment</v>
       </c>
       <c r="B238" s="31" t="s">
@@ -8349,7 +8346,7 @@
     </row>
     <row r="239" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A239" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Animalfreeinnovations</v>
       </c>
       <c r="B239" s="31" t="s">
@@ -8378,7 +8375,7 @@
     </row>
     <row r="240" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A240" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>zonmwpa:Organisationofcareandprevention</v>
       </c>
       <c r="B240" s="31" t="s">
@@ -8407,7 +8404,7 @@
     </row>
     <row r="241" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A241" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A241:A261" si="4">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B241," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
         <v>zonmwpa:Careandpreventionforvulnerablecitizens</v>
       </c>
       <c r="B241" s="31" t="s">

</xml_diff>

<commit_message>
another try at \u000A
</commit_message>
<xml_diff>
--- a/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
+++ b/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/fair-data-collective/zonmw-project-admin/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB2D2FC-59CD-5A4F-94DB-451CB6A049B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4699ACF-6FCD-624B-A48A-9964E9111800}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="46900" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="46900" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-termilogy" sheetId="1" r:id="rId1"/>
@@ -662,14 +662,6 @@
     <t>Economic resilience</t>
   </si>
   <si>
-    <t>Beroepsvereniging
-Praktijkverpleegkundigen enPraktijkondersteuners (V&amp;VN)</t>
-  </si>
-  <si>
-    <t>Federatie van Medisch Wetenschappelijke
-Verenigingen (FMWV)</t>
-  </si>
-  <si>
     <t>Landelijke Huisartsen Vereniging (LHV)</t>
   </si>
   <si>
@@ -682,196 +674,24 @@
     <t>Nederlandsche Internisten Vereeniging (NIV)</t>
   </si>
   <si>
-    <t>Nederlandse
-Orthopaedische Vereniging (NOV)</t>
-  </si>
-  <si>
     <t>Nederlandse Genetische Vereniging (NGV)</t>
   </si>
   <si>
-    <t>Nederlandse Vereniging
-Celbiologie (NVvC)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-van Artsen voor Revalidatie en Physische Geneeskunde</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-van Biochemie en Moleculaire Biologie (NVBMB)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Allergologie (NVVA)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Arbeids- en Bedrijfsgeneeskunde (NVAB)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Duikgeneeskunde (NVD)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Fysiologie (NVF)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Gentherapie (NVGT)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Hematologie (NVvH)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Humane Genetica (NVHG)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Immunologie (NVVI)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Kindergeneeskunde (NVK)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Klinische Chemie en Laboratoriumgeneeskunde (NVKC)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Klinische Farmacologie en Biofarmacie</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Klinische Geriatrie (NVKG)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Medische Microbiologie (NVMM)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Medische Oncologie (NVMO)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Oncologie (NVvO)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Parasitologie (NVP)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Pathologie (NVVP)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Proefdierkunde (NVP)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging
-voor Reumatologie (NVR)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging Keel-Neus-Oorheelkunde
-en Heelkunde van het Hoofd Halsgebied</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging v.
-Neuropathologie (NVVNP)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging van Artsen voor
-Longziekten en Tuberculose (NVALT)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging van Artsen voor
-Verstandelijk Gehandicapten</t>
-  </si>
-  <si>
     <t>Nederlandse Vereniging van Diëtisten</t>
   </si>
   <si>
-    <t>Nederlandse Vereniging van Maag-, Darm- en
-Leverartsen (MDL)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging van Neurochirurgen
-(NVVN)</t>
-  </si>
-  <si>
     <t>Nederlandse Vereniging van Neurologie (NVN)</t>
   </si>
   <si>
-    <t>Nederlandse Vereniging voor
-Verzekeringsgeneeskunde (NVVG)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging voor Anesthesiologie
-(NAV)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging voor Dermatologie en
-Venereologie (NVDV)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging voor Heelkunde
-(NVvH)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging voor Nucleaire
-Geneeskunde (NVNG)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging voor Obstetrie en
-Gynaecologie (NVOG)</t>
-  </si>
-  <si>
     <t>Nederlandse Vereniging voor Plastische en Reconstructieve Chirurgie (NVPC)</t>
   </si>
   <si>
-    <t>Nederlandse Vereniging voor Psychiatrie
-(NVVP)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging voor Radiologie
-(NVvR)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging voor Radiotherapie
-en Oncologie (NVRO)</t>
-  </si>
-  <si>
-    <t>Nederlandse Vereniging voor Thoraxchirurgie
-(NVT)</t>
-  </si>
-  <si>
     <t>Nederlandse Vereniging voor Urologie (NVU)</t>
   </si>
   <si>
-    <t>Vereniging Specialisten in
-Ouderengeneeskunde (Verenso)</t>
-  </si>
-  <si>
     <t>Vereniging van Epidemiologie (VvE)</t>
   </si>
   <si>
-    <t>Vereniging van Medisch
-Wetenschappelijke Onderzoekers (V.M.W.O.)</t>
-  </si>
-  <si>
-    <t>Vereniging voor
-Informatieverwerking in de Zorg (VMBI)</t>
-  </si>
-  <si>
-    <t>Vereniging voor
-Sportgeneeskunde</t>
-  </si>
-  <si>
     <t>Vereniging voor Infectieziekten (VIZ)</t>
   </si>
   <si>
@@ -984,6 +804,141 @@
   </si>
   <si>
     <t>2020-10-30T13:43:00+00:00</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging van Artsen voor Revalidatie en Physische Geneeskunde</t>
+  </si>
+  <si>
+    <t>Beroepsvereniging Praktijkverpleegkundigen enPraktijkondersteuners (V&amp;VN)</t>
+  </si>
+  <si>
+    <t>Federatie van Medisch Wetenschappelijke Verenigingen (FMWV)</t>
+  </si>
+  <si>
+    <t>Nederlandse Orthopaedische Vereniging (NOV)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging Celbiologie (NVvC)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging van Biochemie en Moleculaire Biologie (NVBMB)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Allergologie (NVVA)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Arbeids- en Bedrijfsgeneeskunde (NVAB)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Duikgeneeskunde (NVD)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Fysiologie (NVF)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Gentherapie (NVGT)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Hematologie (NVvH)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Humane Genetica (NVHG)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Immunologie (NVVI)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Kindergeneeskunde (NVK)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Klinische Chemie en Laboratoriumgeneeskunde (NVKC)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Klinische Farmacologie en Biofarmacie</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Klinische Geriatrie (NVKG)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Medische Microbiologie (NVMM)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Medische Oncologie (NVMO)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Oncologie (NVvO)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Parasitologie (NVP)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Pathologie (NVVP)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Reumatologie (NVR)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Proefdierkunde (NVP)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging Keel-Neus-Oorheelkunde en Heelkunde van het Hoofd Halsgebied</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging v. Neuropathologie (NVVNP)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging van Artsen voor Longziekten en Tuberculose (NVALT)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging van Artsen voor Verstandelijk Gehandicapten</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging van Maag-, Darm- en Leverartsen (MDL)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging van Neurochirurgen (NVVN)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Verzekeringsgeneeskunde (NVVG)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Anesthesiologie (NAV)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Dermatologie en Venereologie (NVDV)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Heelkunde (NVvH)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Nucleaire Geneeskunde (NVNG)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Obstetrie en Gynaecologie (NVOG)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Psychiatrie (NVVP)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Radiologie (NVvR)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Radiotherapie en Oncologie (NVRO)</t>
+  </si>
+  <si>
+    <t>Nederlandse Vereniging voor Thoraxchirurgie (NVT)</t>
+  </si>
+  <si>
+    <t>Vereniging Specialisten in Ouderengeneeskunde (Verenso)</t>
+  </si>
+  <si>
+    <t>Vereniging van Medisch Wetenschappelijke Onderzoekers (V.M.W.O.)</t>
+  </si>
+  <si>
+    <t>Vereniging voor Informatieverwerking in de Zorg (VMBI)</t>
+  </si>
+  <si>
+    <t>Vereniging voor Sportgeneeskunde</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1202,6 +1157,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1422,14 +1380,14 @@
   </sheetPr>
   <dimension ref="A1:T1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="96" workbookViewId="0">
+      <selection activeCell="B227" sqref="B227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60.42578125" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="81.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.28515625" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" customWidth="1"/>
     <col min="6" max="6" width="40.7109375" customWidth="1"/>
@@ -1657,7 +1615,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>293</v>
+        <v>248</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1683,7 +1641,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>294</v>
+        <v>249</v>
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="3"/>
@@ -1709,7 +1667,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>294</v>
+        <v>249</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="3"/>
@@ -2485,11 +2443,11 @@
         <v>zonmwpa:Service</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>278</v>
+        <v>233</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="33" t="s">
-        <v>279</v>
+        <v>234</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="15" t="s">
@@ -2521,7 +2479,7 @@
       <c r="C40" s="27"/>
       <c r="D40" s="19"/>
       <c r="E40" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F40" s="27"/>
       <c r="G40" s="27"/>
@@ -2550,7 +2508,7 @@
       <c r="C41" s="27"/>
       <c r="D41" s="19"/>
       <c r="E41" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F41" s="27"/>
       <c r="G41" s="27"/>
@@ -2579,7 +2537,7 @@
       <c r="C42" s="27"/>
       <c r="D42" s="19"/>
       <c r="E42" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
@@ -2608,7 +2566,7 @@
       <c r="C43" s="27"/>
       <c r="D43" s="19"/>
       <c r="E43" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F43" s="27"/>
       <c r="G43" s="27"/>
@@ -2637,7 +2595,7 @@
       <c r="C44" s="27"/>
       <c r="D44" s="19"/>
       <c r="E44" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F44" s="27"/>
       <c r="G44" s="27"/>
@@ -2666,7 +2624,7 @@
       <c r="C45" s="27"/>
       <c r="D45" s="19"/>
       <c r="E45" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F45" s="27"/>
       <c r="G45" s="27"/>
@@ -2695,7 +2653,7 @@
       <c r="C46" s="27"/>
       <c r="D46" s="19"/>
       <c r="E46" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F46" s="27"/>
       <c r="G46" s="27"/>
@@ -2724,7 +2682,7 @@
       <c r="C47" s="27"/>
       <c r="D47" s="19"/>
       <c r="E47" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F47" s="27"/>
       <c r="G47" s="27"/>
@@ -2753,7 +2711,7 @@
       <c r="C48" s="27"/>
       <c r="D48" s="19"/>
       <c r="E48" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F48" s="27"/>
       <c r="G48" s="27"/>
@@ -2782,7 +2740,7 @@
       <c r="C49" s="27"/>
       <c r="D49" s="19"/>
       <c r="E49" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F49" s="27"/>
       <c r="G49" s="27"/>
@@ -2811,7 +2769,7 @@
       <c r="C50" s="27"/>
       <c r="D50" s="26"/>
       <c r="E50" s="35" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="F50" s="27"/>
       <c r="G50" s="28"/>
@@ -2835,11 +2793,11 @@
         <v>zonmwpa:TypeOfMaterial</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>286</v>
+        <v>241</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="33" t="s">
-        <v>281</v>
+        <v>236</v>
       </c>
       <c r="E51" s="17"/>
       <c r="F51" s="15" t="s">
@@ -2871,7 +2829,7 @@
       <c r="C52" s="27"/>
       <c r="D52" s="19"/>
       <c r="E52" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
@@ -2900,7 +2858,7 @@
       <c r="C53" s="27"/>
       <c r="D53" s="19"/>
       <c r="E53" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F53" s="27"/>
       <c r="G53" s="27"/>
@@ -2929,7 +2887,7 @@
       <c r="C54" s="27"/>
       <c r="D54" s="19"/>
       <c r="E54" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F54" s="27"/>
       <c r="G54" s="27"/>
@@ -2958,7 +2916,7 @@
       <c r="C55" s="27"/>
       <c r="D55" s="19"/>
       <c r="E55" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F55" s="27"/>
       <c r="G55" s="27"/>
@@ -2987,7 +2945,7 @@
       <c r="C56" s="27"/>
       <c r="D56" s="19"/>
       <c r="E56" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F56" s="27"/>
       <c r="G56" s="27"/>
@@ -3016,7 +2974,7 @@
       <c r="C57" s="27"/>
       <c r="D57" s="19"/>
       <c r="E57" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F57" s="27"/>
       <c r="G57" s="27"/>
@@ -3045,7 +3003,7 @@
       <c r="C58" s="27"/>
       <c r="D58" s="19"/>
       <c r="E58" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F58" s="27"/>
       <c r="G58" s="27"/>
@@ -3074,7 +3032,7 @@
       <c r="C59" s="27"/>
       <c r="D59" s="19"/>
       <c r="E59" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F59" s="27"/>
       <c r="G59" s="27"/>
@@ -3103,7 +3061,7 @@
       <c r="C60" s="27"/>
       <c r="D60" s="19"/>
       <c r="E60" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F60" s="27"/>
       <c r="G60" s="27"/>
@@ -3132,7 +3090,7 @@
       <c r="C61" s="27"/>
       <c r="D61" s="19"/>
       <c r="E61" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F61" s="27"/>
       <c r="G61" s="27"/>
@@ -3161,7 +3119,7 @@
       <c r="C62" s="27"/>
       <c r="D62" s="19"/>
       <c r="E62" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F62" s="27"/>
       <c r="G62" s="27"/>
@@ -3190,7 +3148,7 @@
       <c r="C63" s="27"/>
       <c r="D63" s="19"/>
       <c r="E63" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F63" s="27"/>
       <c r="G63" s="27"/>
@@ -3219,7 +3177,7 @@
       <c r="C64" s="27"/>
       <c r="D64" s="19"/>
       <c r="E64" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F64" s="27"/>
       <c r="G64" s="27"/>
@@ -3248,7 +3206,7 @@
       <c r="C65" s="27"/>
       <c r="D65" s="19"/>
       <c r="E65" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F65" s="27"/>
       <c r="G65" s="27"/>
@@ -3277,7 +3235,7 @@
       <c r="C66" s="27"/>
       <c r="D66" s="19"/>
       <c r="E66" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F66" s="27"/>
       <c r="G66" s="27"/>
@@ -3306,7 +3264,7 @@
       <c r="C67" s="27"/>
       <c r="D67" s="19"/>
       <c r="E67" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F67" s="27"/>
       <c r="G67" s="27"/>
@@ -3335,7 +3293,7 @@
       <c r="C68" s="27"/>
       <c r="D68" s="19"/>
       <c r="E68" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F68" s="27"/>
       <c r="G68" s="27"/>
@@ -3364,7 +3322,7 @@
       <c r="C69" s="27"/>
       <c r="D69" s="19"/>
       <c r="E69" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F69" s="27"/>
       <c r="G69" s="27"/>
@@ -3393,7 +3351,7 @@
       <c r="C70" s="27"/>
       <c r="D70" s="19"/>
       <c r="E70" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F70" s="27"/>
       <c r="G70" s="27"/>
@@ -3422,7 +3380,7 @@
       <c r="C71" s="27"/>
       <c r="D71" s="19"/>
       <c r="E71" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F71" s="27"/>
       <c r="G71" s="27"/>
@@ -3451,7 +3409,7 @@
       <c r="C72" s="27"/>
       <c r="D72" s="26"/>
       <c r="E72" s="34" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="F72" s="27"/>
       <c r="G72" s="28"/>
@@ -3475,11 +3433,11 @@
         <v>zonmwpa:TypeOfData</v>
       </c>
       <c r="B73" s="33" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="33" t="s">
-        <v>283</v>
+        <v>238</v>
       </c>
       <c r="E73" s="17"/>
       <c r="F73" s="15" t="s">
@@ -3511,7 +3469,7 @@
       <c r="C74" s="27"/>
       <c r="D74" s="19"/>
       <c r="E74" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F74" s="27"/>
       <c r="G74" s="27"/>
@@ -3540,7 +3498,7 @@
       <c r="C75" s="27"/>
       <c r="D75" s="19"/>
       <c r="E75" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F75" s="27"/>
       <c r="G75" s="27"/>
@@ -3569,7 +3527,7 @@
       <c r="C76" s="27"/>
       <c r="D76" s="19"/>
       <c r="E76" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F76" s="27"/>
       <c r="G76" s="27"/>
@@ -3598,7 +3556,7 @@
       <c r="C77" s="27"/>
       <c r="D77" s="19"/>
       <c r="E77" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F77" s="27"/>
       <c r="G77" s="27"/>
@@ -3627,7 +3585,7 @@
       <c r="C78" s="27"/>
       <c r="D78" s="19"/>
       <c r="E78" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F78" s="27"/>
       <c r="G78" s="27"/>
@@ -3656,7 +3614,7 @@
       <c r="C79" s="27"/>
       <c r="D79" s="19"/>
       <c r="E79" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F79" s="27"/>
       <c r="G79" s="27"/>
@@ -3685,7 +3643,7 @@
       <c r="C80" s="27"/>
       <c r="D80" s="19"/>
       <c r="E80" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F80" s="27"/>
       <c r="G80" s="27"/>
@@ -3714,7 +3672,7 @@
       <c r="C81" s="27"/>
       <c r="D81" s="19"/>
       <c r="E81" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F81" s="27"/>
       <c r="G81" s="27"/>
@@ -3743,7 +3701,7 @@
       <c r="C82" s="27"/>
       <c r="D82" s="19"/>
       <c r="E82" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F82" s="27"/>
       <c r="G82" s="27"/>
@@ -3772,7 +3730,7 @@
       <c r="C83" s="27"/>
       <c r="D83" s="19"/>
       <c r="E83" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F83" s="27"/>
       <c r="G83" s="27"/>
@@ -3801,7 +3759,7 @@
       <c r="C84" s="27"/>
       <c r="D84" s="19"/>
       <c r="E84" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="27"/>
@@ -3830,7 +3788,7 @@
       <c r="C85" s="27"/>
       <c r="D85" s="19"/>
       <c r="E85" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F85" s="27"/>
       <c r="G85" s="27"/>
@@ -3859,7 +3817,7 @@
       <c r="C86" s="27"/>
       <c r="D86" s="19"/>
       <c r="E86" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F86" s="27"/>
       <c r="G86" s="27"/>
@@ -3888,7 +3846,7 @@
       <c r="C87" s="27"/>
       <c r="D87" s="19"/>
       <c r="E87" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F87" s="27"/>
       <c r="G87" s="27"/>
@@ -3917,7 +3875,7 @@
       <c r="C88" s="27"/>
       <c r="D88" s="26"/>
       <c r="E88" s="34" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F88" s="27"/>
       <c r="G88" s="28"/>
@@ -3941,11 +3899,11 @@
         <v>zonmwpa:TypeOfCollection</v>
       </c>
       <c r="B89" s="33" t="s">
-        <v>288</v>
+        <v>243</v>
       </c>
       <c r="C89" s="15"/>
       <c r="D89" s="33" t="s">
-        <v>287</v>
+        <v>242</v>
       </c>
       <c r="E89" s="17"/>
       <c r="F89" s="15" t="s">
@@ -3977,7 +3935,7 @@
       <c r="C90" s="27"/>
       <c r="D90" s="19"/>
       <c r="E90" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F90" s="27"/>
       <c r="G90" s="27"/>
@@ -4006,7 +3964,7 @@
       <c r="C91" s="27"/>
       <c r="D91" s="19"/>
       <c r="E91" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F91" s="27"/>
       <c r="G91" s="27"/>
@@ -4035,7 +3993,7 @@
       <c r="C92" s="27"/>
       <c r="D92" s="19"/>
       <c r="E92" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F92" s="27"/>
       <c r="G92" s="27"/>
@@ -4064,7 +4022,7 @@
       <c r="C93" s="27"/>
       <c r="D93" s="19"/>
       <c r="E93" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F93" s="27"/>
       <c r="G93" s="27"/>
@@ -4093,7 +4051,7 @@
       <c r="C94" s="27"/>
       <c r="D94" s="19"/>
       <c r="E94" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F94" s="27"/>
       <c r="G94" s="27"/>
@@ -4122,7 +4080,7 @@
       <c r="C95" s="27"/>
       <c r="D95" s="19"/>
       <c r="E95" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F95" s="27"/>
       <c r="G95" s="27"/>
@@ -4151,7 +4109,7 @@
       <c r="C96" s="27"/>
       <c r="D96" s="19"/>
       <c r="E96" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F96" s="27"/>
       <c r="G96" s="27"/>
@@ -4180,7 +4138,7 @@
       <c r="C97" s="27"/>
       <c r="D97" s="19"/>
       <c r="E97" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F97" s="27"/>
       <c r="G97" s="27"/>
@@ -4209,7 +4167,7 @@
       <c r="C98" s="27"/>
       <c r="D98" s="19"/>
       <c r="E98" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F98" s="27"/>
       <c r="G98" s="27"/>
@@ -4238,7 +4196,7 @@
       <c r="C99" s="27"/>
       <c r="D99" s="26"/>
       <c r="E99" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F99" s="27"/>
       <c r="G99" s="27"/>
@@ -4267,7 +4225,7 @@
       <c r="C100" s="27"/>
       <c r="D100" s="19"/>
       <c r="E100" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F100" s="27"/>
       <c r="G100" s="27"/>
@@ -4296,7 +4254,7 @@
       <c r="C101" s="27"/>
       <c r="D101" s="19"/>
       <c r="E101" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F101" s="27"/>
       <c r="G101" s="27"/>
@@ -4325,7 +4283,7 @@
       <c r="C102" s="27"/>
       <c r="D102" s="19"/>
       <c r="E102" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F102" s="27"/>
       <c r="G102" s="27"/>
@@ -4354,7 +4312,7 @@
       <c r="C103" s="27"/>
       <c r="D103" s="19"/>
       <c r="E103" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F103" s="27"/>
       <c r="G103" s="27"/>
@@ -4383,7 +4341,7 @@
       <c r="C104" s="27"/>
       <c r="D104" s="19"/>
       <c r="E104" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F104" s="27"/>
       <c r="G104" s="27"/>
@@ -4412,7 +4370,7 @@
       <c r="C105" s="27"/>
       <c r="D105" s="19"/>
       <c r="E105" s="34" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F105" s="27"/>
       <c r="G105" s="27"/>
@@ -6298,7 +6256,7 @@
         <v>zonmwpa:Institution</v>
       </c>
       <c r="B170" s="33" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="C170" s="16"/>
       <c r="D170" s="16" t="s">
@@ -6326,16 +6284,15 @@
     <row r="171" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Beroepsvereniging
-PraktijkverpleegkundigenenPraktijkondersteuners-V-VN</v>
-      </c>
-      <c r="B171" s="26" t="s">
-        <v>202</v>
+        <v>zonmwpa:BeroepsverenigingPraktijkverpleegkundigenenPraktijkondersteuners-V-VN</v>
+      </c>
+      <c r="B171" s="31" t="s">
+        <v>251</v>
       </c>
       <c r="C171" s="30"/>
       <c r="D171" s="26"/>
       <c r="E171" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F171" s="30"/>
       <c r="G171" s="30"/>
@@ -6356,16 +6313,15 @@
     <row r="172" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:FederatievanMedischWetenschappelijke
-Verenigingen-FMWV</v>
-      </c>
-      <c r="B172" s="26" t="s">
-        <v>203</v>
+        <v>zonmwpa:FederatievanMedischWetenschappelijkeVerenigingen-FMWV</v>
+      </c>
+      <c r="B172" s="31" t="s">
+        <v>252</v>
       </c>
       <c r="C172" s="30"/>
       <c r="D172" s="26"/>
       <c r="E172" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F172" s="30"/>
       <c r="G172" s="30"/>
@@ -6388,13 +6344,13 @@
         <f t="shared" si="2"/>
         <v>zonmwpa:LandelijkeHuisartsenVereniging-LHV</v>
       </c>
-      <c r="B173" s="26" t="s">
-        <v>204</v>
+      <c r="B173" s="31" t="s">
+        <v>202</v>
       </c>
       <c r="C173" s="30"/>
       <c r="D173" s="26"/>
       <c r="E173" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F173" s="30"/>
       <c r="G173" s="30"/>
@@ -6417,13 +6373,13 @@
         <f t="shared" si="2"/>
         <v>zonmwpa:NederlandsHuisartsenGenootschap-NHG</v>
       </c>
-      <c r="B174" s="26" t="s">
-        <v>205</v>
+      <c r="B174" s="31" t="s">
+        <v>203</v>
       </c>
       <c r="C174" s="30"/>
       <c r="D174" s="26"/>
       <c r="E174" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F174" s="30"/>
       <c r="G174" s="30"/>
@@ -6446,13 +6402,13 @@
         <f t="shared" si="2"/>
         <v>zonmwpa:NederlandsOogheelkundigGezelschap-NOG</v>
       </c>
-      <c r="B175" s="26" t="s">
-        <v>206</v>
+      <c r="B175" s="31" t="s">
+        <v>204</v>
       </c>
       <c r="C175" s="30"/>
       <c r="D175" s="26"/>
       <c r="E175" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F175" s="30"/>
       <c r="G175" s="30"/>
@@ -6475,13 +6431,13 @@
         <f t="shared" si="2"/>
         <v>zonmwpa:NederlandscheInternistenVereeniging-NIV</v>
       </c>
-      <c r="B176" s="26" t="s">
-        <v>207</v>
+      <c r="B176" s="31" t="s">
+        <v>205</v>
       </c>
       <c r="C176" s="30"/>
       <c r="D176" s="26"/>
       <c r="E176" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F176" s="30"/>
       <c r="G176" s="30"/>
@@ -6499,19 +6455,18 @@
       <c r="S176" s="3"/>
       <c r="T176" s="3"/>
     </row>
-    <row r="177" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="26" t="str">
-        <f t="shared" ref="A177:A240" si="3">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B177," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>zonmwpa:Nederlandse
-OrthopaedischeVereniging-NOV</v>
-      </c>
-      <c r="B177" s="26" t="s">
-        <v>208</v>
+        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B177," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>zonmwpa:NederlandseOrthopaedischeVereniging-NOV</v>
+      </c>
+      <c r="B177" s="39" t="s">
+        <v>253</v>
       </c>
       <c r="C177" s="30"/>
       <c r="D177" s="26"/>
       <c r="E177" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F177" s="30"/>
       <c r="G177" s="30"/>
@@ -6531,16 +6486,16 @@
     </row>
     <row r="178" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A177:A240" si="3">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B178," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
         <v>zonmwpa:NederlandseGenetischeVereniging-NGV</v>
       </c>
-      <c r="B178" s="26" t="s">
-        <v>209</v>
+      <c r="B178" s="31" t="s">
+        <v>206</v>
       </c>
       <c r="C178" s="30"/>
       <c r="D178" s="26"/>
       <c r="E178" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F178" s="30"/>
       <c r="G178" s="30"/>
@@ -6561,16 +6516,15 @@
     <row r="179" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-Celbiologie-NVvC</v>
-      </c>
-      <c r="B179" s="26" t="s">
-        <v>210</v>
+        <v>zonmwpa:NederlandseVerenigingCelbiologie-NVvC</v>
+      </c>
+      <c r="B179" s="31" t="s">
+        <v>254</v>
       </c>
       <c r="C179" s="30"/>
       <c r="D179" s="26"/>
       <c r="E179" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F179" s="30"/>
       <c r="G179" s="30"/>
@@ -6591,16 +6545,15 @@
     <row r="180" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-vanArtsenvoorRevalidatieenPhysischeGeneeskunde</v>
-      </c>
-      <c r="B180" s="26" t="s">
-        <v>211</v>
+        <v>zonmwpa:NederlandseVerenigingvanArtsenvoorRevalidatieenPhysischeGeneeskunde</v>
+      </c>
+      <c r="B180" s="31" t="s">
+        <v>250</v>
       </c>
       <c r="C180" s="30"/>
       <c r="D180" s="26"/>
       <c r="E180" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F180" s="30"/>
       <c r="G180" s="30"/>
@@ -6621,16 +6574,15 @@
     <row r="181" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-vanBiochemieenMoleculaireBiologie-NVBMB</v>
-      </c>
-      <c r="B181" s="26" t="s">
-        <v>212</v>
+        <v>zonmwpa:NederlandseVerenigingvanBiochemieenMoleculaireBiologie-NVBMB</v>
+      </c>
+      <c r="B181" s="31" t="s">
+        <v>255</v>
       </c>
       <c r="C181" s="30"/>
       <c r="D181" s="26"/>
       <c r="E181" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F181" s="30"/>
       <c r="G181" s="30"/>
@@ -6651,16 +6603,15 @@
     <row r="182" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorAllergologie-NVVA</v>
-      </c>
-      <c r="B182" s="26" t="s">
-        <v>213</v>
+        <v>zonmwpa:NederlandseVerenigingvoorAllergologie-NVVA</v>
+      </c>
+      <c r="B182" s="31" t="s">
+        <v>256</v>
       </c>
       <c r="C182" s="30"/>
       <c r="D182" s="26"/>
       <c r="E182" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F182" s="30"/>
       <c r="G182" s="30"/>
@@ -6681,16 +6632,15 @@
     <row r="183" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorArbeids-enBedrijfsgeneeskunde-NVAB</v>
-      </c>
-      <c r="B183" s="26" t="s">
-        <v>214</v>
+        <v>zonmwpa:NederlandseVerenigingvoorArbeids-enBedrijfsgeneeskunde-NVAB</v>
+      </c>
+      <c r="B183" s="31" t="s">
+        <v>257</v>
       </c>
       <c r="C183" s="30"/>
       <c r="D183" s="26"/>
       <c r="E183" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F183" s="30"/>
       <c r="G183" s="30"/>
@@ -6711,16 +6661,15 @@
     <row r="184" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorDuikgeneeskunde-NVD</v>
-      </c>
-      <c r="B184" s="26" t="s">
-        <v>215</v>
+        <v>zonmwpa:NederlandseVerenigingvoorDuikgeneeskunde-NVD</v>
+      </c>
+      <c r="B184" s="31" t="s">
+        <v>258</v>
       </c>
       <c r="C184" s="30"/>
       <c r="D184" s="26"/>
       <c r="E184" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F184" s="30"/>
       <c r="G184" s="30"/>
@@ -6741,16 +6690,15 @@
     <row r="185" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorFysiologie-NVF</v>
-      </c>
-      <c r="B185" s="26" t="s">
-        <v>216</v>
+        <v>zonmwpa:NederlandseVerenigingvoorFysiologie-NVF</v>
+      </c>
+      <c r="B185" s="31" t="s">
+        <v>259</v>
       </c>
       <c r="C185" s="30"/>
       <c r="D185" s="26"/>
       <c r="E185" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F185" s="30"/>
       <c r="G185" s="30"/>
@@ -6771,16 +6719,15 @@
     <row r="186" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorGentherapie-NVGT</v>
-      </c>
-      <c r="B186" s="26" t="s">
-        <v>217</v>
+        <v>zonmwpa:NederlandseVerenigingvoorGentherapie-NVGT</v>
+      </c>
+      <c r="B186" s="31" t="s">
+        <v>260</v>
       </c>
       <c r="C186" s="30"/>
       <c r="D186" s="26"/>
       <c r="E186" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F186" s="30"/>
       <c r="G186" s="30"/>
@@ -6801,16 +6748,15 @@
     <row r="187" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorHematologie-NVvH</v>
-      </c>
-      <c r="B187" s="26" t="s">
-        <v>218</v>
+        <v>zonmwpa:NederlandseVerenigingvoorHematologie-NVvH</v>
+      </c>
+      <c r="B187" s="31" t="s">
+        <v>261</v>
       </c>
       <c r="C187" s="30"/>
       <c r="D187" s="26"/>
       <c r="E187" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F187" s="30"/>
       <c r="G187" s="30"/>
@@ -6831,16 +6777,15 @@
     <row r="188" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorHumaneGenetica-NVHG</v>
-      </c>
-      <c r="B188" s="26" t="s">
-        <v>219</v>
+        <v>zonmwpa:NederlandseVerenigingvoorHumaneGenetica-NVHG</v>
+      </c>
+      <c r="B188" s="31" t="s">
+        <v>262</v>
       </c>
       <c r="C188" s="30"/>
       <c r="D188" s="26"/>
       <c r="E188" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F188" s="30"/>
       <c r="G188" s="30"/>
@@ -6861,16 +6806,15 @@
     <row r="189" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorImmunologie-NVVI</v>
-      </c>
-      <c r="B189" s="26" t="s">
-        <v>220</v>
+        <v>zonmwpa:NederlandseVerenigingvoorImmunologie-NVVI</v>
+      </c>
+      <c r="B189" s="31" t="s">
+        <v>263</v>
       </c>
       <c r="C189" s="30"/>
       <c r="D189" s="26"/>
       <c r="E189" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F189" s="30"/>
       <c r="G189" s="30"/>
@@ -6891,16 +6835,15 @@
     <row r="190" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorKindergeneeskunde-NVK</v>
-      </c>
-      <c r="B190" s="26" t="s">
-        <v>221</v>
+        <v>zonmwpa:NederlandseVerenigingvoorKindergeneeskunde-NVK</v>
+      </c>
+      <c r="B190" s="31" t="s">
+        <v>264</v>
       </c>
       <c r="C190" s="30"/>
       <c r="D190" s="26"/>
       <c r="E190" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F190" s="30"/>
       <c r="G190" s="30"/>
@@ -6921,16 +6864,15 @@
     <row r="191" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorKlinischeChemieenLaboratoriumgeneeskunde-NVKC</v>
-      </c>
-      <c r="B191" s="26" t="s">
-        <v>222</v>
+        <v>zonmwpa:NederlandseVerenigingvoorKlinischeChemieenLaboratoriumgeneeskunde-NVKC</v>
+      </c>
+      <c r="B191" s="31" t="s">
+        <v>265</v>
       </c>
       <c r="C191" s="30"/>
       <c r="D191" s="26"/>
       <c r="E191" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F191" s="30"/>
       <c r="G191" s="30"/>
@@ -6951,16 +6893,15 @@
     <row r="192" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorKlinischeFarmacologieenBiofarmacie</v>
-      </c>
-      <c r="B192" s="26" t="s">
-        <v>223</v>
+        <v>zonmwpa:NederlandseVerenigingvoorKlinischeFarmacologieenBiofarmacie</v>
+      </c>
+      <c r="B192" s="31" t="s">
+        <v>266</v>
       </c>
       <c r="C192" s="30"/>
       <c r="D192" s="26"/>
       <c r="E192" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F192" s="30"/>
       <c r="G192" s="30"/>
@@ -6981,16 +6922,15 @@
     <row r="193" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorKlinischeGeriatrie-NVKG</v>
-      </c>
-      <c r="B193" s="26" t="s">
-        <v>224</v>
+        <v>zonmwpa:NederlandseVerenigingvoorKlinischeGeriatrie-NVKG</v>
+      </c>
+      <c r="B193" s="31" t="s">
+        <v>267</v>
       </c>
       <c r="C193" s="30"/>
       <c r="D193" s="26"/>
       <c r="E193" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F193" s="30"/>
       <c r="G193" s="30"/>
@@ -7011,16 +6951,15 @@
     <row r="194" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorMedischeMicrobiologie-NVMM</v>
-      </c>
-      <c r="B194" s="26" t="s">
-        <v>225</v>
+        <v>zonmwpa:NederlandseVerenigingvoorMedischeMicrobiologie-NVMM</v>
+      </c>
+      <c r="B194" s="31" t="s">
+        <v>268</v>
       </c>
       <c r="C194" s="30"/>
       <c r="D194" s="26"/>
       <c r="E194" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F194" s="30"/>
       <c r="G194" s="30"/>
@@ -7041,16 +6980,15 @@
     <row r="195" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorMedischeOncologie-NVMO</v>
-      </c>
-      <c r="B195" s="26" t="s">
-        <v>226</v>
+        <v>zonmwpa:NederlandseVerenigingvoorMedischeOncologie-NVMO</v>
+      </c>
+      <c r="B195" s="31" t="s">
+        <v>269</v>
       </c>
       <c r="C195" s="30"/>
       <c r="D195" s="26"/>
       <c r="E195" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F195" s="30"/>
       <c r="G195" s="30"/>
@@ -7071,16 +7009,15 @@
     <row r="196" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorOncologie-NVvO</v>
-      </c>
-      <c r="B196" s="26" t="s">
-        <v>227</v>
+        <v>zonmwpa:NederlandseVerenigingvoorOncologie-NVvO</v>
+      </c>
+      <c r="B196" s="31" t="s">
+        <v>270</v>
       </c>
       <c r="C196" s="30"/>
       <c r="D196" s="26"/>
       <c r="E196" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F196" s="30"/>
       <c r="G196" s="30"/>
@@ -7101,16 +7038,15 @@
     <row r="197" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorParasitologie-NVP</v>
-      </c>
-      <c r="B197" s="26" t="s">
-        <v>228</v>
+        <v>zonmwpa:NederlandseVerenigingvoorParasitologie-NVP</v>
+      </c>
+      <c r="B197" s="31" t="s">
+        <v>271</v>
       </c>
       <c r="C197" s="30"/>
       <c r="D197" s="26"/>
       <c r="E197" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F197" s="30"/>
       <c r="G197" s="30"/>
@@ -7131,16 +7067,15 @@
     <row r="198" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorPathologie-NVVP</v>
-      </c>
-      <c r="B198" s="26" t="s">
-        <v>229</v>
+        <v>zonmwpa:NederlandseVerenigingvoorPathologie-NVVP</v>
+      </c>
+      <c r="B198" s="31" t="s">
+        <v>272</v>
       </c>
       <c r="C198" s="30"/>
       <c r="D198" s="26"/>
       <c r="E198" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F198" s="30"/>
       <c r="G198" s="30"/>
@@ -7161,16 +7096,15 @@
     <row r="199" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorProefdierkunde-NVP</v>
-      </c>
-      <c r="B199" s="26" t="s">
-        <v>230</v>
+        <v>zonmwpa:NederlandseVerenigingvoorProefdierkunde-NVP</v>
+      </c>
+      <c r="B199" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="C199" s="30"/>
       <c r="D199" s="26"/>
       <c r="E199" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F199" s="30"/>
       <c r="G199" s="30"/>
@@ -7191,16 +7125,15 @@
     <row r="200" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVereniging
-voorReumatologie-NVR</v>
-      </c>
-      <c r="B200" s="26" t="s">
-        <v>231</v>
+        <v>zonmwpa:NederlandseVerenigingvoorReumatologie-NVR</v>
+      </c>
+      <c r="B200" s="31" t="s">
+        <v>273</v>
       </c>
       <c r="C200" s="30"/>
       <c r="D200" s="26"/>
       <c r="E200" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F200" s="30"/>
       <c r="G200" s="30"/>
@@ -7221,16 +7154,15 @@
     <row r="201" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingKeel-Neus-Oorheelkunde
-enHeelkundevanhetHoofdHalsgebied</v>
-      </c>
-      <c r="B201" s="26" t="s">
-        <v>232</v>
+        <v>zonmwpa:NederlandseVerenigingKeel-Neus-OorheelkundeenHeelkundevanhetHoofdHalsgebied</v>
+      </c>
+      <c r="B201" s="31" t="s">
+        <v>275</v>
       </c>
       <c r="C201" s="30"/>
       <c r="D201" s="26"/>
       <c r="E201" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F201" s="30"/>
       <c r="G201" s="30"/>
@@ -7251,16 +7183,15 @@
     <row r="202" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingv.
-Neuropathologie-NVVNP</v>
-      </c>
-      <c r="B202" s="26" t="s">
-        <v>233</v>
+        <v>zonmwpa:NederlandseVerenigingv.Neuropathologie-NVVNP</v>
+      </c>
+      <c r="B202" s="31" t="s">
+        <v>276</v>
       </c>
       <c r="C202" s="30"/>
       <c r="D202" s="26"/>
       <c r="E202" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F202" s="30"/>
       <c r="G202" s="30"/>
@@ -7281,16 +7212,15 @@
     <row r="203" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvanArtsenvoor
-LongziektenenTuberculose-NVALT</v>
-      </c>
-      <c r="B203" s="26" t="s">
-        <v>234</v>
+        <v>zonmwpa:NederlandseVerenigingvanArtsenvoorLongziektenenTuberculose-NVALT</v>
+      </c>
+      <c r="B203" s="31" t="s">
+        <v>277</v>
       </c>
       <c r="C203" s="30"/>
       <c r="D203" s="26"/>
       <c r="E203" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F203" s="30"/>
       <c r="G203" s="30"/>
@@ -7311,16 +7241,15 @@
     <row r="204" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvanArtsenvoor
-VerstandelijkGehandicapten</v>
-      </c>
-      <c r="B204" s="26" t="s">
-        <v>235</v>
+        <v>zonmwpa:NederlandseVerenigingvanArtsenvoorVerstandelijkGehandicapten</v>
+      </c>
+      <c r="B204" s="31" t="s">
+        <v>278</v>
       </c>
       <c r="C204" s="30"/>
       <c r="D204" s="26"/>
       <c r="E204" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F204" s="30"/>
       <c r="G204" s="30"/>
@@ -7344,12 +7273,12 @@
         <v>zonmwpa:NederlandseVerenigingvanDiëtisten</v>
       </c>
       <c r="B205" s="31" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="C205" s="30"/>
       <c r="D205" s="26"/>
       <c r="E205" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F205" s="30"/>
       <c r="G205" s="30"/>
@@ -7370,16 +7299,15 @@
     <row r="206" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvanMaag-Darm-en
-Leverartsen-MDL</v>
-      </c>
-      <c r="B206" s="26" t="s">
-        <v>237</v>
+        <v>zonmwpa:NederlandseVerenigingvanMaag-Darm-enLeverartsen-MDL</v>
+      </c>
+      <c r="B206" s="31" t="s">
+        <v>279</v>
       </c>
       <c r="C206" s="30"/>
       <c r="D206" s="26"/>
       <c r="E206" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F206" s="30"/>
       <c r="G206" s="30"/>
@@ -7400,16 +7328,15 @@
     <row r="207" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvanNeurochirurgen
--NVVN</v>
-      </c>
-      <c r="B207" s="26" t="s">
-        <v>238</v>
+        <v>zonmwpa:NederlandseVerenigingvanNeurochirurgen-NVVN</v>
+      </c>
+      <c r="B207" s="31" t="s">
+        <v>280</v>
       </c>
       <c r="C207" s="30"/>
       <c r="D207" s="26"/>
       <c r="E207" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F207" s="30"/>
       <c r="G207" s="30"/>
@@ -7432,13 +7359,13 @@
         <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvanNeurologie-NVN</v>
       </c>
-      <c r="B208" s="26" t="s">
-        <v>239</v>
+      <c r="B208" s="31" t="s">
+        <v>208</v>
       </c>
       <c r="C208" s="30"/>
       <c r="D208" s="26"/>
       <c r="E208" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F208" s="30"/>
       <c r="G208" s="30"/>
@@ -7459,16 +7386,15 @@
     <row r="209" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoor
-Verzekeringsgeneeskunde-NVVG</v>
-      </c>
-      <c r="B209" s="26" t="s">
-        <v>240</v>
+        <v>zonmwpa:NederlandseVerenigingvoorVerzekeringsgeneeskunde-NVVG</v>
+      </c>
+      <c r="B209" s="31" t="s">
+        <v>281</v>
       </c>
       <c r="C209" s="30"/>
       <c r="D209" s="26"/>
       <c r="E209" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F209" s="30"/>
       <c r="G209" s="30"/>
@@ -7489,16 +7415,15 @@
     <row r="210" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoorAnesthesiologie
--NAV</v>
-      </c>
-      <c r="B210" s="26" t="s">
-        <v>241</v>
+        <v>zonmwpa:NederlandseVerenigingvoorAnesthesiologie-NAV</v>
+      </c>
+      <c r="B210" s="31" t="s">
+        <v>282</v>
       </c>
       <c r="C210" s="30"/>
       <c r="D210" s="26"/>
       <c r="E210" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F210" s="30"/>
       <c r="G210" s="30"/>
@@ -7519,16 +7444,15 @@
     <row r="211" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoorDermatologieen
-Venereologie-NVDV</v>
-      </c>
-      <c r="B211" s="26" t="s">
-        <v>242</v>
+        <v>zonmwpa:NederlandseVerenigingvoorDermatologieenVenereologie-NVDV</v>
+      </c>
+      <c r="B211" s="31" t="s">
+        <v>283</v>
       </c>
       <c r="C211" s="30"/>
       <c r="D211" s="26"/>
       <c r="E211" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F211" s="30"/>
       <c r="G211" s="30"/>
@@ -7549,16 +7473,15 @@
     <row r="212" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoorHeelkunde
--NVvH</v>
-      </c>
-      <c r="B212" s="26" t="s">
-        <v>243</v>
+        <v>zonmwpa:NederlandseVerenigingvoorHeelkunde-NVvH</v>
+      </c>
+      <c r="B212" s="31" t="s">
+        <v>284</v>
       </c>
       <c r="C212" s="30"/>
       <c r="D212" s="26"/>
       <c r="E212" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F212" s="30"/>
       <c r="G212" s="30"/>
@@ -7579,16 +7502,15 @@
     <row r="213" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoorNucleaire
-Geneeskunde-NVNG</v>
-      </c>
-      <c r="B213" s="26" t="s">
-        <v>244</v>
+        <v>zonmwpa:NederlandseVerenigingvoorNucleaireGeneeskunde-NVNG</v>
+      </c>
+      <c r="B213" s="31" t="s">
+        <v>285</v>
       </c>
       <c r="C213" s="30"/>
       <c r="D213" s="26"/>
       <c r="E213" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F213" s="30"/>
       <c r="G213" s="30"/>
@@ -7609,16 +7531,15 @@
     <row r="214" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoorObstetrieen
-Gynaecologie-NVOG</v>
-      </c>
-      <c r="B214" s="26" t="s">
-        <v>245</v>
+        <v>zonmwpa:NederlandseVerenigingvoorObstetrieenGynaecologie-NVOG</v>
+      </c>
+      <c r="B214" s="31" t="s">
+        <v>286</v>
       </c>
       <c r="C214" s="30"/>
       <c r="D214" s="26"/>
       <c r="E214" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F214" s="30"/>
       <c r="G214" s="30"/>
@@ -7641,13 +7562,13 @@
         <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorPlastischeenReconstructieveChirurgie-NVPC</v>
       </c>
-      <c r="B215" s="26" t="s">
-        <v>246</v>
+      <c r="B215" s="31" t="s">
+        <v>209</v>
       </c>
       <c r="C215" s="30"/>
       <c r="D215" s="26"/>
       <c r="E215" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F215" s="30"/>
       <c r="G215" s="30"/>
@@ -7668,16 +7589,15 @@
     <row r="216" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoorPsychiatrie
--NVVP</v>
-      </c>
-      <c r="B216" s="26" t="s">
-        <v>247</v>
+        <v>zonmwpa:NederlandseVerenigingvoorPsychiatrie-NVVP</v>
+      </c>
+      <c r="B216" s="31" t="s">
+        <v>287</v>
       </c>
       <c r="C216" s="30"/>
       <c r="D216" s="26"/>
       <c r="E216" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F216" s="30"/>
       <c r="G216" s="30"/>
@@ -7698,16 +7618,15 @@
     <row r="217" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoorRadiologie
--NVvR</v>
-      </c>
-      <c r="B217" s="26" t="s">
-        <v>248</v>
+        <v>zonmwpa:NederlandseVerenigingvoorRadiologie-NVvR</v>
+      </c>
+      <c r="B217" s="31" t="s">
+        <v>288</v>
       </c>
       <c r="C217" s="30"/>
       <c r="D217" s="26"/>
       <c r="E217" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F217" s="30"/>
       <c r="G217" s="30"/>
@@ -7728,16 +7647,15 @@
     <row r="218" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoorRadiotherapie
-enOncologie-NVRO</v>
-      </c>
-      <c r="B218" s="26" t="s">
-        <v>249</v>
+        <v>zonmwpa:NederlandseVerenigingvoorRadiotherapieenOncologie-NVRO</v>
+      </c>
+      <c r="B218" s="31" t="s">
+        <v>289</v>
       </c>
       <c r="C218" s="30"/>
       <c r="D218" s="26"/>
       <c r="E218" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F218" s="30"/>
       <c r="G218" s="30"/>
@@ -7758,16 +7676,15 @@
     <row r="219" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NederlandseVerenigingvoorThoraxchirurgie
--NVT</v>
-      </c>
-      <c r="B219" s="26" t="s">
-        <v>250</v>
+        <v>zonmwpa:NederlandseVerenigingvoorThoraxchirurgie-NVT</v>
+      </c>
+      <c r="B219" s="31" t="s">
+        <v>290</v>
       </c>
       <c r="C219" s="30"/>
       <c r="D219" s="26"/>
       <c r="E219" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F219" s="30"/>
       <c r="G219" s="30"/>
@@ -7790,13 +7707,13 @@
         <f t="shared" si="3"/>
         <v>zonmwpa:NederlandseVerenigingvoorUrologie-NVU</v>
       </c>
-      <c r="B220" s="26" t="s">
-        <v>251</v>
+      <c r="B220" s="31" t="s">
+        <v>210</v>
       </c>
       <c r="C220" s="30"/>
       <c r="D220" s="26"/>
       <c r="E220" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F220" s="30"/>
       <c r="G220" s="30"/>
@@ -7817,16 +7734,15 @@
     <row r="221" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:VerenigingSpecialistenin
-Ouderengeneeskunde-Verenso</v>
-      </c>
-      <c r="B221" s="26" t="s">
-        <v>252</v>
+        <v>zonmwpa:VerenigingSpecialisteninOuderengeneeskunde-Verenso</v>
+      </c>
+      <c r="B221" s="31" t="s">
+        <v>291</v>
       </c>
       <c r="C221" s="30"/>
       <c r="D221" s="26"/>
       <c r="E221" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F221" s="30"/>
       <c r="G221" s="30"/>
@@ -7849,13 +7765,13 @@
         <f t="shared" si="3"/>
         <v>zonmwpa:VerenigingvanEpidemiologie-VvE</v>
       </c>
-      <c r="B222" s="26" t="s">
-        <v>253</v>
+      <c r="B222" s="31" t="s">
+        <v>211</v>
       </c>
       <c r="C222" s="30"/>
       <c r="D222" s="26"/>
       <c r="E222" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F222" s="30"/>
       <c r="G222" s="30"/>
@@ -7876,16 +7792,15 @@
     <row r="223" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:VerenigingvanMedisch
-WetenschappelijkeOnderzoekers-V.M.W.O.</v>
-      </c>
-      <c r="B223" s="26" t="s">
-        <v>254</v>
+        <v>zonmwpa:VerenigingvanMedischWetenschappelijkeOnderzoekers-V.M.W.O.</v>
+      </c>
+      <c r="B223" s="31" t="s">
+        <v>292</v>
       </c>
       <c r="C223" s="30"/>
       <c r="D223" s="26"/>
       <c r="E223" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F223" s="30"/>
       <c r="G223" s="30"/>
@@ -7906,16 +7821,15 @@
     <row r="224" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Verenigingvoor
-InformatieverwerkingindeZorg-VMBI</v>
-      </c>
-      <c r="B224" s="26" t="s">
-        <v>255</v>
+        <v>zonmwpa:VerenigingvoorInformatieverwerkingindeZorg-VMBI</v>
+      </c>
+      <c r="B224" s="31" t="s">
+        <v>293</v>
       </c>
       <c r="C224" s="30"/>
       <c r="D224" s="26"/>
       <c r="E224" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F224" s="30"/>
       <c r="G224" s="30"/>
@@ -7936,16 +7850,15 @@
     <row r="225" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Verenigingvoor
-Sportgeneeskunde</v>
-      </c>
-      <c r="B225" s="26" t="s">
-        <v>256</v>
+        <v>zonmwpa:VerenigingvoorSportgeneeskunde</v>
+      </c>
+      <c r="B225" s="31" t="s">
+        <v>294</v>
       </c>
       <c r="C225" s="30"/>
       <c r="D225" s="26"/>
       <c r="E225" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F225" s="30"/>
       <c r="G225" s="30"/>
@@ -7968,13 +7881,13 @@
         <f t="shared" si="3"/>
         <v>zonmwpa:VerenigingvoorInfectieziekten-VIZ</v>
       </c>
-      <c r="B226" s="26" t="s">
-        <v>257</v>
+      <c r="B226" s="31" t="s">
+        <v>212</v>
       </c>
       <c r="C226" s="30"/>
       <c r="D226" s="26"/>
       <c r="E226" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F226" s="30"/>
       <c r="G226" s="30"/>
@@ -7998,12 +7911,12 @@
         <v>zonmwpa:Otherinstitution</v>
       </c>
       <c r="B227" s="31" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="C227" s="30"/>
       <c r="D227" s="26"/>
       <c r="E227" s="34" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F227" s="30"/>
       <c r="G227" s="30"/>
@@ -8027,11 +7940,11 @@
         <v>zonmwpa:FocusArea</v>
       </c>
       <c r="B228" s="33" t="s">
-        <v>290</v>
+        <v>245</v>
       </c>
       <c r="C228" s="16"/>
       <c r="D228" s="33" t="s">
-        <v>291</v>
+        <v>246</v>
       </c>
       <c r="E228" s="17"/>
       <c r="F228" s="16" t="s">
@@ -8145,7 +8058,7 @@
         <v>zonmwpa:OtherFocusArea</v>
       </c>
       <c r="B232" s="31" t="s">
-        <v>274</v>
+        <v>229</v>
       </c>
       <c r="C232" s="30"/>
       <c r="D232" s="26"/>
@@ -8174,11 +8087,11 @@
         <v>zonmwpa:Theme</v>
       </c>
       <c r="B233" s="33" t="s">
-        <v>276</v>
+        <v>231</v>
       </c>
       <c r="C233" s="16"/>
       <c r="D233" s="33" t="s">
-        <v>292</v>
+        <v>247</v>
       </c>
       <c r="E233" s="17"/>
       <c r="F233" s="16" t="s">
@@ -8210,7 +8123,7 @@
       <c r="C234" s="30"/>
       <c r="D234" s="26"/>
       <c r="E234" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F234" s="30"/>
       <c r="G234" s="30"/>
@@ -8239,7 +8152,7 @@
       <c r="C235" s="30"/>
       <c r="D235" s="26"/>
       <c r="E235" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F235" s="30"/>
       <c r="G235" s="30"/>
@@ -8268,7 +8181,7 @@
       <c r="C236" s="30"/>
       <c r="D236" s="26"/>
       <c r="E236" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F236" s="30"/>
       <c r="G236" s="30"/>
@@ -8297,7 +8210,7 @@
       <c r="C237" s="30"/>
       <c r="D237" s="26"/>
       <c r="E237" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F237" s="30"/>
       <c r="G237" s="30"/>
@@ -8326,7 +8239,7 @@
       <c r="C238" s="30"/>
       <c r="D238" s="26"/>
       <c r="E238" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F238" s="30"/>
       <c r="G238" s="30"/>
@@ -8355,7 +8268,7 @@
       <c r="C239" s="30"/>
       <c r="D239" s="26"/>
       <c r="E239" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F239" s="30"/>
       <c r="G239" s="30"/>
@@ -8384,7 +8297,7 @@
       <c r="C240" s="30"/>
       <c r="D240" s="26"/>
       <c r="E240" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F240" s="30"/>
       <c r="G240" s="30"/>
@@ -8413,7 +8326,7 @@
       <c r="C241" s="30"/>
       <c r="D241" s="26"/>
       <c r="E241" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F241" s="30"/>
       <c r="G241" s="30"/>
@@ -8442,7 +8355,7 @@
       <c r="C242" s="30"/>
       <c r="D242" s="26"/>
       <c r="E242" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F242" s="30"/>
       <c r="G242" s="30"/>
@@ -8471,7 +8384,7 @@
       <c r="C243" s="30"/>
       <c r="D243" s="26"/>
       <c r="E243" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F243" s="30"/>
       <c r="G243" s="30"/>
@@ -8500,7 +8413,7 @@
       <c r="C244" s="30"/>
       <c r="D244" s="26"/>
       <c r="E244" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F244" s="30"/>
       <c r="G244" s="30"/>
@@ -8529,7 +8442,7 @@
       <c r="C245" s="30"/>
       <c r="D245" s="26"/>
       <c r="E245" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F245" s="30"/>
       <c r="G245" s="30"/>
@@ -8558,7 +8471,7 @@
       <c r="C246" s="30"/>
       <c r="D246" s="26"/>
       <c r="E246" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F246" s="30"/>
       <c r="G246" s="30"/>
@@ -8582,12 +8495,12 @@
         <v>zonmwpa:OtherTheme</v>
       </c>
       <c r="B247" s="31" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="C247" s="30"/>
       <c r="D247" s="26"/>
       <c r="E247" s="34" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="F247" s="30"/>
       <c r="G247" s="30"/>
@@ -8642,7 +8555,7 @@
         <v>zonmwpa:Drenthe</v>
       </c>
       <c r="B249" s="26" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="C249" s="30"/>
       <c r="D249" s="26"/>
@@ -8671,7 +8584,7 @@
         <v>zonmwpa:Flevoland</v>
       </c>
       <c r="B250" s="26" t="s">
-        <v>261</v>
+        <v>216</v>
       </c>
       <c r="C250" s="30"/>
       <c r="D250" s="26"/>
@@ -8700,7 +8613,7 @@
         <v>zonmwpa:Friesland</v>
       </c>
       <c r="B251" s="26" t="s">
-        <v>262</v>
+        <v>217</v>
       </c>
       <c r="C251" s="30"/>
       <c r="D251" s="26"/>
@@ -8729,7 +8642,7 @@
         <v>zonmwpa:Gelderland</v>
       </c>
       <c r="B252" s="26" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="C252" s="30"/>
       <c r="D252" s="26"/>
@@ -8758,7 +8671,7 @@
         <v>zonmwpa:Groningen</v>
       </c>
       <c r="B253" s="26" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="C253" s="30"/>
       <c r="D253" s="26"/>
@@ -8787,7 +8700,7 @@
         <v>zonmwpa:Limburg</v>
       </c>
       <c r="B254" s="26" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="C254" s="30"/>
       <c r="D254" s="26"/>
@@ -8816,7 +8729,7 @@
         <v>zonmwpa:Noord-Brabant</v>
       </c>
       <c r="B255" s="26" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="C255" s="30"/>
       <c r="D255" s="26"/>
@@ -8845,7 +8758,7 @@
         <v>zonmwpa:Noord-Holland</v>
       </c>
       <c r="B256" s="26" t="s">
-        <v>267</v>
+        <v>222</v>
       </c>
       <c r="C256" s="30"/>
       <c r="D256" s="26"/>
@@ -8874,7 +8787,7 @@
         <v>zonmwpa:Overijssel</v>
       </c>
       <c r="B257" s="26" t="s">
-        <v>268</v>
+        <v>223</v>
       </c>
       <c r="C257" s="30"/>
       <c r="D257" s="26"/>
@@ -8903,7 +8816,7 @@
         <v>zonmwpa:Utrecht</v>
       </c>
       <c r="B258" s="26" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="C258" s="30"/>
       <c r="D258" s="26"/>
@@ -8932,7 +8845,7 @@
         <v>zonmwpa:Zeeland</v>
       </c>
       <c r="B259" s="26" t="s">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="C259" s="30"/>
       <c r="D259" s="26"/>
@@ -8961,7 +8874,7 @@
         <v>zonmwpa:Zuid-Holland</v>
       </c>
       <c r="B260" s="26" t="s">
-        <v>271</v>
+        <v>226</v>
       </c>
       <c r="C260" s="30"/>
       <c r="D260" s="26"/>
@@ -8990,7 +8903,7 @@
         <v>zonmwpa:OtherProvince</v>
       </c>
       <c r="B261" s="31" t="s">
-        <v>272</v>
+        <v>227</v>
       </c>
       <c r="C261" s="30"/>
       <c r="D261" s="26"/>

</xml_diff>

<commit_message>
fix a label that lacked spaces
</commit_message>
<xml_diff>
--- a/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
+++ b/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/fair-data-collective/zonmw-project-admin/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19DA0CC-8014-2842-94C9-121B29EFC33C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F0F5C3-220F-9047-879C-6F3CFF0251D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="46900" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28660" yWindow="460" windowWidth="28400" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-termilogy" sheetId="1" r:id="rId1"/>
@@ -171,9 +171,6 @@
     <t>Neighbourhood</t>
   </si>
   <si>
-    <t>OtherStudyArea</t>
-  </si>
-  <si>
     <t>zonmwpa:SizeOfCollection</t>
   </si>
   <si>
@@ -913,13 +910,16 @@
   </si>
   <si>
     <t>1.2.0</t>
+  </si>
+  <si>
+    <t>Other Study Area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1019,6 +1019,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1079,7 +1086,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1150,6 +1157,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1370,8 +1378,8 @@
   </sheetPr>
   <dimension ref="A1:T1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1419,7 +1427,7 @@
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="40" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="3"/>
@@ -1605,7 +1613,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1631,7 +1639,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="3"/>
@@ -1657,7 +1665,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C11" s="36"/>
       <c r="D11" s="3"/>
@@ -2083,7 +2091,7 @@
         <v>zonmwpa:OtherStudyArea</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>38</v>
+        <v>285</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="26"/>
@@ -2112,11 +2120,11 @@
         <v>zonmwpa:SizeOfCollection</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="15" t="s">
@@ -2143,12 +2151,12 @@
         <v>zonmwpa:Under10</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="19"/>
       <c r="E29" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="28"/>
@@ -2172,12 +2180,12 @@
         <v>zonmwpa:10-100</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" s="19"/>
       <c r="E30" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F30" s="27"/>
       <c r="G30" s="28"/>
@@ -2201,12 +2209,12 @@
         <v>zonmwpa:100-1000</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="27"/>
       <c r="D31" s="19"/>
       <c r="E31" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F31" s="27"/>
       <c r="G31" s="28"/>
@@ -2230,12 +2238,12 @@
         <v>zonmwpa:1000-10.000</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="19"/>
       <c r="E32" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F32" s="27"/>
       <c r="G32" s="28"/>
@@ -2259,12 +2267,12 @@
         <v>zonmwpa:10.000-100.000</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="19"/>
       <c r="E33" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F33" s="27"/>
       <c r="G33" s="28"/>
@@ -2288,12 +2296,12 @@
         <v>zonmwpa:100.000-1.000.000</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="19"/>
       <c r="E34" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F34" s="27"/>
       <c r="G34" s="28"/>
@@ -2317,12 +2325,12 @@
         <v>zonmwpa:1.000.000-10.000.000</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="19"/>
       <c r="E35" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F35" s="27"/>
       <c r="G35" s="28"/>
@@ -2346,12 +2354,12 @@
         <v>zonmwpa:10.000.000-100.000.000</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="19"/>
       <c r="E36" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F36" s="27"/>
       <c r="G36" s="28"/>
@@ -2375,12 +2383,12 @@
         <v>zonmwpa:100.000.000-1.000.000.000</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="19"/>
       <c r="E37" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F37" s="29"/>
       <c r="G37" s="28"/>
@@ -2404,12 +2412,12 @@
         <v>zonmwpa:OtherSizeOfCollection</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C38" s="27"/>
       <c r="D38" s="26"/>
       <c r="E38" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F38" s="27"/>
       <c r="G38" s="28"/>
@@ -2433,11 +2441,11 @@
         <v>zonmwpa:Service</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="15" t="s">
@@ -2464,12 +2472,12 @@
         <v>zonmwpa:BSL-2laboratoriesavailable</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="19"/>
       <c r="E40" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F40" s="27"/>
       <c r="G40" s="27"/>
@@ -2493,12 +2501,12 @@
         <v>zonmwpa:BSL-3laboratoriesavailable</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="27"/>
       <c r="D41" s="19"/>
       <c r="E41" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F41" s="27"/>
       <c r="G41" s="27"/>
@@ -2522,12 +2530,12 @@
         <v>zonmwpa:MemberCOVID-19Network</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" s="27"/>
       <c r="D42" s="19"/>
       <c r="E42" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
@@ -2551,12 +2559,12 @@
         <v>zonmwpa:AntibodyDevelopment</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="27"/>
       <c r="D43" s="19"/>
       <c r="E43" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F43" s="27"/>
       <c r="G43" s="27"/>
@@ -2580,12 +2588,12 @@
         <v>zonmwpa:LaboratoriesdoingPCR-baseddiagnosis</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="19"/>
       <c r="E44" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F44" s="27"/>
       <c r="G44" s="27"/>
@@ -2609,12 +2617,12 @@
         <v>zonmwpa:Proteomicsstudiesincludingproteinengineeringandproteininteractions</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="19"/>
       <c r="E45" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F45" s="27"/>
       <c r="G45" s="27"/>
@@ -2638,12 +2646,12 @@
         <v>zonmwpa:Screeningtoolsforsearchingvirusproteasesinhibitors</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="19"/>
       <c r="E46" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F46" s="27"/>
       <c r="G46" s="27"/>
@@ -2667,12 +2675,12 @@
         <v>zonmwpa:AnimalTestingFacility</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C47" s="27"/>
       <c r="D47" s="19"/>
       <c r="E47" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F47" s="27"/>
       <c r="G47" s="27"/>
@@ -2696,12 +2704,12 @@
         <v>zonmwpa:Abilitytosetupclinicaltrials</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="27"/>
       <c r="D48" s="19"/>
       <c r="E48" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F48" s="27"/>
       <c r="G48" s="27"/>
@@ -2725,12 +2733,12 @@
         <v>zonmwpa:VirusSequencingFacility</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="19"/>
       <c r="E49" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F49" s="27"/>
       <c r="G49" s="27"/>
@@ -2754,12 +2762,12 @@
         <v>zonmwpa:OtherServices</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="27"/>
       <c r="D50" s="26"/>
       <c r="E50" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F50" s="27"/>
       <c r="G50" s="28"/>
@@ -2783,11 +2791,11 @@
         <v>zonmwpa:TypeOfMaterial</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E51" s="17"/>
       <c r="F51" s="15" t="s">
@@ -2814,12 +2822,12 @@
         <v>zonmwpa:BuffyCoat</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C52" s="27"/>
       <c r="D52" s="19"/>
       <c r="E52" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
@@ -2843,12 +2851,12 @@
         <v>zonmwpa:cDNADivmRNA</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C53" s="27"/>
       <c r="D53" s="19"/>
       <c r="E53" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F53" s="27"/>
       <c r="G53" s="27"/>
@@ -2872,12 +2880,12 @@
         <v>zonmwpa:Celllines</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" s="19"/>
       <c r="E54" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F54" s="27"/>
       <c r="G54" s="27"/>
@@ -2901,12 +2909,12 @@
         <v>zonmwpa:DNA</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" s="27"/>
       <c r="D55" s="19"/>
       <c r="E55" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F55" s="27"/>
       <c r="G55" s="27"/>
@@ -2930,12 +2938,12 @@
         <v>zonmwpa:Faeces</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56" s="27"/>
       <c r="D56" s="19"/>
       <c r="E56" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F56" s="27"/>
       <c r="G56" s="27"/>
@@ -2959,12 +2967,12 @@
         <v>zonmwpa:microRNA</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C57" s="27"/>
       <c r="D57" s="19"/>
       <c r="E57" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F57" s="27"/>
       <c r="G57" s="27"/>
@@ -2988,12 +2996,12 @@
         <v>zonmwpa:Nasalswab</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C58" s="27"/>
       <c r="D58" s="19"/>
       <c r="E58" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F58" s="27"/>
       <c r="G58" s="27"/>
@@ -3017,12 +3025,12 @@
         <v>zonmwpa:Notavailable</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59" s="27"/>
       <c r="D59" s="19"/>
       <c r="E59" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F59" s="27"/>
       <c r="G59" s="27"/>
@@ -3046,12 +3054,12 @@
         <v>zonmwpa:Pathogen</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C60" s="27"/>
       <c r="D60" s="19"/>
       <c r="E60" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F60" s="27"/>
       <c r="G60" s="27"/>
@@ -3075,12 +3083,12 @@
         <v>zonmwpa:Peripheralbloodcells</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C61" s="27"/>
       <c r="D61" s="19"/>
       <c r="E61" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F61" s="27"/>
       <c r="G61" s="27"/>
@@ -3104,12 +3112,12 @@
         <v>zonmwpa:Plasma</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C62" s="27"/>
       <c r="D62" s="19"/>
       <c r="E62" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F62" s="27"/>
       <c r="G62" s="27"/>
@@ -3133,12 +3141,12 @@
         <v>zonmwpa:RNA</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C63" s="27"/>
       <c r="D63" s="19"/>
       <c r="E63" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F63" s="27"/>
       <c r="G63" s="27"/>
@@ -3162,12 +3170,12 @@
         <v>zonmwpa:Saliva</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C64" s="27"/>
       <c r="D64" s="19"/>
       <c r="E64" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F64" s="27"/>
       <c r="G64" s="27"/>
@@ -3191,12 +3199,12 @@
         <v>zonmwpa:Serum</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C65" s="27"/>
       <c r="D65" s="19"/>
       <c r="E65" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F65" s="27"/>
       <c r="G65" s="27"/>
@@ -3220,12 +3228,12 @@
         <v>zonmwpa:Throatswab</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C66" s="27"/>
       <c r="D66" s="19"/>
       <c r="E66" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F66" s="27"/>
       <c r="G66" s="27"/>
@@ -3249,12 +3257,12 @@
         <v>zonmwpa:Tissue-cryopreserved</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C67" s="27"/>
       <c r="D67" s="19"/>
       <c r="E67" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F67" s="27"/>
       <c r="G67" s="27"/>
@@ -3278,12 +3286,12 @@
         <v>zonmwpa:Tissue-paraffinpreserved</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C68" s="27"/>
       <c r="D68" s="19"/>
       <c r="E68" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F68" s="27"/>
       <c r="G68" s="27"/>
@@ -3307,12 +3315,12 @@
         <v>zonmwpa:Tissue-stainedsectionsDivslides</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C69" s="27"/>
       <c r="D69" s="19"/>
       <c r="E69" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F69" s="27"/>
       <c r="G69" s="27"/>
@@ -3336,12 +3344,12 @@
         <v>zonmwpa:Urine</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C70" s="27"/>
       <c r="D70" s="19"/>
       <c r="E70" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F70" s="27"/>
       <c r="G70" s="27"/>
@@ -3365,12 +3373,12 @@
         <v>zonmwpa:WholeBlood</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C71" s="27"/>
       <c r="D71" s="19"/>
       <c r="E71" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F71" s="27"/>
       <c r="G71" s="27"/>
@@ -3394,12 +3402,12 @@
         <v>zonmwpa:OtherTypesOfMaterial</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C72" s="27"/>
       <c r="D72" s="26"/>
       <c r="E72" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F72" s="27"/>
       <c r="G72" s="28"/>
@@ -3423,11 +3431,11 @@
         <v>zonmwpa:TypeOfData</v>
       </c>
       <c r="B73" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E73" s="17"/>
       <c r="F73" s="15" t="s">
@@ -3454,12 +3462,12 @@
         <v>zonmwpa:Antibodiestiter-IgMandIgG</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C74" s="27"/>
       <c r="D74" s="19"/>
       <c r="E74" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F74" s="27"/>
       <c r="G74" s="27"/>
@@ -3483,12 +3491,12 @@
         <v>zonmwpa:Biologicalsamples</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C75" s="27"/>
       <c r="D75" s="19"/>
       <c r="E75" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F75" s="27"/>
       <c r="G75" s="27"/>
@@ -3512,12 +3520,12 @@
         <v>zonmwpa:Bloodcountandotherlabresultsespeciallyatthemomentofhospitaladmission</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C76" s="27"/>
       <c r="D76" s="19"/>
       <c r="E76" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F76" s="27"/>
       <c r="G76" s="27"/>
@@ -3541,12 +3549,12 @@
         <v>zonmwpa:Dataonclinicalsymptoms</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C77" s="27"/>
       <c r="D77" s="19"/>
       <c r="E77" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F77" s="27"/>
       <c r="G77" s="27"/>
@@ -3570,12 +3578,12 @@
         <v>zonmwpa:CTimagingoflungs-alternativelyXray</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C78" s="27"/>
       <c r="D78" s="19"/>
       <c r="E78" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F78" s="27"/>
       <c r="G78" s="27"/>
@@ -3599,12 +3607,12 @@
         <v>zonmwpa:Dataondiseasedurationanddiseaseoutcome</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C79" s="27"/>
       <c r="D79" s="19"/>
       <c r="E79" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F79" s="27"/>
       <c r="G79" s="27"/>
@@ -3628,12 +3636,12 @@
         <v>zonmwpa:Genealogicalrecords</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C80" s="27"/>
       <c r="D80" s="19"/>
       <c r="E80" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F80" s="27"/>
       <c r="G80" s="27"/>
@@ -3657,12 +3665,12 @@
         <v>zonmwpa:Imagingdata</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C81" s="27"/>
       <c r="D81" s="19"/>
       <c r="E81" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F81" s="27"/>
       <c r="G81" s="27"/>
@@ -3686,12 +3694,12 @@
         <v>zonmwpa:Medicalrecords</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C82" s="27"/>
       <c r="D82" s="19"/>
       <c r="E82" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F82" s="27"/>
       <c r="G82" s="27"/>
@@ -3715,12 +3723,12 @@
         <v>zonmwpa:Nationalregistries</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C83" s="27"/>
       <c r="D83" s="19"/>
       <c r="E83" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F83" s="27"/>
       <c r="G83" s="27"/>
@@ -3744,12 +3752,12 @@
         <v>zonmwpa:PhysiologicalDivBiochemicalmeasurements</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C84" s="27"/>
       <c r="D84" s="19"/>
       <c r="E84" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="27"/>
@@ -3773,12 +3781,12 @@
         <v>zonmwpa:Surveydata</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C85" s="27"/>
       <c r="D85" s="19"/>
       <c r="E85" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F85" s="27"/>
       <c r="G85" s="27"/>
@@ -3802,12 +3810,12 @@
         <v>zonmwpa:Treatmentprotocol-typesofdrugsused</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C86" s="27"/>
       <c r="D86" s="19"/>
       <c r="E86" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F86" s="27"/>
       <c r="G86" s="27"/>
@@ -3831,12 +3839,12 @@
         <v>zonmwpa:Notavailable</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C87" s="27"/>
       <c r="D87" s="19"/>
       <c r="E87" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F87" s="27"/>
       <c r="G87" s="27"/>
@@ -3860,12 +3868,12 @@
         <v>zonmwpa:OtherTypesOfData</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="26"/>
       <c r="E88" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F88" s="27"/>
       <c r="G88" s="28"/>
@@ -3889,11 +3897,11 @@
         <v>zonmwpa:TypeOfCollection</v>
       </c>
       <c r="B89" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C89" s="15"/>
       <c r="D89" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E89" s="17"/>
       <c r="F89" s="15" t="s">
@@ -3920,12 +3928,12 @@
         <v>zonmwpa:Birthcohort</v>
       </c>
       <c r="B90" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C90" s="27"/>
       <c r="D90" s="19"/>
       <c r="E90" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F90" s="27"/>
       <c r="G90" s="27"/>
@@ -3949,12 +3957,12 @@
         <v>zonmwpa:Case-Control</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C91" s="27"/>
       <c r="D91" s="19"/>
       <c r="E91" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F91" s="27"/>
       <c r="G91" s="27"/>
@@ -3978,12 +3986,12 @@
         <v>zonmwpa:Cohort</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C92" s="27"/>
       <c r="D92" s="19"/>
       <c r="E92" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F92" s="27"/>
       <c r="G92" s="27"/>
@@ -4007,12 +4015,12 @@
         <v>zonmwpa:Cross-sectional</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C93" s="27"/>
       <c r="D93" s="19"/>
       <c r="E93" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F93" s="27"/>
       <c r="G93" s="27"/>
@@ -4036,12 +4044,12 @@
         <v>zonmwpa:Diseasespecific</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C94" s="27"/>
       <c r="D94" s="19"/>
       <c r="E94" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F94" s="27"/>
       <c r="G94" s="27"/>
@@ -4065,12 +4073,12 @@
         <v>zonmwpa:Hospital</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C95" s="27"/>
       <c r="D95" s="19"/>
       <c r="E95" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F95" s="27"/>
       <c r="G95" s="27"/>
@@ -4094,12 +4102,12 @@
         <v>zonmwpa:Imagecollection</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C96" s="27"/>
       <c r="D96" s="19"/>
       <c r="E96" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F96" s="27"/>
       <c r="G96" s="27"/>
@@ -4123,12 +4131,12 @@
         <v>zonmwpa:Longitudinal</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C97" s="27"/>
       <c r="D97" s="19"/>
       <c r="E97" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F97" s="27"/>
       <c r="G97" s="27"/>
@@ -4152,12 +4160,12 @@
         <v>zonmwpa:Non-human</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C98" s="27"/>
       <c r="D98" s="19"/>
       <c r="E98" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F98" s="27"/>
       <c r="G98" s="27"/>
@@ -4181,12 +4189,12 @@
         <v>zonmwpa:OtherTypeofCollection</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C99" s="27"/>
       <c r="D99" s="26"/>
       <c r="E99" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F99" s="27"/>
       <c r="G99" s="27"/>
@@ -4210,12 +4218,12 @@
         <v>zonmwpa:Population-based</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C100" s="27"/>
       <c r="D100" s="19"/>
       <c r="E100" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F100" s="27"/>
       <c r="G100" s="27"/>
@@ -4239,12 +4247,12 @@
         <v>zonmwpa:Prospectivestudy</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C101" s="27"/>
       <c r="D101" s="19"/>
       <c r="E101" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F101" s="27"/>
       <c r="G101" s="27"/>
@@ -4268,12 +4276,12 @@
         <v>zonmwpa:Qualitycontrol</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C102" s="27"/>
       <c r="D102" s="19"/>
       <c r="E102" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F102" s="27"/>
       <c r="G102" s="27"/>
@@ -4297,12 +4305,12 @@
         <v>zonmwpa:Rarediseasecollection</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C103" s="27"/>
       <c r="D103" s="19"/>
       <c r="E103" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F103" s="27"/>
       <c r="G103" s="27"/>
@@ -4326,12 +4334,12 @@
         <v>zonmwpa:Samplecollection</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C104" s="27"/>
       <c r="D104" s="19"/>
       <c r="E104" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F104" s="27"/>
       <c r="G104" s="27"/>
@@ -4355,12 +4363,12 @@
         <v>zonmwpa:Twin-study</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C105" s="27"/>
       <c r="D105" s="19"/>
       <c r="E105" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F105" s="27"/>
       <c r="G105" s="27"/>
@@ -4384,11 +4392,11 @@
         <v>zonmwpa:Population</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C106" s="15"/>
       <c r="D106" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E106" s="17"/>
       <c r="F106" s="15" t="s">
@@ -4415,12 +4423,12 @@
         <v>zonmwpa:Populationwide</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C107" s="27"/>
       <c r="D107" s="19"/>
       <c r="E107" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F107" s="27"/>
       <c r="G107" s="27"/>
@@ -4444,12 +4452,12 @@
         <v>zonmwpa:Neonates</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C108" s="27"/>
       <c r="D108" s="19"/>
       <c r="E108" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F108" s="27"/>
       <c r="G108" s="27"/>
@@ -4473,12 +4481,12 @@
         <v>zonmwpa:Children-0-18years</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C109" s="27"/>
       <c r="D109" s="19"/>
       <c r="E109" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F109" s="27"/>
       <c r="G109" s="27"/>
@@ -4502,12 +4510,12 @@
         <v>zonmwpa:Primaryschoolchildren-4-12years</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C110" s="27"/>
       <c r="D110" s="19"/>
       <c r="E110" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F110" s="27"/>
       <c r="G110" s="27"/>
@@ -4531,12 +4539,12 @@
         <v>zonmwpa:Teenager-12-18years</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C111" s="27"/>
       <c r="D111" s="19"/>
       <c r="E111" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F111" s="27"/>
       <c r="G111" s="27"/>
@@ -4560,12 +4568,12 @@
         <v>zonmwpa:Youngpeople-16-27years</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C112" s="27"/>
       <c r="D112" s="19"/>
       <c r="E112" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F112" s="27"/>
       <c r="G112" s="27"/>
@@ -4589,12 +4597,12 @@
         <v>zonmwpa:Youngadults18-21years</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C113" s="27"/>
       <c r="D113" s="19"/>
       <c r="E113" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F113" s="27"/>
       <c r="G113" s="27"/>
@@ -4618,12 +4626,12 @@
         <v>zonmwpa:Adults-18-65years</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C114" s="27"/>
       <c r="D114" s="19"/>
       <c r="E114" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F114" s="27"/>
       <c r="G114" s="27"/>
@@ -4647,12 +4655,12 @@
         <v>zonmwpa:Elderly-65plus</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C115" s="27"/>
       <c r="D115" s="19"/>
       <c r="E115" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F115" s="27"/>
       <c r="G115" s="27"/>
@@ -4676,12 +4684,12 @@
         <v>zonmwpa:Vulnerableelderly</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C116" s="27"/>
       <c r="D116" s="19"/>
       <c r="E116" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F116" s="27"/>
       <c r="G116" s="27"/>
@@ -4705,12 +4713,12 @@
         <v>zonmwpa:Pregnantwomen</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C117" s="27"/>
       <c r="D117" s="19"/>
       <c r="E117" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F117" s="27"/>
       <c r="G117" s="27"/>
@@ -4734,12 +4742,12 @@
         <v>zonmwpa:Peoplewithaspecificethnicbackground</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C118" s="27"/>
       <c r="D118" s="19"/>
       <c r="E118" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F118" s="27"/>
       <c r="G118" s="27"/>
@@ -4763,12 +4771,12 @@
         <v>zonmwpa:Peoplewithamigrationbackground</v>
       </c>
       <c r="B119" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C119" s="27"/>
       <c r="D119" s="19"/>
       <c r="E119" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F119" s="27"/>
       <c r="G119" s="27"/>
@@ -4792,12 +4800,12 @@
         <v>zonmwpa:Peoplewithachronicillness</v>
       </c>
       <c r="B120" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C120" s="27"/>
       <c r="D120" s="19"/>
       <c r="E120" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F120" s="27"/>
       <c r="G120" s="27"/>
@@ -4821,12 +4829,12 @@
         <v>zonmwpa:Peoplewithaphysicaldisability</v>
       </c>
       <c r="B121" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C121" s="27"/>
       <c r="D121" s="19"/>
       <c r="E121" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F121" s="27"/>
       <c r="G121" s="27"/>
@@ -4850,12 +4858,12 @@
         <v>zonmwpa:Mentallychallengedpeople</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C122" s="27"/>
       <c r="D122" s="19"/>
       <c r="E122" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F122" s="27"/>
       <c r="G122" s="27"/>
@@ -4879,12 +4887,12 @@
         <v>zonmwpa:Peoplewithararecondition</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C123" s="27"/>
       <c r="D123" s="19"/>
       <c r="E123" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F123" s="27"/>
       <c r="G123" s="27"/>
@@ -4908,12 +4916,12 @@
         <v>zonmwpa:Peoplewithalowsocio-economicstatus</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C124" s="27"/>
       <c r="D124" s="19"/>
       <c r="E124" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F124" s="27"/>
       <c r="G124" s="27"/>
@@ -4937,12 +4945,12 @@
         <v>zonmwpa:Workingpeople</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C125" s="27"/>
       <c r="D125" s="19"/>
       <c r="E125" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F125" s="27"/>
       <c r="G125" s="27"/>
@@ -4966,12 +4974,12 @@
         <v>zonmwpa:Topathletes</v>
       </c>
       <c r="B126" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C126" s="27"/>
       <c r="D126" s="19"/>
       <c r="E126" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F126" s="27"/>
       <c r="G126" s="27"/>
@@ -4995,12 +5003,12 @@
         <v>zonmwpa:Men</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C127" s="27"/>
       <c r="D127" s="19"/>
       <c r="E127" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F127" s="27"/>
       <c r="G127" s="27"/>
@@ -5024,12 +5032,12 @@
         <v>zonmwpa:Women</v>
       </c>
       <c r="B128" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C128" s="27"/>
       <c r="D128" s="19"/>
       <c r="E128" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F128" s="27"/>
       <c r="G128" s="27"/>
@@ -5053,12 +5061,12 @@
         <v>zonmwpa:OtherPopulation</v>
       </c>
       <c r="B129" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C129" s="27"/>
       <c r="D129" s="26"/>
       <c r="E129" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F129" s="27"/>
       <c r="G129" s="27"/>
@@ -5082,11 +5090,11 @@
         <v>zonmwpa:CareProcessPhase</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C130" s="15"/>
       <c r="D130" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E130" s="17"/>
       <c r="F130" s="15" t="s">
@@ -5113,12 +5121,12 @@
         <v>zonmwpa:Prevention</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C131" s="27"/>
       <c r="D131" s="19"/>
       <c r="E131" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F131" s="27"/>
       <c r="G131" s="27"/>
@@ -5142,12 +5150,12 @@
         <v>zonmwpa:Diagnosis</v>
       </c>
       <c r="B132" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C132" s="27"/>
       <c r="D132" s="19"/>
       <c r="E132" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F132" s="27"/>
       <c r="G132" s="27"/>
@@ -5171,12 +5179,12 @@
         <v>zonmwpa:Therapy</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C133" s="27"/>
       <c r="D133" s="19"/>
       <c r="E133" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F133" s="27"/>
       <c r="G133" s="27"/>
@@ -5200,12 +5208,12 @@
         <v>zonmwpa:Follow-up</v>
       </c>
       <c r="B134" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C134" s="27"/>
       <c r="D134" s="19"/>
       <c r="E134" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F134" s="27"/>
       <c r="G134" s="27"/>
@@ -5229,12 +5237,12 @@
         <v>zonmwpa:Aftercare</v>
       </c>
       <c r="B135" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C135" s="27"/>
       <c r="D135" s="19"/>
       <c r="E135" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F135" s="27"/>
       <c r="G135" s="27"/>
@@ -5258,12 +5266,12 @@
         <v>zonmwpa:Palliative</v>
       </c>
       <c r="B136" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C136" s="27"/>
       <c r="D136" s="19"/>
       <c r="E136" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F136" s="27"/>
       <c r="G136" s="27"/>
@@ -5287,12 +5295,12 @@
         <v>zonmwpa:Information</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C137" s="27"/>
       <c r="D137" s="19"/>
       <c r="E137" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F137" s="27"/>
       <c r="G137" s="27"/>
@@ -5316,12 +5324,12 @@
         <v>zonmwpa:Earlydetection-screening</v>
       </c>
       <c r="B138" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C138" s="27"/>
       <c r="D138" s="19"/>
       <c r="E138" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F138" s="27"/>
       <c r="G138" s="27"/>
@@ -5345,12 +5353,12 @@
         <v>zonmwpa:Organizationofcare</v>
       </c>
       <c r="B139" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C139" s="27"/>
       <c r="D139" s="19"/>
       <c r="E139" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F139" s="27"/>
       <c r="G139" s="27"/>
@@ -5374,12 +5382,12 @@
         <v>zonmwpa:OtherCareProcessPhase</v>
       </c>
       <c r="B140" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C140" s="27"/>
       <c r="D140" s="26"/>
       <c r="E140" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F140" s="27"/>
       <c r="G140" s="27"/>
@@ -5403,11 +5411,11 @@
         <v>zonmwpa:Setting</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C141" s="15"/>
       <c r="D141" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E141" s="17"/>
       <c r="F141" s="15" t="s">
@@ -5434,12 +5442,12 @@
         <v>zonmwpa:Primarycare</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C142" s="27"/>
       <c r="D142" s="19"/>
       <c r="E142" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F142" s="27"/>
       <c r="G142" s="27"/>
@@ -5463,12 +5471,12 @@
         <v>zonmwpa:Second-linecare</v>
       </c>
       <c r="B143" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C143" s="27"/>
       <c r="D143" s="19"/>
       <c r="E143" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F143" s="27"/>
       <c r="G143" s="27"/>
@@ -5492,12 +5500,12 @@
         <v>zonmwpa:Prevention</v>
       </c>
       <c r="B144" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C144" s="27"/>
       <c r="D144" s="19"/>
       <c r="E144" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F144" s="27"/>
       <c r="G144" s="27"/>
@@ -5521,12 +5529,12 @@
         <v>zonmwpa:Healthcareinstitution</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C145" s="27"/>
       <c r="D145" s="19"/>
       <c r="E145" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F145" s="27"/>
       <c r="G145" s="27"/>
@@ -5550,12 +5558,12 @@
         <v>zonmwpa:Cattle</v>
       </c>
       <c r="B146" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C146" s="27"/>
       <c r="D146" s="19"/>
       <c r="E146" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F146" s="27"/>
       <c r="G146" s="27"/>
@@ -5579,12 +5587,12 @@
         <v>zonmwpa:Transmural</v>
       </c>
       <c r="B147" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C147" s="27"/>
       <c r="D147" s="19"/>
       <c r="E147" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F147" s="27"/>
       <c r="G147" s="27"/>
@@ -5608,12 +5616,12 @@
         <v>zonmwpa:Nursinghomecare</v>
       </c>
       <c r="B148" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C148" s="27"/>
       <c r="D148" s="19"/>
       <c r="E148" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F148" s="27"/>
       <c r="G148" s="27"/>
@@ -5637,12 +5645,12 @@
         <v>zonmwpa:Hospitalcare</v>
       </c>
       <c r="B149" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C149" s="27"/>
       <c r="D149" s="19"/>
       <c r="E149" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F149" s="27"/>
       <c r="G149" s="27"/>
@@ -5666,12 +5674,12 @@
         <v>zonmwpa:Homecare</v>
       </c>
       <c r="B150" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C150" s="27"/>
       <c r="D150" s="19"/>
       <c r="E150" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F150" s="27"/>
       <c r="G150" s="27"/>
@@ -5695,12 +5703,12 @@
         <v>zonmwpa:Education-schoolandupbringing</v>
       </c>
       <c r="B151" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C151" s="27"/>
       <c r="D151" s="19"/>
       <c r="E151" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F151" s="27"/>
       <c r="G151" s="27"/>
@@ -5724,12 +5732,12 @@
         <v>zonmwpa:WorkandIncome</v>
       </c>
       <c r="B152" s="26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C152" s="27"/>
       <c r="D152" s="19"/>
       <c r="E152" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F152" s="27"/>
       <c r="G152" s="27"/>
@@ -5758,7 +5766,7 @@
       <c r="C153" s="27"/>
       <c r="D153" s="19"/>
       <c r="E153" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F153" s="27"/>
       <c r="G153" s="27"/>
@@ -5782,12 +5790,12 @@
         <v>zonmwpa:Care</v>
       </c>
       <c r="B154" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C154" s="27"/>
       <c r="D154" s="19"/>
       <c r="E154" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F154" s="27"/>
       <c r="G154" s="27"/>
@@ -5811,12 +5819,12 @@
         <v>zonmwpa:Earlydetection-screening</v>
       </c>
       <c r="B155" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C155" s="27"/>
       <c r="D155" s="19"/>
       <c r="E155" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F155" s="27"/>
       <c r="G155" s="27"/>
@@ -5840,12 +5848,12 @@
         <v>zonmwpa:Justice</v>
       </c>
       <c r="B156" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C156" s="27"/>
       <c r="D156" s="19"/>
       <c r="E156" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F156" s="27"/>
       <c r="G156" s="27"/>
@@ -5869,12 +5877,12 @@
         <v>zonmwpa:Socialdomain</v>
       </c>
       <c r="B157" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C157" s="27"/>
       <c r="D157" s="19"/>
       <c r="E157" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F157" s="27"/>
       <c r="G157" s="27"/>
@@ -5898,12 +5906,12 @@
         <v>zonmwpa:Youth</v>
       </c>
       <c r="B158" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C158" s="27"/>
       <c r="D158" s="19"/>
       <c r="E158" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F158" s="27"/>
       <c r="G158" s="27"/>
@@ -5927,12 +5935,12 @@
         <v>zonmwpa:SocialSupport</v>
       </c>
       <c r="B159" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C159" s="27"/>
       <c r="D159" s="19"/>
       <c r="E159" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F159" s="27"/>
       <c r="G159" s="27"/>
@@ -5956,12 +5964,12 @@
         <v>zonmwpa:SportDivhealthDivwellness</v>
       </c>
       <c r="B160" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C160" s="27"/>
       <c r="D160" s="19"/>
       <c r="E160" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F160" s="27"/>
       <c r="G160" s="27"/>
@@ -5985,12 +5993,12 @@
         <v>zonmwpa:Disabledcare</v>
       </c>
       <c r="B161" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C161" s="27"/>
       <c r="D161" s="19"/>
       <c r="E161" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F161" s="27"/>
       <c r="G161" s="27"/>
@@ -6014,12 +6022,12 @@
         <v>zonmwpa:Long-termmentalhealthcare</v>
       </c>
       <c r="B162" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C162" s="27"/>
       <c r="D162" s="19"/>
       <c r="E162" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F162" s="27"/>
       <c r="G162" s="27"/>
@@ -6043,12 +6051,12 @@
         <v>zonmwpa:Youth-healthcare</v>
       </c>
       <c r="B163" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C163" s="27"/>
       <c r="D163" s="19"/>
       <c r="E163" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F163" s="27"/>
       <c r="G163" s="27"/>
@@ -6072,12 +6080,12 @@
         <v>zonmwpa:Generalpractitionercare</v>
       </c>
       <c r="B164" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C164" s="27"/>
       <c r="D164" s="19"/>
       <c r="E164" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F164" s="27"/>
       <c r="G164" s="27"/>
@@ -6101,12 +6109,12 @@
         <v>zonmwpa:Elderlycare</v>
       </c>
       <c r="B165" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C165" s="27"/>
       <c r="D165" s="19"/>
       <c r="E165" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F165" s="27"/>
       <c r="G165" s="27"/>
@@ -6130,12 +6138,12 @@
         <v>zonmwpa:ClientsandDivorpatientorganization</v>
       </c>
       <c r="B166" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C166" s="27"/>
       <c r="D166" s="19"/>
       <c r="E166" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F166" s="27"/>
       <c r="G166" s="27"/>
@@ -6159,12 +6167,12 @@
         <v>zonmwpa:Measuringinstrument</v>
       </c>
       <c r="B167" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C167" s="27"/>
       <c r="D167" s="19"/>
       <c r="E167" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F167" s="27"/>
       <c r="G167" s="27"/>
@@ -6188,12 +6196,12 @@
         <v>zonmwpa:Experimentalgarden</v>
       </c>
       <c r="B168" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C168" s="27"/>
       <c r="D168" s="19"/>
       <c r="E168" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F168" s="27"/>
       <c r="G168" s="27"/>
@@ -6217,12 +6225,12 @@
         <v>zonmwpa:OtherSetting</v>
       </c>
       <c r="B169" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C169" s="27"/>
       <c r="D169" s="26"/>
       <c r="E169" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F169" s="27"/>
       <c r="G169" s="27"/>
@@ -6246,11 +6254,11 @@
         <v>zonmwpa:Institution</v>
       </c>
       <c r="B170" s="33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C170" s="16"/>
       <c r="D170" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E170" s="17"/>
       <c r="F170" s="16" t="s">
@@ -6277,12 +6285,12 @@
         <v>zonmwpa:AcademicMedicalCenter-AmsterdamUMC</v>
       </c>
       <c r="B171" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C171" s="30"/>
       <c r="D171" s="26"/>
       <c r="E171" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F171" s="30"/>
       <c r="G171" s="30"/>
@@ -6306,12 +6314,12 @@
         <v>zonmwpa:AmsterdamHealthandTechnologyInstitute-AHTI</v>
       </c>
       <c r="B172" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C172" s="30"/>
       <c r="D172" s="26"/>
       <c r="E172" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F172" s="30"/>
       <c r="G172" s="30"/>
@@ -6335,12 +6343,12 @@
         <v>zonmwpa:DelftUniversityofTechnology</v>
       </c>
       <c r="B173" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C173" s="30"/>
       <c r="D173" s="26"/>
       <c r="E173" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F173" s="30"/>
       <c r="G173" s="30"/>
@@ -6364,12 +6372,12 @@
         <v>zonmwpa:EindhovenUniversityofTechnology</v>
       </c>
       <c r="B174" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C174" s="30"/>
       <c r="D174" s="26"/>
       <c r="E174" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F174" s="30"/>
       <c r="G174" s="30"/>
@@ -6393,12 +6401,12 @@
         <v>zonmwpa:ErasmusCentrumvoorZorgbestuur</v>
       </c>
       <c r="B175" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C175" s="30"/>
       <c r="D175" s="26"/>
       <c r="E175" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F175" s="30"/>
       <c r="G175" s="30"/>
@@ -6422,12 +6430,12 @@
         <v>zonmwpa:ErasmusMC</v>
       </c>
       <c r="B176" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C176" s="30"/>
       <c r="D176" s="26"/>
       <c r="E176" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F176" s="30"/>
       <c r="G176" s="30"/>
@@ -6451,12 +6459,12 @@
         <v>zonmwpa:ErasmusUniversityRotterdam</v>
       </c>
       <c r="B177" s="38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C177" s="30"/>
       <c r="D177" s="26"/>
       <c r="E177" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F177" s="30"/>
       <c r="G177" s="30"/>
@@ -6480,12 +6488,12 @@
         <v>zonmwpa:ExpertisecentrumNederlands</v>
       </c>
       <c r="B178" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C178" s="30"/>
       <c r="D178" s="26"/>
       <c r="E178" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F178" s="30"/>
       <c r="G178" s="30"/>
@@ -6509,12 +6517,12 @@
         <v>zonmwpa:FederalUniversityofRiodeJaneiro</v>
       </c>
       <c r="B179" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C179" s="30"/>
       <c r="D179" s="26"/>
       <c r="E179" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F179" s="30"/>
       <c r="G179" s="30"/>
@@ -6538,12 +6546,12 @@
         <v>zonmwpa:GGDAmsterdam-PublicHealthServiceofAmsterdam</v>
       </c>
       <c r="B180" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C180" s="30"/>
       <c r="D180" s="26"/>
       <c r="E180" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F180" s="30"/>
       <c r="G180" s="30"/>
@@ -6567,12 +6575,12 @@
         <v>zonmwpa:GGDZuidHollandZuid</v>
       </c>
       <c r="B181" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C181" s="30"/>
       <c r="D181" s="26"/>
       <c r="E181" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F181" s="30"/>
       <c r="G181" s="30"/>
@@ -6596,12 +6604,12 @@
         <v>zonmwpa:GOFAIRFoundation</v>
       </c>
       <c r="B182" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C182" s="30"/>
       <c r="D182" s="26"/>
       <c r="E182" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F182" s="30"/>
       <c r="G182" s="30"/>
@@ -6625,12 +6633,12 @@
         <v>zonmwpa:HogeschoolLeiden-UniversityofAppliedSciencesLeiden</v>
       </c>
       <c r="B183" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C183" s="30"/>
       <c r="D183" s="26"/>
       <c r="E183" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F183" s="30"/>
       <c r="G183" s="30"/>
@@ -6654,12 +6662,12 @@
         <v>zonmwpa:HogeschoolvanAmsterdam-AmsterdamUniversityofAppliedSciences</v>
       </c>
       <c r="B184" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C184" s="30"/>
       <c r="D184" s="26"/>
       <c r="E184" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F184" s="30"/>
       <c r="G184" s="30"/>
@@ -6683,12 +6691,12 @@
         <v>zonmwpa:IKNL-NetherlandsComprehensiveCancerOrganisation</v>
       </c>
       <c r="B185" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C185" s="30"/>
       <c r="D185" s="26"/>
       <c r="E185" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F185" s="30"/>
       <c r="G185" s="30"/>
@@ -6712,12 +6720,12 @@
         <v>zonmwpa:LeidenUniversity</v>
       </c>
       <c r="B186" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C186" s="30"/>
       <c r="D186" s="26"/>
       <c r="E186" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F186" s="30"/>
       <c r="G186" s="30"/>
@@ -6741,12 +6749,12 @@
         <v>zonmwpa:LeidenUniversityMedicalCenter</v>
       </c>
       <c r="B187" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C187" s="30"/>
       <c r="D187" s="26"/>
       <c r="E187" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F187" s="30"/>
       <c r="G187" s="30"/>
@@ -6770,12 +6778,12 @@
         <v>zonmwpa:MaastrichtUniversity</v>
       </c>
       <c r="B188" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C188" s="30"/>
       <c r="D188" s="26"/>
       <c r="E188" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F188" s="30"/>
       <c r="G188" s="30"/>
@@ -6799,12 +6807,12 @@
         <v>zonmwpa:MaastrichtUniversityMedicalCentre</v>
       </c>
       <c r="B189" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C189" s="30"/>
       <c r="D189" s="26"/>
       <c r="E189" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F189" s="30"/>
       <c r="G189" s="30"/>
@@ -6828,12 +6836,12 @@
         <v>zonmwpa:NetherlandsComprehensiveCancerOrganisation</v>
       </c>
       <c r="B190" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C190" s="30"/>
       <c r="D190" s="26"/>
       <c r="E190" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F190" s="30"/>
       <c r="G190" s="30"/>
@@ -6857,12 +6865,12 @@
         <v>zonmwpa:NetherlandsHeartInstitute</v>
       </c>
       <c r="B191" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C191" s="30"/>
       <c r="D191" s="26"/>
       <c r="E191" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F191" s="30"/>
       <c r="G191" s="30"/>
@@ -6886,12 +6894,12 @@
         <v>zonmwpa:NIVEL-NetherlandsInstituteforHealthServicesResearch</v>
       </c>
       <c r="B192" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C192" s="30"/>
       <c r="D192" s="26"/>
       <c r="E192" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F192" s="30"/>
       <c r="G192" s="30"/>
@@ -6915,12 +6923,12 @@
         <v>zonmwpa:NSCR-NetherlandsInstitutefortheStudyofCrimeandLawEnforcement</v>
       </c>
       <c r="B193" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C193" s="30"/>
       <c r="D193" s="26"/>
       <c r="E193" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F193" s="30"/>
       <c r="G193" s="30"/>
@@ -6944,12 +6952,12 @@
         <v>zonmwpa:PublicHealthServiceofAmsterdam</v>
       </c>
       <c r="B194" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C194" s="30"/>
       <c r="D194" s="26"/>
       <c r="E194" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F194" s="30"/>
       <c r="G194" s="30"/>
@@ -6973,12 +6981,12 @@
         <v>zonmwpa:PublicProcurementResearchCentre-PPRC</v>
       </c>
       <c r="B195" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C195" s="30"/>
       <c r="D195" s="26"/>
       <c r="E195" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F195" s="30"/>
       <c r="G195" s="30"/>
@@ -7002,12 +7010,12 @@
         <v>zonmwpa:RadboudUniversityNijmegen</v>
       </c>
       <c r="B196" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C196" s="30"/>
       <c r="D196" s="26"/>
       <c r="E196" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F196" s="30"/>
       <c r="G196" s="30"/>
@@ -7031,12 +7039,12 @@
         <v>zonmwpa:RadboudUniversityNijmegenMedicalCentre</v>
       </c>
       <c r="B197" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C197" s="30"/>
       <c r="D197" s="26"/>
       <c r="E197" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F197" s="30"/>
       <c r="G197" s="30"/>
@@ -7060,12 +7068,12 @@
         <v>zonmwpa:ReadeResearchBV</v>
       </c>
       <c r="B198" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C198" s="30"/>
       <c r="D198" s="26"/>
       <c r="E198" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F198" s="30"/>
       <c r="G198" s="30"/>
@@ -7089,12 +7097,12 @@
         <v>zonmwpa:RIVM-NationalInstituteforPublicHealthandtheEnvironment</v>
       </c>
       <c r="B199" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C199" s="30"/>
       <c r="D199" s="26"/>
       <c r="E199" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F199" s="30"/>
       <c r="G199" s="30"/>
@@ -7118,12 +7126,12 @@
         <v>zonmwpa:Sanquin</v>
       </c>
       <c r="B200" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C200" s="30"/>
       <c r="D200" s="26"/>
       <c r="E200" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F200" s="30"/>
       <c r="G200" s="30"/>
@@ -7147,12 +7155,12 @@
         <v>zonmwpa:SaxionUniversityofAppliedSciences</v>
       </c>
       <c r="B201" s="31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C201" s="30"/>
       <c r="D201" s="26"/>
       <c r="E201" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F201" s="30"/>
       <c r="G201" s="30"/>
@@ -7176,12 +7184,12 @@
         <v>zonmwpa:SEOEconomischOnderzoek</v>
       </c>
       <c r="B202" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C202" s="30"/>
       <c r="D202" s="26"/>
       <c r="E202" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F202" s="30"/>
       <c r="G202" s="30"/>
@@ -7205,12 +7213,12 @@
         <v>zonmwpa:SpaarneGasthuis-SpaarneZiekenhuis</v>
       </c>
       <c r="B203" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C203" s="30"/>
       <c r="D203" s="26"/>
       <c r="E203" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F203" s="30"/>
       <c r="G203" s="30"/>
@@ -7234,12 +7242,12 @@
         <v>zonmwpa:TilburgUniversity</v>
       </c>
       <c r="B204" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C204" s="30"/>
       <c r="D204" s="26"/>
       <c r="E204" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F204" s="30"/>
       <c r="G204" s="30"/>
@@ -7263,12 +7271,12 @@
         <v>zonmwpa:TNO-NetherlandsOrganisationforAppliedScientificResearch</v>
       </c>
       <c r="B205" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C205" s="30"/>
       <c r="D205" s="26"/>
       <c r="E205" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F205" s="30"/>
       <c r="G205" s="30"/>
@@ -7292,12 +7300,12 @@
         <v>zonmwpa:UniversityMedicalCenterGroningen</v>
       </c>
       <c r="B206" s="31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C206" s="30"/>
       <c r="D206" s="26"/>
       <c r="E206" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F206" s="30"/>
       <c r="G206" s="30"/>
@@ -7321,12 +7329,12 @@
         <v>zonmwpa:UniversityMedicalCenterUtrecht</v>
       </c>
       <c r="B207" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C207" s="30"/>
       <c r="D207" s="26"/>
       <c r="E207" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F207" s="30"/>
       <c r="G207" s="30"/>
@@ -7350,12 +7358,12 @@
         <v>zonmwpa:UniversityofAmsterdam</v>
       </c>
       <c r="B208" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C208" s="30"/>
       <c r="D208" s="26"/>
       <c r="E208" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F208" s="30"/>
       <c r="G208" s="30"/>
@@ -7379,12 +7387,12 @@
         <v>zonmwpa:UniversityofGroningen</v>
       </c>
       <c r="B209" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C209" s="30"/>
       <c r="D209" s="26"/>
       <c r="E209" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F209" s="30"/>
       <c r="G209" s="30"/>
@@ -7408,12 +7416,12 @@
         <v>zonmwpa:UniversityofHumanisticStudies</v>
       </c>
       <c r="B210" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C210" s="30"/>
       <c r="D210" s="26"/>
       <c r="E210" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F210" s="30"/>
       <c r="G210" s="30"/>
@@ -7437,12 +7445,12 @@
         <v>zonmwpa:UniversityofTwente</v>
       </c>
       <c r="B211" s="31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C211" s="30"/>
       <c r="D211" s="26"/>
       <c r="E211" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F211" s="30"/>
       <c r="G211" s="30"/>
@@ -7466,12 +7474,12 @@
         <v>zonmwpa:UtrechtUniversity</v>
       </c>
       <c r="B212" s="31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C212" s="30"/>
       <c r="D212" s="26"/>
       <c r="E212" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F212" s="30"/>
       <c r="G212" s="30"/>
@@ -7495,12 +7503,12 @@
         <v>zonmwpa:Veiligheids-enGezondheidsregioGelderland-Midden</v>
       </c>
       <c r="B213" s="31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C213" s="30"/>
       <c r="D213" s="26"/>
       <c r="E213" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F213" s="30"/>
       <c r="G213" s="30"/>
@@ -7524,12 +7532,12 @@
         <v>zonmwpa:VUAmsterdam</v>
       </c>
       <c r="B214" s="31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C214" s="30"/>
       <c r="D214" s="26"/>
       <c r="E214" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F214" s="30"/>
       <c r="G214" s="30"/>
@@ -7553,12 +7561,12 @@
         <v>zonmwpa:VUUniversityMedicalCenter</v>
       </c>
       <c r="B215" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C215" s="30"/>
       <c r="D215" s="26"/>
       <c r="E215" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F215" s="30"/>
       <c r="G215" s="30"/>
@@ -7582,12 +7590,12 @@
         <v>zonmwpa:WageningenUniversity-Research</v>
       </c>
       <c r="B216" s="31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C216" s="30"/>
       <c r="D216" s="26"/>
       <c r="E216" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F216" s="30"/>
       <c r="G216" s="30"/>
@@ -7611,12 +7619,12 @@
         <v>zonmwpa:ZonMw-NetherlandsOrganisationforHealthResearchandDevelopment</v>
       </c>
       <c r="B217" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C217" s="30"/>
       <c r="D217" s="26"/>
       <c r="E217" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F217" s="30"/>
       <c r="G217" s="30"/>
@@ -7640,12 +7648,12 @@
         <v>zonmwpa:Otherinstitution</v>
       </c>
       <c r="B218" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C218" s="30"/>
       <c r="D218" s="26"/>
       <c r="E218" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F218" s="30"/>
       <c r="G218" s="30"/>
@@ -7669,11 +7677,11 @@
         <v>zonmwpa:FocusArea</v>
       </c>
       <c r="B219" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C219" s="16"/>
       <c r="D219" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E219" s="17"/>
       <c r="F219" s="16" t="s">
@@ -7696,16 +7704,16 @@
     </row>
     <row r="220" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B220," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
         <v>zonmwpa:Predictivediagnosticsandtreatment</v>
       </c>
       <c r="B220" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C220" s="30"/>
       <c r="D220" s="26"/>
       <c r="E220" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F220" s="30"/>
       <c r="G220" s="30"/>
@@ -7729,12 +7737,12 @@
         <v>zonmwpa:Careandprevention</v>
       </c>
       <c r="B221" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C221" s="30"/>
       <c r="D221" s="26"/>
       <c r="E221" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F221" s="30"/>
       <c r="G221" s="30"/>
@@ -7758,12 +7766,12 @@
         <v>zonmwpa:Effectsonsociety</v>
       </c>
       <c r="B222" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C222" s="30"/>
       <c r="D222" s="26"/>
       <c r="E222" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F222" s="30"/>
       <c r="G222" s="30"/>
@@ -7787,12 +7795,12 @@
         <v>zonmwpa:OtherFocusArea</v>
       </c>
       <c r="B223" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C223" s="30"/>
       <c r="D223" s="26"/>
       <c r="E223" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F223" s="30"/>
       <c r="G223" s="30"/>
@@ -7816,11 +7824,11 @@
         <v>zonmwpa:Theme</v>
       </c>
       <c r="B224" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C224" s="16"/>
       <c r="D224" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E224" s="17"/>
       <c r="F224" s="16" t="s">
@@ -7847,12 +7855,12 @@
         <v>zonmwpa:Treatment</v>
       </c>
       <c r="B225" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C225" s="30"/>
       <c r="D225" s="26"/>
       <c r="E225" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F225" s="30"/>
       <c r="G225" s="30"/>
@@ -7876,12 +7884,12 @@
         <v>zonmwpa:Diagnosticsofinfection</v>
       </c>
       <c r="B226" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C226" s="30"/>
       <c r="D226" s="26"/>
       <c r="E226" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F226" s="30"/>
       <c r="G226" s="30"/>
@@ -7905,12 +7913,12 @@
         <v>zonmwpa:Riskanalysisandprognostics</v>
       </c>
       <c r="B227" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C227" s="30"/>
       <c r="D227" s="26"/>
       <c r="E227" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F227" s="30"/>
       <c r="G227" s="30"/>
@@ -7934,12 +7942,12 @@
         <v>zonmwpa:Virus-immunity-immuneresponseandpathogenesis</v>
       </c>
       <c r="B228" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C228" s="30"/>
       <c r="D228" s="26"/>
       <c r="E228" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F228" s="30"/>
       <c r="G228" s="30"/>
@@ -7963,12 +7971,12 @@
         <v>zonmwpa:Clinicaltreatment</v>
       </c>
       <c r="B229" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C229" s="30"/>
       <c r="D229" s="26"/>
       <c r="E229" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F229" s="30"/>
       <c r="G229" s="30"/>
@@ -7992,12 +8000,12 @@
         <v>zonmwpa:Animalfreeinnovations</v>
       </c>
       <c r="B230" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C230" s="30"/>
       <c r="D230" s="26"/>
       <c r="E230" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F230" s="30"/>
       <c r="G230" s="30"/>
@@ -8021,12 +8029,12 @@
         <v>zonmwpa:Organisationofcareandprevention</v>
       </c>
       <c r="B231" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C231" s="30"/>
       <c r="D231" s="26"/>
       <c r="E231" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F231" s="30"/>
       <c r="G231" s="30"/>
@@ -8050,12 +8058,12 @@
         <v>zonmwpa:Careandpreventionforvulnerablecitizens</v>
       </c>
       <c r="B232" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C232" s="30"/>
       <c r="D232" s="26"/>
       <c r="E232" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F232" s="30"/>
       <c r="G232" s="30"/>
@@ -8079,12 +8087,12 @@
         <v>zonmwpa:Transmissionandepidemiology</v>
       </c>
       <c r="B233" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C233" s="30"/>
       <c r="D233" s="26"/>
       <c r="E233" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F233" s="30"/>
       <c r="G233" s="30"/>
@@ -8108,12 +8116,12 @@
         <v>zonmwpa:Palliativecare</v>
       </c>
       <c r="B234" s="31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C234" s="30"/>
       <c r="D234" s="26"/>
       <c r="E234" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F234" s="30"/>
       <c r="G234" s="30"/>
@@ -8137,12 +8145,12 @@
         <v>zonmwpa:Impactofmeasuresorstrategies</v>
       </c>
       <c r="B235" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C235" s="30"/>
       <c r="D235" s="26"/>
       <c r="E235" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F235" s="30"/>
       <c r="G235" s="30"/>
@@ -8166,12 +8174,12 @@
         <v>zonmwpa:Resilienceofsociety</v>
       </c>
       <c r="B236" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C236" s="30"/>
       <c r="D236" s="26"/>
       <c r="E236" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F236" s="30"/>
       <c r="G236" s="30"/>
@@ -8195,12 +8203,12 @@
         <v>zonmwpa:Economicresilience</v>
       </c>
       <c r="B237" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C237" s="30"/>
       <c r="D237" s="26"/>
       <c r="E237" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F237" s="30"/>
       <c r="G237" s="30"/>
@@ -8224,12 +8232,12 @@
         <v>zonmwpa:OtherTheme</v>
       </c>
       <c r="B238" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C238" s="30"/>
       <c r="D238" s="26"/>
       <c r="E238" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F238" s="30"/>
       <c r="G238" s="30"/>
@@ -8253,11 +8261,11 @@
         <v>zonmwpa:Province</v>
       </c>
       <c r="B239" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C239" s="16"/>
       <c r="D239" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E239" s="17"/>
       <c r="F239" s="16" t="s">
@@ -8284,12 +8292,12 @@
         <v>zonmwpa:Drenthe</v>
       </c>
       <c r="B240" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C240" s="30"/>
       <c r="D240" s="26"/>
       <c r="E240" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F240" s="30"/>
       <c r="G240" s="30"/>
@@ -8313,12 +8321,12 @@
         <v>zonmwpa:Flevoland</v>
       </c>
       <c r="B241" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C241" s="30"/>
       <c r="D241" s="26"/>
       <c r="E241" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F241" s="30"/>
       <c r="G241" s="30"/>
@@ -8342,12 +8350,12 @@
         <v>zonmwpa:Friesland</v>
       </c>
       <c r="B242" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C242" s="30"/>
       <c r="D242" s="26"/>
       <c r="E242" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F242" s="30"/>
       <c r="G242" s="30"/>
@@ -8371,12 +8379,12 @@
         <v>zonmwpa:Gelderland</v>
       </c>
       <c r="B243" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C243" s="30"/>
       <c r="D243" s="26"/>
       <c r="E243" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F243" s="30"/>
       <c r="G243" s="30"/>
@@ -8400,12 +8408,12 @@
         <v>zonmwpa:Groningen</v>
       </c>
       <c r="B244" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C244" s="30"/>
       <c r="D244" s="26"/>
       <c r="E244" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F244" s="30"/>
       <c r="G244" s="30"/>
@@ -8429,12 +8437,12 @@
         <v>zonmwpa:Limburg</v>
       </c>
       <c r="B245" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C245" s="30"/>
       <c r="D245" s="26"/>
       <c r="E245" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F245" s="30"/>
       <c r="G245" s="30"/>
@@ -8458,12 +8466,12 @@
         <v>zonmwpa:Noord-Brabant</v>
       </c>
       <c r="B246" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C246" s="30"/>
       <c r="D246" s="26"/>
       <c r="E246" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F246" s="30"/>
       <c r="G246" s="30"/>
@@ -8487,12 +8495,12 @@
         <v>zonmwpa:Noord-Holland</v>
       </c>
       <c r="B247" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C247" s="30"/>
       <c r="D247" s="26"/>
       <c r="E247" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F247" s="30"/>
       <c r="G247" s="30"/>
@@ -8516,12 +8524,12 @@
         <v>zonmwpa:Overijssel</v>
       </c>
       <c r="B248" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C248" s="30"/>
       <c r="D248" s="26"/>
       <c r="E248" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F248" s="30"/>
       <c r="G248" s="30"/>
@@ -8545,12 +8553,12 @@
         <v>zonmwpa:Utrecht</v>
       </c>
       <c r="B249" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C249" s="30"/>
       <c r="D249" s="26"/>
       <c r="E249" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F249" s="30"/>
       <c r="G249" s="30"/>
@@ -8574,12 +8582,12 @@
         <v>zonmwpa:Zeeland</v>
       </c>
       <c r="B250" s="26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C250" s="30"/>
       <c r="D250" s="26"/>
       <c r="E250" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F250" s="30"/>
       <c r="G250" s="30"/>
@@ -8603,12 +8611,12 @@
         <v>zonmwpa:Zuid-Holland</v>
       </c>
       <c r="B251" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C251" s="30"/>
       <c r="D251" s="26"/>
       <c r="E251" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F251" s="30"/>
       <c r="G251" s="30"/>
@@ -8632,12 +8640,12 @@
         <v>zonmwpa:OtherProvince</v>
       </c>
       <c r="B252" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C252" s="30"/>
       <c r="D252" s="26"/>
       <c r="E252" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F252" s="30"/>
       <c r="G252" s="30"/>

</xml_diff>

<commit_message>
added http://www.w3.org/2001/XMLSchema# in prefix
</commit_message>
<xml_diff>
--- a/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
+++ b/ontology/FDCCOVIDProjectAdminVocabularies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary_Drive/work/repos/FAIR-data/zonmw-project-admin/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5D068-2190-2847-A3FE-05D09C8A77B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F0E74F-ED46-7146-9B9A-DC9DA6E2E3C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="44520" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="296">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -946,6 +946,12 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>xsd</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2001/XMLSchema#</t>
   </si>
 </sst>
 </file>
@@ -1422,10 +1428,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U1026"/>
+  <dimension ref="A1:U1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1585,14 +1591,16 @@
       <c r="U5" s="3"/>
     </row>
     <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
+      <c r="A6" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="41"/>
+        <v>294</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D6" s="43"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1613,7 +1621,7 @@
     </row>
     <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>10</v>
@@ -1640,10 +1648,10 @@
     </row>
     <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="41"/>
@@ -1667,10 +1675,10 @@
     </row>
     <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="41"/>
@@ -1694,10 +1702,10 @@
     </row>
     <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>286</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="41"/>
@@ -1721,12 +1729,12 @@
     </row>
     <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="C11" s="37"/>
+        <v>16</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="41"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1748,13 +1756,13 @@
     </row>
     <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>236</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="44"/>
+        <v>17</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1774,10 +1782,14 @@
       <c r="U12" s="3"/>
     </row>
     <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="41"/>
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1797,8 +1809,8 @@
       <c r="U13" s="3"/>
     </row>
     <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="41"/>
       <c r="E14" s="3"/>
@@ -1912,8 +1924,8 @@
       <c r="U18" s="3"/>
     </row>
     <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="3"/>
       <c r="D19" s="41"/>
       <c r="E19" s="3"/>
@@ -1934,37 +1946,17 @@
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
     </row>
-    <row r="20" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="45" t="s">
-        <v>292</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>27</v>
-      </c>
+    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1977,26 +1969,37 @@
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
     </row>
-    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="str">
-        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B21," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
-        <v>zonmwpa:Deprecated</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
+    <row r="21" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>292</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -2010,24 +2013,20 @@
       <c r="U21" s="3"/>
     </row>
     <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="str">
+      <c r="A22" s="16" t="str">
         <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B22," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
-        <v>zonmwpa:StudyArea</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="46" t="s">
-        <v>293</v>
-      </c>
+        <v>zonmwpa:Deprecated</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="46"/>
       <c r="E22" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G22" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="16" t="s">
         <v>30</v>
       </c>
       <c r="H22" s="18"/>
@@ -2046,25 +2045,29 @@
       <c r="U22" s="3"/>
     </row>
     <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="str">
+      <c r="A23" s="13" t="str">
         <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B23," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
-        <v>zonmwpa:Township</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="47" t="s">
+        <v>zonmwpa:StudyArea</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="21"/>
+      <c r="E23" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -2079,23 +2082,23 @@
     </row>
     <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="str">
-        <f t="shared" ref="A24:A86" si="0">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B24," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>zonmwpa:Rural</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="48" t="s">
+        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B24," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"),"ë","e"))</f>
+        <v>zonmwpa:Township</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="47" t="s">
         <v>293</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="25"/>
       <c r="J24" s="21"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -2111,24 +2114,24 @@
     </row>
     <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>zonmwpa:Multiplemunicipalities</v>
+        <f t="shared" ref="A25:A87" si="0">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B25," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>zonmwpa:Rural</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E25" s="19"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="21"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="28"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -2144,23 +2147,23 @@
     <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Provincial</v>
+        <v>zonmwpa:Multiplemunicipalities</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E26" s="22"/>
+      <c r="E26" s="19"/>
       <c r="F26" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="27"/>
+      <c r="G26" s="21"/>
       <c r="H26" s="28"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -2176,23 +2179,23 @@
     <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Regional</v>
+        <v>zonmwpa:Provincial</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E27" s="19"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="23" t="s">
         <v>32</v>
       </c>
       <c r="G27" s="27"/>
       <c r="H27" s="28"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -2208,10 +2211,10 @@
     <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Neighbourhood</v>
+        <v>zonmwpa:Regional</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="48" t="s">
@@ -2240,16 +2243,16 @@
     <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:OtherStudyArea</v>
+        <v>zonmwpa:Neighbourhood</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>284</v>
+        <v>37</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E29" s="26"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="23" t="s">
         <v>32</v>
       </c>
@@ -2270,29 +2273,25 @@
       <c r="U29" s="3"/>
     </row>
     <row r="30" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="str">
+      <c r="A30" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:SizeOfCollection</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="46" t="s">
+        <v>zonmwpa:OtherStudyArea</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E30" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="27"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -2306,25 +2305,29 @@
       <c r="U30" s="3"/>
     </row>
     <row r="31" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="19" t="str">
+      <c r="A31" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Under10</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="48" t="s">
+        <v>zonmwpa:SizeOfCollection</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="E31" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -2340,10 +2343,10 @@
     <row r="32" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:10-100</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>42</v>
+        <v>zonmwpa:Under10</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>41</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="48" t="s">
@@ -2372,10 +2375,10 @@
     <row r="33" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:100-1000</v>
+        <v>zonmwpa:10-100</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="48" t="s">
@@ -2404,10 +2407,10 @@
     <row r="34" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:1000-10.000</v>
+        <v>zonmwpa:100-1000</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="48" t="s">
@@ -2436,10 +2439,10 @@
     <row r="35" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:10.000-100.000</v>
+        <v>zonmwpa:1000-10.000</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="48" t="s">
@@ -2468,10 +2471,10 @@
     <row r="36" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:100.000-1.000.000</v>
+        <v>zonmwpa:10.000-100.000</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="48" t="s">
@@ -2500,10 +2503,10 @@
     <row r="37" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:1.000.000-10.000.000</v>
+        <v>zonmwpa:100.000-1.000.000</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="48" t="s">
@@ -2532,10 +2535,10 @@
     <row r="38" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:10.000.000-100.000.000</v>
+        <v>zonmwpa:1.000.000-10.000.000</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="27"/>
       <c r="D38" s="48" t="s">
@@ -2564,10 +2567,10 @@
     <row r="39" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:100.000.000-1.000.000.000</v>
+        <v>zonmwpa:10.000.000-100.000.000</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="48" t="s">
@@ -2577,7 +2580,7 @@
       <c r="F39" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G39" s="29"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="28"/>
       <c r="I39" s="27"/>
       <c r="J39" s="27"/>
@@ -2596,20 +2599,20 @@
     <row r="40" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:OtherSizeOfCollection</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>50</v>
+        <v>zonmwpa:100.000.000-1.000.000.000</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E40" s="26"/>
+      <c r="E40" s="19"/>
       <c r="F40" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G40" s="27"/>
+      <c r="G40" s="29"/>
       <c r="H40" s="28"/>
       <c r="I40" s="27"/>
       <c r="J40" s="27"/>
@@ -2626,29 +2629,25 @@
       <c r="U40" s="3"/>
     </row>
     <row r="41" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="13" t="str">
+      <c r="A41" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Service</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="46" t="s">
+        <v>zonmwpa:OtherSizeOfCollection</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E41" s="33" t="s">
-        <v>222</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G41" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G41" s="27"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -2662,25 +2661,29 @@
       <c r="U41" s="3"/>
     </row>
     <row r="42" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="str">
+      <c r="A42" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:BSL-2laboratoriesavailable</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="48" t="s">
+        <v>zonmwpa:Service</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="35" t="s">
-        <v>223</v>
-      </c>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
+      <c r="E42" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
@@ -2696,10 +2699,10 @@
     <row r="43" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:BSL-3laboratoriesavailable</v>
+        <v>zonmwpa:BSL-2laboratoriesavailable</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="27"/>
       <c r="D43" s="48" t="s">
@@ -2728,10 +2731,10 @@
     <row r="44" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:MemberCOVID-19Network</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>53</v>
+        <v>zonmwpa:BSL-3laboratoriesavailable</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="48" t="s">
@@ -2760,10 +2763,10 @@
     <row r="45" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:AntibodyDevelopment</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>54</v>
+        <v>zonmwpa:MemberCOVID-19Network</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="48" t="s">
@@ -2792,10 +2795,10 @@
     <row r="46" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:LaboratoriesdoingPCR-baseddiagnosis</v>
+        <v>zonmwpa:AntibodyDevelopment</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="48" t="s">
@@ -2824,10 +2827,10 @@
     <row r="47" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Proteomicsstudiesincludingproteinengineeringandproteininteractions</v>
+        <v>zonmwpa:LaboratoriesdoingPCR-baseddiagnosis</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="27"/>
       <c r="D47" s="48" t="s">
@@ -2856,10 +2859,10 @@
     <row r="48" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Screeningtoolsforsearchingvirusproteasesinhibitors</v>
+        <v>zonmwpa:Proteomicsstudiesincludingproteinengineeringandproteininteractions</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" s="27"/>
       <c r="D48" s="48" t="s">
@@ -2888,10 +2891,10 @@
     <row r="49" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:AnimalTestingFacility</v>
+        <v>zonmwpa:Screeningtoolsforsearchingvirusproteasesinhibitors</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="48" t="s">
@@ -2920,10 +2923,10 @@
     <row r="50" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Abilitytosetupclinicaltrials</v>
+        <v>zonmwpa:AnimalTestingFacility</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="27"/>
       <c r="D50" s="48" t="s">
@@ -2952,10 +2955,10 @@
     <row r="51" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:VirusSequencingFacility</v>
+        <v>zonmwpa:Abilitytosetupclinicaltrials</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51" s="27"/>
       <c r="D51" s="48" t="s">
@@ -2984,21 +2987,21 @@
     <row r="52" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:OtherServices</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>61</v>
+        <v>zonmwpa:VirusSequencingFacility</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="C52" s="27"/>
       <c r="D52" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E52" s="26"/>
+      <c r="E52" s="19"/>
       <c r="F52" s="35" t="s">
         <v>223</v>
       </c>
       <c r="G52" s="27"/>
-      <c r="H52" s="28"/>
+      <c r="H52" s="27"/>
       <c r="I52" s="27"/>
       <c r="J52" s="27"/>
       <c r="K52" s="3"/>
@@ -3014,29 +3017,25 @@
       <c r="U52" s="3"/>
     </row>
     <row r="53" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="13" t="str">
+      <c r="A53" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:TypeOfMaterial</v>
-      </c>
-      <c r="B53" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="46" t="s">
+        <v>zonmwpa:OtherServices</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="27"/>
+      <c r="D53" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E53" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="F53" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G53" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="G53" s="27"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="27"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
@@ -3050,25 +3049,29 @@
       <c r="U53" s="3"/>
     </row>
     <row r="54" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="19" t="str">
+      <c r="A54" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:BuffyCoat</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="48" t="s">
+        <v>zonmwpa:TypeOfMaterial</v>
+      </c>
+      <c r="B54" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E54" s="19"/>
-      <c r="F54" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
+      <c r="E54" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
@@ -3084,10 +3087,10 @@
     <row r="55" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:cDNADivmRNA</v>
+        <v>zonmwpa:BuffyCoat</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" s="27"/>
       <c r="D55" s="48" t="s">
@@ -3116,10 +3119,10 @@
     <row r="56" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Celllines</v>
+        <v>zonmwpa:cDNADivmRNA</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" s="27"/>
       <c r="D56" s="48" t="s">
@@ -3148,10 +3151,10 @@
     <row r="57" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:DNA</v>
+        <v>zonmwpa:Celllines</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="27"/>
       <c r="D57" s="48" t="s">
@@ -3180,10 +3183,10 @@
     <row r="58" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Faeces</v>
+        <v>zonmwpa:DNA</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="27"/>
       <c r="D58" s="48" t="s">
@@ -3212,10 +3215,10 @@
     <row r="59" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:microRNA</v>
+        <v>zonmwpa:Faeces</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" s="27"/>
       <c r="D59" s="48" t="s">
@@ -3244,10 +3247,10 @@
     <row r="60" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Nasalswab</v>
+        <v>zonmwpa:microRNA</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C60" s="27"/>
       <c r="D60" s="48" t="s">
@@ -3276,10 +3279,10 @@
     <row r="61" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Notavailable</v>
+        <v>zonmwpa:Nasalswab</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C61" s="27"/>
       <c r="D61" s="48" t="s">
@@ -3308,10 +3311,10 @@
     <row r="62" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Pathogen</v>
+        <v>zonmwpa:Notavailable</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C62" s="27"/>
       <c r="D62" s="48" t="s">
@@ -3340,10 +3343,10 @@
     <row r="63" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Peripheralbloodcells</v>
+        <v>zonmwpa:Pathogen</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C63" s="27"/>
       <c r="D63" s="48" t="s">
@@ -3372,10 +3375,10 @@
     <row r="64" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Plasma</v>
+        <v>zonmwpa:Peripheralbloodcells</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C64" s="27"/>
       <c r="D64" s="48" t="s">
@@ -3404,10 +3407,10 @@
     <row r="65" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:RNA</v>
+        <v>zonmwpa:Plasma</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C65" s="27"/>
       <c r="D65" s="48" t="s">
@@ -3436,10 +3439,10 @@
     <row r="66" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Saliva</v>
+        <v>zonmwpa:RNA</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" s="27"/>
       <c r="D66" s="48" t="s">
@@ -3468,10 +3471,10 @@
     <row r="67" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Serum</v>
+        <v>zonmwpa:Saliva</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C67" s="27"/>
       <c r="D67" s="48" t="s">
@@ -3500,10 +3503,10 @@
     <row r="68" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Throatswab</v>
+        <v>zonmwpa:Serum</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C68" s="27"/>
       <c r="D68" s="48" t="s">
@@ -3532,10 +3535,10 @@
     <row r="69" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Tissue-cryopreserved</v>
+        <v>zonmwpa:Throatswab</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C69" s="27"/>
       <c r="D69" s="48" t="s">
@@ -3564,10 +3567,10 @@
     <row r="70" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Tissue-paraffinpreserved</v>
+        <v>zonmwpa:Tissue-cryopreserved</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C70" s="27"/>
       <c r="D70" s="48" t="s">
@@ -3596,10 +3599,10 @@
     <row r="71" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Tissue-stainedsectionsDivslides</v>
+        <v>zonmwpa:Tissue-paraffinpreserved</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C71" s="27"/>
       <c r="D71" s="48" t="s">
@@ -3628,10 +3631,10 @@
     <row r="72" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Urine</v>
+        <v>zonmwpa:Tissue-stainedsectionsDivslides</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C72" s="27"/>
       <c r="D72" s="48" t="s">
@@ -3660,10 +3663,10 @@
     <row r="73" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:WholeBlood</v>
+        <v>zonmwpa:Urine</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C73" s="27"/>
       <c r="D73" s="48" t="s">
@@ -3692,21 +3695,21 @@
     <row r="74" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:OtherTypesOfMaterial</v>
-      </c>
-      <c r="B74" s="26" t="s">
-        <v>82</v>
+        <v>zonmwpa:WholeBlood</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="C74" s="27"/>
       <c r="D74" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E74" s="26"/>
+      <c r="E74" s="19"/>
       <c r="F74" s="34" t="s">
         <v>225</v>
       </c>
       <c r="G74" s="27"/>
-      <c r="H74" s="28"/>
+      <c r="H74" s="27"/>
       <c r="I74" s="27"/>
       <c r="J74" s="27"/>
       <c r="K74" s="3"/>
@@ -3722,29 +3725,25 @@
       <c r="U74" s="3"/>
     </row>
     <row r="75" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="13" t="str">
+      <c r="A75" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:TypeOfData</v>
-      </c>
-      <c r="B75" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="46" t="s">
+        <v>zonmwpa:OtherTypesOfMaterial</v>
+      </c>
+      <c r="B75" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" s="27"/>
+      <c r="D75" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E75" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="F75" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G75" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="G75" s="27"/>
+      <c r="H75" s="28"/>
+      <c r="I75" s="27"/>
+      <c r="J75" s="27"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
       <c r="M75" s="3"/>
@@ -3758,25 +3757,29 @@
       <c r="U75" s="3"/>
     </row>
     <row r="76" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="19" t="str">
+      <c r="A76" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Antibodiestiter-IgMandIgG</v>
-      </c>
-      <c r="B76" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C76" s="27"/>
-      <c r="D76" s="48" t="s">
+        <v>zonmwpa:TypeOfData</v>
+      </c>
+      <c r="B76" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="C76" s="15"/>
+      <c r="D76" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E76" s="19"/>
-      <c r="F76" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="G76" s="27"/>
-      <c r="H76" s="27"/>
-      <c r="I76" s="27"/>
-      <c r="J76" s="27"/>
+      <c r="E76" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G76" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
       <c r="M76" s="3"/>
@@ -3792,10 +3795,10 @@
     <row r="77" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Biologicalsamples</v>
+        <v>zonmwpa:Antibodiestiter-IgMandIgG</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C77" s="27"/>
       <c r="D77" s="48" t="s">
@@ -3824,10 +3827,10 @@
     <row r="78" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Bloodcountandotherlabresultsespeciallyatthemomentofhospitaladmission</v>
+        <v>zonmwpa:Biologicalsamples</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C78" s="27"/>
       <c r="D78" s="48" t="s">
@@ -3856,10 +3859,10 @@
     <row r="79" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Dataonclinicalsymptoms</v>
+        <v>zonmwpa:Bloodcountandotherlabresultsespeciallyatthemomentofhospitaladmission</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C79" s="27"/>
       <c r="D79" s="48" t="s">
@@ -3888,10 +3891,10 @@
     <row r="80" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:CTimagingoflungs-alternativelyXray</v>
+        <v>zonmwpa:Dataonclinicalsymptoms</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C80" s="27"/>
       <c r="D80" s="48" t="s">
@@ -3920,10 +3923,10 @@
     <row r="81" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Dataondiseasedurationanddiseaseoutcome</v>
+        <v>zonmwpa:CTimagingoflungs-alternativelyXray</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C81" s="27"/>
       <c r="D81" s="48" t="s">
@@ -3952,10 +3955,10 @@
     <row r="82" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Genealogicalrecords</v>
+        <v>zonmwpa:Dataondiseasedurationanddiseaseoutcome</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C82" s="27"/>
       <c r="D82" s="48" t="s">
@@ -3984,10 +3987,10 @@
     <row r="83" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Imagingdata</v>
+        <v>zonmwpa:Genealogicalrecords</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C83" s="27"/>
       <c r="D83" s="48" t="s">
@@ -4016,10 +4019,10 @@
     <row r="84" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Medicalrecords</v>
+        <v>zonmwpa:Imagingdata</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C84" s="27"/>
       <c r="D84" s="48" t="s">
@@ -4048,10 +4051,10 @@
     <row r="85" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:Nationalregistries</v>
+        <v>zonmwpa:Medicalrecords</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C85" s="27"/>
       <c r="D85" s="48" t="s">
@@ -4080,10 +4083,10 @@
     <row r="86" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>zonmwpa:PhysiologicalDivBiochemicalmeasurements</v>
+        <v>zonmwpa:Nationalregistries</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C86" s="27"/>
       <c r="D86" s="48" t="s">
@@ -4111,11 +4114,11 @@
     </row>
     <row r="87" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="19" t="str">
-        <f t="shared" ref="A87:A113" si="1">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B87," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>zonmwpa:Surveydata</v>
+        <f t="shared" si="0"/>
+        <v>zonmwpa:PhysiologicalDivBiochemicalmeasurements</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C87" s="27"/>
       <c r="D87" s="48" t="s">
@@ -4143,11 +4146,11 @@
     </row>
     <row r="88" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>zonmwpa:Treatmentprotocol-typesofdrugsused</v>
+        <f t="shared" ref="A88:A114" si="1">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B88," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>zonmwpa:Surveydata</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="48" t="s">
@@ -4176,10 +4179,10 @@
     <row r="89" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Notavailable</v>
+        <v>zonmwpa:Treatmentprotocol-typesofdrugsused</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C89" s="27"/>
       <c r="D89" s="48" t="s">
@@ -4208,21 +4211,21 @@
     <row r="90" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:OtherTypesOfData</v>
-      </c>
-      <c r="B90" s="26" t="s">
-        <v>96</v>
+        <v>zonmwpa:Notavailable</v>
+      </c>
+      <c r="B90" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="C90" s="27"/>
       <c r="D90" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E90" s="26"/>
+      <c r="E90" s="19"/>
       <c r="F90" s="34" t="s">
         <v>228</v>
       </c>
       <c r="G90" s="27"/>
-      <c r="H90" s="28"/>
+      <c r="H90" s="27"/>
       <c r="I90" s="27"/>
       <c r="J90" s="27"/>
       <c r="K90" s="3"/>
@@ -4238,29 +4241,25 @@
       <c r="U90" s="3"/>
     </row>
     <row r="91" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="13" t="str">
+      <c r="A91" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:TypeOfCollection</v>
-      </c>
-      <c r="B91" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="C91" s="15"/>
-      <c r="D91" s="46" t="s">
+        <v>zonmwpa:OtherTypesOfData</v>
+      </c>
+      <c r="B91" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C91" s="27"/>
+      <c r="D91" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E91" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="F91" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G91" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="18"/>
-      <c r="I91" s="18"/>
-      <c r="J91" s="18"/>
+      <c r="E91" s="26"/>
+      <c r="F91" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="G91" s="27"/>
+      <c r="H91" s="28"/>
+      <c r="I91" s="27"/>
+      <c r="J91" s="27"/>
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
       <c r="M91" s="3"/>
@@ -4274,25 +4273,29 @@
       <c r="U91" s="3"/>
     </row>
     <row r="92" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="19" t="str">
+      <c r="A92" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Birthcohort</v>
-      </c>
-      <c r="B92" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C92" s="27"/>
-      <c r="D92" s="48" t="s">
+        <v>zonmwpa:TypeOfCollection</v>
+      </c>
+      <c r="B92" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="C92" s="15"/>
+      <c r="D92" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E92" s="19"/>
-      <c r="F92" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="G92" s="27"/>
-      <c r="H92" s="27"/>
-      <c r="I92" s="27"/>
-      <c r="J92" s="27"/>
+      <c r="E92" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="F92" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G92" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+      <c r="J92" s="18"/>
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
       <c r="M92" s="3"/>
@@ -4308,10 +4311,10 @@
     <row r="93" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Case-Control</v>
+        <v>zonmwpa:Birthcohort</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C93" s="27"/>
       <c r="D93" s="48" t="s">
@@ -4340,10 +4343,10 @@
     <row r="94" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Cohort</v>
+        <v>zonmwpa:Case-Control</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C94" s="27"/>
       <c r="D94" s="48" t="s">
@@ -4372,10 +4375,10 @@
     <row r="95" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Cross-sectional</v>
+        <v>zonmwpa:Cohort</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C95" s="27"/>
       <c r="D95" s="48" t="s">
@@ -4404,10 +4407,10 @@
     <row r="96" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Diseasespecific</v>
+        <v>zonmwpa:Cross-sectional</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C96" s="27"/>
       <c r="D96" s="48" t="s">
@@ -4436,10 +4439,10 @@
     <row r="97" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Hospital</v>
+        <v>zonmwpa:Diseasespecific</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C97" s="27"/>
       <c r="D97" s="48" t="s">
@@ -4468,10 +4471,10 @@
     <row r="98" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Imagecollection</v>
+        <v>zonmwpa:Hospital</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C98" s="27"/>
       <c r="D98" s="48" t="s">
@@ -4500,10 +4503,10 @@
     <row r="99" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Longitudinal</v>
+        <v>zonmwpa:Imagecollection</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C99" s="27"/>
       <c r="D99" s="48" t="s">
@@ -4532,10 +4535,10 @@
     <row r="100" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Non-human</v>
+        <v>zonmwpa:Longitudinal</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C100" s="27"/>
       <c r="D100" s="48" t="s">
@@ -4564,16 +4567,16 @@
     <row r="101" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:OtherTypeofCollection</v>
-      </c>
-      <c r="B101" s="26" t="s">
-        <v>106</v>
+        <v>zonmwpa:Non-human</v>
+      </c>
+      <c r="B101" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="C101" s="27"/>
       <c r="D101" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E101" s="26"/>
+      <c r="E101" s="19"/>
       <c r="F101" s="34" t="s">
         <v>232</v>
       </c>
@@ -4596,16 +4599,16 @@
     <row r="102" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Population-based</v>
-      </c>
-      <c r="B102" s="19" t="s">
-        <v>107</v>
+        <v>zonmwpa:OtherTypeofCollection</v>
+      </c>
+      <c r="B102" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="C102" s="27"/>
       <c r="D102" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E102" s="19"/>
+      <c r="E102" s="26"/>
       <c r="F102" s="34" t="s">
         <v>232</v>
       </c>
@@ -4628,10 +4631,10 @@
     <row r="103" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Prospectivestudy</v>
+        <v>zonmwpa:Population-based</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C103" s="27"/>
       <c r="D103" s="48" t="s">
@@ -4660,10 +4663,10 @@
     <row r="104" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Qualitycontrol</v>
+        <v>zonmwpa:Prospectivestudy</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C104" s="27"/>
       <c r="D104" s="48" t="s">
@@ -4692,10 +4695,10 @@
     <row r="105" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Rarediseasecollection</v>
+        <v>zonmwpa:Qualitycontrol</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C105" s="27"/>
       <c r="D105" s="48" t="s">
@@ -4724,10 +4727,10 @@
     <row r="106" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Samplecollection</v>
+        <v>zonmwpa:Rarediseasecollection</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C106" s="27"/>
       <c r="D106" s="48" t="s">
@@ -4756,10 +4759,10 @@
     <row r="107" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Twin-study</v>
+        <v>zonmwpa:Samplecollection</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C107" s="27"/>
       <c r="D107" s="48" t="s">
@@ -4786,29 +4789,25 @@
       <c r="U107" s="3"/>
     </row>
     <row r="108" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A108" s="13" t="str">
+      <c r="A108" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Population</v>
-      </c>
-      <c r="B108" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C108" s="15"/>
-      <c r="D108" s="46" t="s">
+        <v>zonmwpa:Twin-study</v>
+      </c>
+      <c r="B108" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C108" s="27"/>
+      <c r="D108" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E108" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="F108" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G108" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H108" s="18"/>
-      <c r="I108" s="18"/>
-      <c r="J108" s="18"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="G108" s="27"/>
+      <c r="H108" s="27"/>
+      <c r="I108" s="27"/>
+      <c r="J108" s="27"/>
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
       <c r="M108" s="3"/>
@@ -4822,25 +4821,29 @@
       <c r="U108" s="3"/>
     </row>
     <row r="109" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="19" t="str">
+      <c r="A109" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Populationwide</v>
-      </c>
-      <c r="B109" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="C109" s="27"/>
-      <c r="D109" s="48" t="s">
+        <v>zonmwpa:Population</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C109" s="15"/>
+      <c r="D109" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E109" s="19"/>
-      <c r="F109" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="27"/>
+      <c r="E109" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="F109" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G109" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H109" s="18"/>
+      <c r="I109" s="18"/>
+      <c r="J109" s="18"/>
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
       <c r="M109" s="3"/>
@@ -4856,10 +4859,10 @@
     <row r="110" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Neonates</v>
+        <v>zonmwpa:Populationwide</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C110" s="27"/>
       <c r="D110" s="48" t="s">
@@ -4888,10 +4891,10 @@
     <row r="111" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Children-0-18years</v>
+        <v>zonmwpa:Neonates</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C111" s="27"/>
       <c r="D111" s="48" t="s">
@@ -4920,10 +4923,10 @@
     <row r="112" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Primaryschoolchildren-4-12years</v>
+        <v>zonmwpa:Children-0-18years</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C112" s="27"/>
       <c r="D112" s="48" t="s">
@@ -4952,10 +4955,10 @@
     <row r="113" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>zonmwpa:Teenager-12-18years</v>
+        <v>zonmwpa:Primaryschoolchildren-4-12years</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C113" s="27"/>
       <c r="D113" s="48" t="s">
@@ -4983,11 +4986,11 @@
     </row>
     <row r="114" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="19" t="str">
-        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B114," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>zonmwpa:Youngpeople-16-27years</v>
+        <f t="shared" si="1"/>
+        <v>zonmwpa:Teenager-12-18years</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C114" s="27"/>
       <c r="D114" s="48" t="s">
@@ -5015,11 +5018,11 @@
     </row>
     <row r="115" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="19" t="str">
-        <f t="shared" ref="A115:A178" si="2">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B115," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>zonmwpa:Youngadults18-21years</v>
+        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B115," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>zonmwpa:Youngpeople-16-27years</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C115" s="27"/>
       <c r="D115" s="48" t="s">
@@ -5047,11 +5050,11 @@
     </row>
     <row r="116" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>zonmwpa:Adults-18-65years</v>
+        <f t="shared" ref="A116:A179" si="2">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B116," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>zonmwpa:Youngadults18-21years</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C116" s="27"/>
       <c r="D116" s="48" t="s">
@@ -5080,10 +5083,10 @@
     <row r="117" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Elderly-65plus</v>
+        <v>zonmwpa:Adults-18-65years</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C117" s="27"/>
       <c r="D117" s="48" t="s">
@@ -5112,10 +5115,10 @@
     <row r="118" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Vulnerableelderly</v>
+        <v>zonmwpa:Elderly-65plus</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C118" s="27"/>
       <c r="D118" s="48" t="s">
@@ -5144,10 +5147,10 @@
     <row r="119" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Pregnantwomen</v>
+        <v>zonmwpa:Vulnerableelderly</v>
       </c>
       <c r="B119" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C119" s="27"/>
       <c r="D119" s="48" t="s">
@@ -5176,10 +5179,10 @@
     <row r="120" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Peoplewithaspecificethnicbackground</v>
+        <v>zonmwpa:Pregnantwomen</v>
       </c>
       <c r="B120" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C120" s="27"/>
       <c r="D120" s="48" t="s">
@@ -5208,10 +5211,10 @@
     <row r="121" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Peoplewithamigrationbackground</v>
+        <v>zonmwpa:Peoplewithaspecificethnicbackground</v>
       </c>
       <c r="B121" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C121" s="27"/>
       <c r="D121" s="48" t="s">
@@ -5240,10 +5243,10 @@
     <row r="122" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Peoplewithachronicillness</v>
+        <v>zonmwpa:Peoplewithamigrationbackground</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C122" s="27"/>
       <c r="D122" s="48" t="s">
@@ -5272,10 +5275,10 @@
     <row r="123" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Peoplewithaphysicaldisability</v>
+        <v>zonmwpa:Peoplewithachronicillness</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C123" s="27"/>
       <c r="D123" s="48" t="s">
@@ -5304,10 +5307,10 @@
     <row r="124" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Mentallychallengedpeople</v>
+        <v>zonmwpa:Peoplewithaphysicaldisability</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C124" s="27"/>
       <c r="D124" s="48" t="s">
@@ -5336,10 +5339,10 @@
     <row r="125" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Peoplewithararecondition</v>
+        <v>zonmwpa:Mentallychallengedpeople</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C125" s="27"/>
       <c r="D125" s="48" t="s">
@@ -5368,10 +5371,10 @@
     <row r="126" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Peoplewithalowsocio-economicstatus</v>
+        <v>zonmwpa:Peoplewithararecondition</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C126" s="27"/>
       <c r="D126" s="48" t="s">
@@ -5400,10 +5403,10 @@
     <row r="127" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Workingpeople</v>
+        <v>zonmwpa:Peoplewithalowsocio-economicstatus</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C127" s="27"/>
       <c r="D127" s="48" t="s">
@@ -5432,10 +5435,10 @@
     <row r="128" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Topathletes</v>
-      </c>
-      <c r="B128" s="26" t="s">
-        <v>135</v>
+        <v>zonmwpa:Workingpeople</v>
+      </c>
+      <c r="B128" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="C128" s="27"/>
       <c r="D128" s="48" t="s">
@@ -5464,10 +5467,10 @@
     <row r="129" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Men</v>
-      </c>
-      <c r="B129" s="19" t="s">
-        <v>136</v>
+        <v>zonmwpa:Topathletes</v>
+      </c>
+      <c r="B129" s="26" t="s">
+        <v>135</v>
       </c>
       <c r="C129" s="27"/>
       <c r="D129" s="48" t="s">
@@ -5496,10 +5499,10 @@
     <row r="130" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Women</v>
+        <v>zonmwpa:Men</v>
       </c>
       <c r="B130" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C130" s="27"/>
       <c r="D130" s="48" t="s">
@@ -5528,16 +5531,16 @@
     <row r="131" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:OtherPopulation</v>
-      </c>
-      <c r="B131" s="26" t="s">
-        <v>138</v>
+        <v>zonmwpa:Women</v>
+      </c>
+      <c r="B131" s="19" t="s">
+        <v>137</v>
       </c>
       <c r="C131" s="27"/>
       <c r="D131" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E131" s="26"/>
+      <c r="E131" s="19"/>
       <c r="F131" s="30" t="s">
         <v>116</v>
       </c>
@@ -5558,29 +5561,25 @@
       <c r="U131" s="3"/>
     </row>
     <row r="132" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A132" s="13" t="str">
+      <c r="A132" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:CareProcessPhase</v>
-      </c>
-      <c r="B132" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C132" s="15"/>
-      <c r="D132" s="46" t="s">
+        <v>zonmwpa:OtherPopulation</v>
+      </c>
+      <c r="B132" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C132" s="27"/>
+      <c r="D132" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E132" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F132" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G132" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H132" s="18"/>
-      <c r="I132" s="18"/>
-      <c r="J132" s="18"/>
+      <c r="E132" s="26"/>
+      <c r="F132" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="G132" s="27"/>
+      <c r="H132" s="27"/>
+      <c r="I132" s="27"/>
+      <c r="J132" s="27"/>
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
       <c r="M132" s="3"/>
@@ -5594,25 +5593,29 @@
       <c r="U132" s="3"/>
     </row>
     <row r="133" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A133" s="19" t="str">
+      <c r="A133" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Prevention</v>
-      </c>
-      <c r="B133" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="C133" s="27"/>
-      <c r="D133" s="48" t="s">
+        <v>zonmwpa:CareProcessPhase</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C133" s="15"/>
+      <c r="D133" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E133" s="19"/>
-      <c r="F133" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="G133" s="27"/>
-      <c r="H133" s="27"/>
-      <c r="I133" s="27"/>
-      <c r="J133" s="27"/>
+      <c r="E133" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F133" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G133" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H133" s="18"/>
+      <c r="I133" s="18"/>
+      <c r="J133" s="18"/>
       <c r="K133" s="3"/>
       <c r="L133" s="3"/>
       <c r="M133" s="3"/>
@@ -5628,10 +5631,10 @@
     <row r="134" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Diagnosis</v>
+        <v>zonmwpa:Prevention</v>
       </c>
       <c r="B134" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C134" s="27"/>
       <c r="D134" s="48" t="s">
@@ -5660,10 +5663,10 @@
     <row r="135" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Therapy</v>
+        <v>zonmwpa:Diagnosis</v>
       </c>
       <c r="B135" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C135" s="27"/>
       <c r="D135" s="48" t="s">
@@ -5692,10 +5695,10 @@
     <row r="136" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Follow-up</v>
+        <v>zonmwpa:Therapy</v>
       </c>
       <c r="B136" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C136" s="27"/>
       <c r="D136" s="48" t="s">
@@ -5724,10 +5727,10 @@
     <row r="137" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Aftercare</v>
+        <v>zonmwpa:Follow-up</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C137" s="27"/>
       <c r="D137" s="48" t="s">
@@ -5756,10 +5759,10 @@
     <row r="138" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Palliative</v>
+        <v>zonmwpa:Aftercare</v>
       </c>
       <c r="B138" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C138" s="27"/>
       <c r="D138" s="48" t="s">
@@ -5788,10 +5791,10 @@
     <row r="139" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Information</v>
+        <v>zonmwpa:Palliative</v>
       </c>
       <c r="B139" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C139" s="27"/>
       <c r="D139" s="48" t="s">
@@ -5820,10 +5823,10 @@
     <row r="140" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Earlydetection-screening</v>
+        <v>zonmwpa:Information</v>
       </c>
       <c r="B140" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C140" s="27"/>
       <c r="D140" s="48" t="s">
@@ -5852,10 +5855,10 @@
     <row r="141" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Organizationofcare</v>
+        <v>zonmwpa:Earlydetection-screening</v>
       </c>
       <c r="B141" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C141" s="27"/>
       <c r="D141" s="48" t="s">
@@ -5884,16 +5887,16 @@
     <row r="142" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:OtherCareProcessPhase</v>
-      </c>
-      <c r="B142" s="26" t="s">
-        <v>151</v>
+        <v>zonmwpa:Organizationofcare</v>
+      </c>
+      <c r="B142" s="19" t="s">
+        <v>150</v>
       </c>
       <c r="C142" s="27"/>
       <c r="D142" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E142" s="26"/>
+      <c r="E142" s="19"/>
       <c r="F142" s="30" t="s">
         <v>142</v>
       </c>
@@ -5914,29 +5917,25 @@
       <c r="U142" s="3"/>
     </row>
     <row r="143" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" s="13" t="str">
+      <c r="A143" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Setting</v>
-      </c>
-      <c r="B143" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C143" s="15"/>
-      <c r="D143" s="46" t="s">
+        <v>zonmwpa:OtherCareProcessPhase</v>
+      </c>
+      <c r="B143" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C143" s="27"/>
+      <c r="D143" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E143" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="F143" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G143" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H143" s="18"/>
-      <c r="I143" s="18"/>
-      <c r="J143" s="18"/>
+      <c r="E143" s="26"/>
+      <c r="F143" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="G143" s="27"/>
+      <c r="H143" s="27"/>
+      <c r="I143" s="27"/>
+      <c r="J143" s="27"/>
       <c r="K143" s="3"/>
       <c r="L143" s="3"/>
       <c r="M143" s="3"/>
@@ -5950,25 +5949,29 @@
       <c r="U143" s="3"/>
     </row>
     <row r="144" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A144" s="19" t="str">
+      <c r="A144" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Primarycare</v>
-      </c>
-      <c r="B144" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="C144" s="27"/>
-      <c r="D144" s="48" t="s">
+        <v>zonmwpa:Setting</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C144" s="15"/>
+      <c r="D144" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E144" s="19"/>
-      <c r="F144" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="G144" s="27"/>
-      <c r="H144" s="27"/>
-      <c r="I144" s="27"/>
-      <c r="J144" s="27"/>
+      <c r="E144" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F144" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G144" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H144" s="18"/>
+      <c r="I144" s="18"/>
+      <c r="J144" s="18"/>
       <c r="K144" s="3"/>
       <c r="L144" s="3"/>
       <c r="M144" s="3"/>
@@ -5984,10 +5987,10 @@
     <row r="145" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Second-linecare</v>
+        <v>zonmwpa:Primarycare</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C145" s="27"/>
       <c r="D145" s="48" t="s">
@@ -6016,10 +6019,10 @@
     <row r="146" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Prevention</v>
+        <v>zonmwpa:Second-linecare</v>
       </c>
       <c r="B146" s="19" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="C146" s="27"/>
       <c r="D146" s="48" t="s">
@@ -6048,10 +6051,10 @@
     <row r="147" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Healthcareinstitution</v>
+        <v>zonmwpa:Prevention</v>
       </c>
       <c r="B147" s="19" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C147" s="27"/>
       <c r="D147" s="48" t="s">
@@ -6080,10 +6083,10 @@
     <row r="148" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Cattle</v>
+        <v>zonmwpa:Healthcareinstitution</v>
       </c>
       <c r="B148" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C148" s="27"/>
       <c r="D148" s="48" t="s">
@@ -6112,10 +6115,10 @@
     <row r="149" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Transmural</v>
+        <v>zonmwpa:Cattle</v>
       </c>
       <c r="B149" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C149" s="27"/>
       <c r="D149" s="48" t="s">
@@ -6144,10 +6147,10 @@
     <row r="150" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Nursinghomecare</v>
+        <v>zonmwpa:Transmural</v>
       </c>
       <c r="B150" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C150" s="27"/>
       <c r="D150" s="48" t="s">
@@ -6176,10 +6179,10 @@
     <row r="151" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Hospitalcare</v>
+        <v>zonmwpa:Nursinghomecare</v>
       </c>
       <c r="B151" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C151" s="27"/>
       <c r="D151" s="48" t="s">
@@ -6208,10 +6211,10 @@
     <row r="152" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Homecare</v>
+        <v>zonmwpa:Hospitalcare</v>
       </c>
       <c r="B152" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C152" s="27"/>
       <c r="D152" s="48" t="s">
@@ -6240,10 +6243,10 @@
     <row r="153" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Education-schoolandupbringing</v>
+        <v>zonmwpa:Homecare</v>
       </c>
       <c r="B153" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C153" s="27"/>
       <c r="D153" s="48" t="s">
@@ -6272,10 +6275,10 @@
     <row r="154" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:WorkandIncome</v>
-      </c>
-      <c r="B154" s="26" t="s">
-        <v>164</v>
+        <v>zonmwpa:Education-schoolandupbringing</v>
+      </c>
+      <c r="B154" s="19" t="s">
+        <v>163</v>
       </c>
       <c r="C154" s="27"/>
       <c r="D154" s="48" t="s">
@@ -6304,10 +6307,10 @@
     <row r="155" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Neighbourhood</v>
-      </c>
-      <c r="B155" s="19" t="s">
-        <v>37</v>
+        <v>zonmwpa:WorkandIncome</v>
+      </c>
+      <c r="B155" s="26" t="s">
+        <v>164</v>
       </c>
       <c r="C155" s="27"/>
       <c r="D155" s="48" t="s">
@@ -6336,10 +6339,10 @@
     <row r="156" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Care</v>
+        <v>zonmwpa:Neighbourhood</v>
       </c>
       <c r="B156" s="19" t="s">
-        <v>165</v>
+        <v>37</v>
       </c>
       <c r="C156" s="27"/>
       <c r="D156" s="48" t="s">
@@ -6368,10 +6371,10 @@
     <row r="157" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Earlydetection-screening</v>
+        <v>zonmwpa:Care</v>
       </c>
       <c r="B157" s="19" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C157" s="27"/>
       <c r="D157" s="48" t="s">
@@ -6400,10 +6403,10 @@
     <row r="158" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Justice</v>
+        <v>zonmwpa:Earlydetection-screening</v>
       </c>
       <c r="B158" s="19" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C158" s="27"/>
       <c r="D158" s="48" t="s">
@@ -6432,10 +6435,10 @@
     <row r="159" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Socialdomain</v>
+        <v>zonmwpa:Justice</v>
       </c>
       <c r="B159" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C159" s="27"/>
       <c r="D159" s="48" t="s">
@@ -6464,10 +6467,10 @@
     <row r="160" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Youth</v>
+        <v>zonmwpa:Socialdomain</v>
       </c>
       <c r="B160" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C160" s="27"/>
       <c r="D160" s="48" t="s">
@@ -6496,10 +6499,10 @@
     <row r="161" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:SocialSupport</v>
+        <v>zonmwpa:Youth</v>
       </c>
       <c r="B161" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C161" s="27"/>
       <c r="D161" s="48" t="s">
@@ -6528,10 +6531,10 @@
     <row r="162" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:SportDivhealthDivwellness</v>
+        <v>zonmwpa:SocialSupport</v>
       </c>
       <c r="B162" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C162" s="27"/>
       <c r="D162" s="48" t="s">
@@ -6560,10 +6563,10 @@
     <row r="163" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Disabledcare</v>
+        <v>zonmwpa:SportDivhealthDivwellness</v>
       </c>
       <c r="B163" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C163" s="27"/>
       <c r="D163" s="48" t="s">
@@ -6592,10 +6595,10 @@
     <row r="164" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Long-termmentalhealthcare</v>
-      </c>
-      <c r="B164" s="26" t="s">
-        <v>172</v>
+        <v>zonmwpa:Disabledcare</v>
+      </c>
+      <c r="B164" s="19" t="s">
+        <v>171</v>
       </c>
       <c r="C164" s="27"/>
       <c r="D164" s="48" t="s">
@@ -6624,10 +6627,10 @@
     <row r="165" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Youth-healthcare</v>
+        <v>zonmwpa:Long-termmentalhealthcare</v>
       </c>
       <c r="B165" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C165" s="27"/>
       <c r="D165" s="48" t="s">
@@ -6656,10 +6659,10 @@
     <row r="166" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Generalpractitionercare</v>
-      </c>
-      <c r="B166" s="19" t="s">
-        <v>174</v>
+        <v>zonmwpa:Youth-healthcare</v>
+      </c>
+      <c r="B166" s="26" t="s">
+        <v>173</v>
       </c>
       <c r="C166" s="27"/>
       <c r="D166" s="48" t="s">
@@ -6688,10 +6691,10 @@
     <row r="167" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Elderlycare</v>
+        <v>zonmwpa:Generalpractitionercare</v>
       </c>
       <c r="B167" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C167" s="27"/>
       <c r="D167" s="48" t="s">
@@ -6720,10 +6723,10 @@
     <row r="168" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:ClientsandDivorpatientorganization</v>
+        <v>zonmwpa:Elderlycare</v>
       </c>
       <c r="B168" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C168" s="27"/>
       <c r="D168" s="48" t="s">
@@ -6752,10 +6755,10 @@
     <row r="169" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Measuringinstrument</v>
+        <v>zonmwpa:ClientsandDivorpatientorganization</v>
       </c>
       <c r="B169" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C169" s="27"/>
       <c r="D169" s="48" t="s">
@@ -6784,10 +6787,10 @@
     <row r="170" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Experimentalgarden</v>
+        <v>zonmwpa:Measuringinstrument</v>
       </c>
       <c r="B170" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C170" s="27"/>
       <c r="D170" s="48" t="s">
@@ -6816,16 +6819,16 @@
     <row r="171" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:OtherSetting</v>
-      </c>
-      <c r="B171" s="26" t="s">
-        <v>179</v>
+        <v>zonmwpa:Experimentalgarden</v>
+      </c>
+      <c r="B171" s="19" t="s">
+        <v>178</v>
       </c>
       <c r="C171" s="27"/>
       <c r="D171" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E171" s="26"/>
+      <c r="E171" s="19"/>
       <c r="F171" s="30" t="s">
         <v>155</v>
       </c>
@@ -6846,25 +6849,25 @@
       <c r="U171" s="3"/>
     </row>
     <row r="172" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A172" s="16" t="str">
+      <c r="A172" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:Institution</v>
-      </c>
-      <c r="B172" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="C172" s="16"/>
-      <c r="D172" s="46"/>
-      <c r="E172" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="F172" s="17"/>
-      <c r="G172" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H172" s="18"/>
-      <c r="I172" s="18"/>
-      <c r="J172" s="18"/>
+        <v>zonmwpa:OtherSetting</v>
+      </c>
+      <c r="B172" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="C172" s="27"/>
+      <c r="D172" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="E172" s="26"/>
+      <c r="F172" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="G172" s="27"/>
+      <c r="H172" s="27"/>
+      <c r="I172" s="27"/>
+      <c r="J172" s="27"/>
       <c r="K172" s="3"/>
       <c r="L172" s="3"/>
       <c r="M172" s="3"/>
@@ -6878,23 +6881,25 @@
       <c r="U172" s="3"/>
     </row>
     <row r="173" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A173" s="26" t="str">
+      <c r="A173" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:AcademicMedicalCenter-AmsterdamUMC</v>
-      </c>
-      <c r="B173" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="C173" s="30"/>
-      <c r="D173" s="48"/>
-      <c r="E173" s="26"/>
-      <c r="F173" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="G173" s="30"/>
-      <c r="H173" s="30"/>
-      <c r="I173" s="30"/>
-      <c r="J173" s="30"/>
+        <v>zonmwpa:Institution</v>
+      </c>
+      <c r="B173" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="C173" s="16"/>
+      <c r="D173" s="46"/>
+      <c r="E173" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="F173" s="17"/>
+      <c r="G173" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H173" s="18"/>
+      <c r="I173" s="18"/>
+      <c r="J173" s="18"/>
       <c r="K173" s="3"/>
       <c r="L173" s="3"/>
       <c r="M173" s="3"/>
@@ -6910,10 +6915,10 @@
     <row r="174" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:AmsterdamHealthandTechnologyInstitute-AHTI</v>
+        <v>zonmwpa:AcademicMedicalCenter-AmsterdamUMC</v>
       </c>
       <c r="B174" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C174" s="30"/>
       <c r="D174" s="48"/>
@@ -6940,10 +6945,10 @@
     <row r="175" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:DelftUniversityofTechnology</v>
+        <v>zonmwpa:AmsterdamHealthandTechnologyInstitute-AHTI</v>
       </c>
       <c r="B175" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C175" s="30"/>
       <c r="D175" s="48"/>
@@ -6970,10 +6975,10 @@
     <row r="176" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:EindhovenUniversityofTechnology</v>
+        <v>zonmwpa:DelftUniversityofTechnology</v>
       </c>
       <c r="B176" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C176" s="30"/>
       <c r="D176" s="48"/>
@@ -7000,10 +7005,10 @@
     <row r="177" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:ErasmusCentrumvoorZorgbestuur</v>
+        <v>zonmwpa:EindhovenUniversityofTechnology</v>
       </c>
       <c r="B177" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C177" s="30"/>
       <c r="D177" s="48"/>
@@ -7030,10 +7035,10 @@
     <row r="178" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>zonmwpa:ErasmusMC</v>
+        <v>zonmwpa:ErasmusCentrumvoorZorgbestuur</v>
       </c>
       <c r="B178" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C178" s="30"/>
       <c r="D178" s="48"/>
@@ -7057,13 +7062,13 @@
       <c r="T178" s="3"/>
       <c r="U178" s="3"/>
     </row>
-    <row r="179" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="26" t="str">
-        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B179," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>zonmwpa:ErasmusUniversityRotterdam</v>
-      </c>
-      <c r="B179" s="38" t="s">
-        <v>243</v>
+        <f t="shared" si="2"/>
+        <v>zonmwpa:ErasmusMC</v>
+      </c>
+      <c r="B179" s="31" t="s">
+        <v>242</v>
       </c>
       <c r="C179" s="30"/>
       <c r="D179" s="48"/>
@@ -7087,13 +7092,13 @@
       <c r="T179" s="3"/>
       <c r="U179" s="3"/>
     </row>
-    <row r="180" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="26" t="str">
-        <f t="shared" ref="A180:A233" si="3">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B180," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>zonmwpa:ExpertisecentrumNederlands</v>
-      </c>
-      <c r="B180" s="31" t="s">
-        <v>244</v>
+        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B180," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>zonmwpa:ErasmusUniversityRotterdam</v>
+      </c>
+      <c r="B180" s="38" t="s">
+        <v>243</v>
       </c>
       <c r="C180" s="30"/>
       <c r="D180" s="48"/>
@@ -7119,11 +7124,11 @@
     </row>
     <row r="181" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="26" t="str">
-        <f t="shared" si="3"/>
-        <v>zonmwpa:FederalUniversityofRiodeJaneiro</v>
+        <f t="shared" ref="A181:A234" si="3">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B181," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>zonmwpa:ExpertisecentrumNederlands</v>
       </c>
       <c r="B181" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C181" s="30"/>
       <c r="D181" s="48"/>
@@ -7150,10 +7155,10 @@
     <row r="182" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:GGDAmsterdam-PublicHealthServiceofAmsterdam</v>
+        <v>zonmwpa:FederalUniversityofRiodeJaneiro</v>
       </c>
       <c r="B182" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C182" s="30"/>
       <c r="D182" s="48"/>
@@ -7180,10 +7185,10 @@
     <row r="183" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:GGDZuidHollandZuid</v>
+        <v>zonmwpa:GGDAmsterdam-PublicHealthServiceofAmsterdam</v>
       </c>
       <c r="B183" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C183" s="30"/>
       <c r="D183" s="48"/>
@@ -7210,10 +7215,10 @@
     <row r="184" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:GOFAIRFoundation</v>
+        <v>zonmwpa:GGDZuidHollandZuid</v>
       </c>
       <c r="B184" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C184" s="30"/>
       <c r="D184" s="48"/>
@@ -7240,10 +7245,10 @@
     <row r="185" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:HogeschoolLeiden-UniversityofAppliedSciencesLeiden</v>
+        <v>zonmwpa:GOFAIRFoundation</v>
       </c>
       <c r="B185" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C185" s="30"/>
       <c r="D185" s="48"/>
@@ -7270,10 +7275,10 @@
     <row r="186" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:HogeschoolvanAmsterdam-AmsterdamUniversityofAppliedSciences</v>
+        <v>zonmwpa:HogeschoolLeiden-UniversityofAppliedSciencesLeiden</v>
       </c>
       <c r="B186" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C186" s="30"/>
       <c r="D186" s="48"/>
@@ -7300,10 +7305,10 @@
     <row r="187" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:IKNL-NetherlandsComprehensiveCancerOrganisation</v>
+        <v>zonmwpa:HogeschoolvanAmsterdam-AmsterdamUniversityofAppliedSciences</v>
       </c>
       <c r="B187" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C187" s="30"/>
       <c r="D187" s="48"/>
@@ -7330,10 +7335,10 @@
     <row r="188" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:LeidenUniversity</v>
+        <v>zonmwpa:IKNL-NetherlandsComprehensiveCancerOrganisation</v>
       </c>
       <c r="B188" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C188" s="30"/>
       <c r="D188" s="48"/>
@@ -7360,10 +7365,10 @@
     <row r="189" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:LeidenUniversityMedicalCenter</v>
+        <v>zonmwpa:LeidenUniversity</v>
       </c>
       <c r="B189" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C189" s="30"/>
       <c r="D189" s="48"/>
@@ -7390,10 +7395,10 @@
     <row r="190" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:MaastrichtUniversity</v>
+        <v>zonmwpa:LeidenUniversityMedicalCenter</v>
       </c>
       <c r="B190" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C190" s="30"/>
       <c r="D190" s="48"/>
@@ -7420,10 +7425,10 @@
     <row r="191" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:MaastrichtUniversityMedicalCentre</v>
+        <v>zonmwpa:MaastrichtUniversity</v>
       </c>
       <c r="B191" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C191" s="30"/>
       <c r="D191" s="48"/>
@@ -7450,10 +7455,10 @@
     <row r="192" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NetherlandsComprehensiveCancerOrganisation</v>
+        <v>zonmwpa:MaastrichtUniversityMedicalCentre</v>
       </c>
       <c r="B192" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C192" s="30"/>
       <c r="D192" s="48"/>
@@ -7480,10 +7485,10 @@
     <row r="193" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NetherlandsHeartInstitute</v>
+        <v>zonmwpa:NetherlandsComprehensiveCancerOrganisation</v>
       </c>
       <c r="B193" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C193" s="30"/>
       <c r="D193" s="48"/>
@@ -7510,10 +7515,10 @@
     <row r="194" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NIVEL-NetherlandsInstituteforHealthServicesResearch</v>
+        <v>zonmwpa:NetherlandsHeartInstitute</v>
       </c>
       <c r="B194" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C194" s="30"/>
       <c r="D194" s="48"/>
@@ -7540,10 +7545,10 @@
     <row r="195" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:NSCR-NetherlandsInstitutefortheStudyofCrimeandLawEnforcement</v>
+        <v>zonmwpa:NIVEL-NetherlandsInstituteforHealthServicesResearch</v>
       </c>
       <c r="B195" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C195" s="30"/>
       <c r="D195" s="48"/>
@@ -7570,10 +7575,10 @@
     <row r="196" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:PublicHealthServiceofAmsterdam</v>
+        <v>zonmwpa:NSCR-NetherlandsInstitutefortheStudyofCrimeandLawEnforcement</v>
       </c>
       <c r="B196" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C196" s="30"/>
       <c r="D196" s="48"/>
@@ -7600,10 +7605,10 @@
     <row r="197" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:PublicProcurementResearchCentre-PPRC</v>
+        <v>zonmwpa:PublicHealthServiceofAmsterdam</v>
       </c>
       <c r="B197" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C197" s="30"/>
       <c r="D197" s="48"/>
@@ -7630,10 +7635,10 @@
     <row r="198" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:RadboudUniversityNijmegen</v>
+        <v>zonmwpa:PublicProcurementResearchCentre-PPRC</v>
       </c>
       <c r="B198" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C198" s="30"/>
       <c r="D198" s="48"/>
@@ -7660,10 +7665,10 @@
     <row r="199" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:RadboudUniversityNijmegenMedicalCentre</v>
+        <v>zonmwpa:RadboudUniversityNijmegen</v>
       </c>
       <c r="B199" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C199" s="30"/>
       <c r="D199" s="48"/>
@@ -7690,10 +7695,10 @@
     <row r="200" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:ReadeResearchBV</v>
+        <v>zonmwpa:RadboudUniversityNijmegenMedicalCentre</v>
       </c>
       <c r="B200" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C200" s="30"/>
       <c r="D200" s="48"/>
@@ -7720,10 +7725,10 @@
     <row r="201" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:RIVM-NationalInstituteforPublicHealthandtheEnvironment</v>
+        <v>zonmwpa:ReadeResearchBV</v>
       </c>
       <c r="B201" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C201" s="30"/>
       <c r="D201" s="48"/>
@@ -7750,10 +7755,10 @@
     <row r="202" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Sanquin</v>
+        <v>zonmwpa:RIVM-NationalInstituteforPublicHealthandtheEnvironment</v>
       </c>
       <c r="B202" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C202" s="30"/>
       <c r="D202" s="48"/>
@@ -7780,10 +7785,10 @@
     <row r="203" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:SaxionUniversityofAppliedSciences</v>
+        <v>zonmwpa:Sanquin</v>
       </c>
       <c r="B203" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C203" s="30"/>
       <c r="D203" s="48"/>
@@ -7810,10 +7815,10 @@
     <row r="204" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:SEOEconomischOnderzoek</v>
+        <v>zonmwpa:SaxionUniversityofAppliedSciences</v>
       </c>
       <c r="B204" s="31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C204" s="30"/>
       <c r="D204" s="48"/>
@@ -7840,10 +7845,10 @@
     <row r="205" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:SpaarneGasthuis-SpaarneZiekenhuis</v>
+        <v>zonmwpa:SEOEconomischOnderzoek</v>
       </c>
       <c r="B205" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C205" s="30"/>
       <c r="D205" s="48"/>
@@ -7870,10 +7875,10 @@
     <row r="206" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:TilburgUniversity</v>
+        <v>zonmwpa:SpaarneGasthuis-SpaarneZiekenhuis</v>
       </c>
       <c r="B206" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C206" s="30"/>
       <c r="D206" s="48"/>
@@ -7900,10 +7905,10 @@
     <row r="207" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:TNO-NetherlandsOrganisationforAppliedScientificResearch</v>
+        <v>zonmwpa:TilburgUniversity</v>
       </c>
       <c r="B207" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C207" s="30"/>
       <c r="D207" s="48"/>
@@ -7930,10 +7935,10 @@
     <row r="208" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:UniversityMedicalCenterGroningen</v>
+        <v>zonmwpa:TNO-NetherlandsOrganisationforAppliedScientificResearch</v>
       </c>
       <c r="B208" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C208" s="30"/>
       <c r="D208" s="48"/>
@@ -7960,10 +7965,10 @@
     <row r="209" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:UniversityMedicalCenterUtrecht</v>
+        <v>zonmwpa:UniversityMedicalCenterGroningen</v>
       </c>
       <c r="B209" s="31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C209" s="30"/>
       <c r="D209" s="48"/>
@@ -7990,10 +7995,10 @@
     <row r="210" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:UniversityofAmsterdam</v>
+        <v>zonmwpa:UniversityMedicalCenterUtrecht</v>
       </c>
       <c r="B210" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C210" s="30"/>
       <c r="D210" s="48"/>
@@ -8020,10 +8025,10 @@
     <row r="211" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:UniversityofGroningen</v>
+        <v>zonmwpa:UniversityofAmsterdam</v>
       </c>
       <c r="B211" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C211" s="30"/>
       <c r="D211" s="48"/>
@@ -8050,10 +8055,10 @@
     <row r="212" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:UniversityofHumanisticStudies</v>
+        <v>zonmwpa:UniversityofGroningen</v>
       </c>
       <c r="B212" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C212" s="30"/>
       <c r="D212" s="48"/>
@@ -8080,10 +8085,10 @@
     <row r="213" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:UniversityofTwente</v>
+        <v>zonmwpa:UniversityofHumanisticStudies</v>
       </c>
       <c r="B213" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C213" s="30"/>
       <c r="D213" s="48"/>
@@ -8110,10 +8115,10 @@
     <row r="214" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:UtrechtUniversity</v>
+        <v>zonmwpa:UniversityofTwente</v>
       </c>
       <c r="B214" s="31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C214" s="30"/>
       <c r="D214" s="48"/>
@@ -8140,10 +8145,10 @@
     <row r="215" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Veiligheids-enGezondheidsregioGelderland-Midden</v>
+        <v>zonmwpa:UtrechtUniversity</v>
       </c>
       <c r="B215" s="31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C215" s="30"/>
       <c r="D215" s="48"/>
@@ -8170,10 +8175,10 @@
     <row r="216" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:VUAmsterdam</v>
+        <v>zonmwpa:Veiligheids-enGezondheidsregioGelderland-Midden</v>
       </c>
       <c r="B216" s="31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C216" s="30"/>
       <c r="D216" s="48"/>
@@ -8200,10 +8205,10 @@
     <row r="217" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:VUUniversityMedicalCenter</v>
+        <v>zonmwpa:VUAmsterdam</v>
       </c>
       <c r="B217" s="31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C217" s="30"/>
       <c r="D217" s="48"/>
@@ -8230,10 +8235,10 @@
     <row r="218" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:WageningenUniversity-Research</v>
+        <v>zonmwpa:VUUniversityMedicalCenter</v>
       </c>
       <c r="B218" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C218" s="30"/>
       <c r="D218" s="48"/>
@@ -8260,10 +8265,10 @@
     <row r="219" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:ZonMw-NetherlandsOrganisationforHealthResearchandDevelopment</v>
+        <v>zonmwpa:WageningenUniversity-Research</v>
       </c>
       <c r="B219" s="31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C219" s="30"/>
       <c r="D219" s="48"/>
@@ -8290,10 +8295,10 @@
     <row r="220" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Otherinstitution</v>
+        <v>zonmwpa:ZonMw-NetherlandsOrganisationforHealthResearchandDevelopment</v>
       </c>
       <c r="B220" s="31" t="s">
-        <v>216</v>
+        <v>283</v>
       </c>
       <c r="C220" s="30"/>
       <c r="D220" s="48"/>
@@ -8318,29 +8323,23 @@
       <c r="U220" s="3"/>
     </row>
     <row r="221" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A221" s="16" t="str">
+      <c r="A221" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:FocusArea</v>
-      </c>
-      <c r="B221" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="C221" s="16"/>
-      <c r="D221" s="46" t="s">
-        <v>293</v>
-      </c>
-      <c r="E221" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="F221" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G221" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H221" s="18"/>
-      <c r="I221" s="18"/>
-      <c r="J221" s="18"/>
+        <v>zonmwpa:Otherinstitution</v>
+      </c>
+      <c r="B221" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="C221" s="30"/>
+      <c r="D221" s="48"/>
+      <c r="E221" s="26"/>
+      <c r="F221" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="G221" s="30"/>
+      <c r="H221" s="30"/>
+      <c r="I221" s="30"/>
+      <c r="J221" s="30"/>
       <c r="K221" s="3"/>
       <c r="L221" s="3"/>
       <c r="M221" s="3"/>
@@ -8354,25 +8353,29 @@
       <c r="U221" s="3"/>
     </row>
     <row r="222" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A222" s="26" t="str">
-        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B222," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>zonmwpa:Predictivediagnosticsandtreatment</v>
-      </c>
-      <c r="B222" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="C222" s="30"/>
-      <c r="D222" s="48" t="s">
+      <c r="A222" s="16" t="str">
+        <f t="shared" si="3"/>
+        <v>zonmwpa:FocusArea</v>
+      </c>
+      <c r="B222" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="C222" s="16"/>
+      <c r="D222" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E222" s="26"/>
-      <c r="F222" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="G222" s="30"/>
-      <c r="H222" s="30"/>
-      <c r="I222" s="30"/>
-      <c r="J222" s="30"/>
+      <c r="E222" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="F222" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G222" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H222" s="18"/>
+      <c r="I222" s="18"/>
+      <c r="J222" s="18"/>
       <c r="K222" s="3"/>
       <c r="L222" s="3"/>
       <c r="M222" s="3"/>
@@ -8387,18 +8390,18 @@
     </row>
     <row r="223" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="26" t="str">
-        <f t="shared" si="3"/>
-        <v>zonmwpa:Careandprevention</v>
+        <f>"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B223," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>zonmwpa:Predictivediagnosticsandtreatment</v>
       </c>
       <c r="B223" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C223" s="30"/>
       <c r="D223" s="48" t="s">
         <v>293</v>
       </c>
       <c r="E223" s="26"/>
-      <c r="F223" s="30" t="s">
+      <c r="F223" s="34" t="s">
         <v>181</v>
       </c>
       <c r="G223" s="30"/>
@@ -8420,10 +8423,10 @@
     <row r="224" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Effectsonsociety</v>
+        <v>zonmwpa:Careandprevention</v>
       </c>
       <c r="B224" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C224" s="30"/>
       <c r="D224" s="48" t="s">
@@ -8452,10 +8455,10 @@
     <row r="225" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:OtherFocusArea</v>
+        <v>zonmwpa:Effectsonsociety</v>
       </c>
       <c r="B225" s="31" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="C225" s="30"/>
       <c r="D225" s="48" t="s">
@@ -8482,29 +8485,25 @@
       <c r="U225" s="3"/>
     </row>
     <row r="226" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A226" s="16" t="str">
+      <c r="A226" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Theme</v>
-      </c>
-      <c r="B226" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="C226" s="16"/>
-      <c r="D226" s="46" t="s">
+        <v>zonmwpa:OtherFocusArea</v>
+      </c>
+      <c r="B226" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="C226" s="30"/>
+      <c r="D226" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E226" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="F226" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="G226" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H226" s="18"/>
-      <c r="I226" s="18"/>
-      <c r="J226" s="18"/>
+      <c r="E226" s="26"/>
+      <c r="F226" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="G226" s="30"/>
+      <c r="H226" s="30"/>
+      <c r="I226" s="30"/>
+      <c r="J226" s="30"/>
       <c r="K226" s="3"/>
       <c r="L226" s="3"/>
       <c r="M226" s="3"/>
@@ -8518,25 +8517,29 @@
       <c r="U226" s="3"/>
     </row>
     <row r="227" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A227" s="26" t="str">
+      <c r="A227" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Treatment</v>
-      </c>
-      <c r="B227" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="C227" s="30"/>
-      <c r="D227" s="48" t="s">
+        <v>zonmwpa:Theme</v>
+      </c>
+      <c r="B227" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="C227" s="16"/>
+      <c r="D227" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="E227" s="26"/>
-      <c r="F227" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="G227" s="30"/>
-      <c r="H227" s="30"/>
-      <c r="I227" s="30"/>
-      <c r="J227" s="30"/>
+      <c r="E227" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="F227" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G227" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H227" s="18"/>
+      <c r="I227" s="18"/>
+      <c r="J227" s="18"/>
       <c r="K227" s="3"/>
       <c r="L227" s="3"/>
       <c r="M227" s="3"/>
@@ -8552,10 +8555,10 @@
     <row r="228" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Diagnosticsofinfection</v>
+        <v>zonmwpa:Treatment</v>
       </c>
       <c r="B228" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C228" s="30"/>
       <c r="D228" s="48" t="s">
@@ -8584,10 +8587,10 @@
     <row r="229" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Riskanalysisandprognostics</v>
+        <v>zonmwpa:Diagnosticsofinfection</v>
       </c>
       <c r="B229" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C229" s="30"/>
       <c r="D229" s="48" t="s">
@@ -8616,10 +8619,10 @@
     <row r="230" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Virus-immunity-immuneresponseandpathogenesis</v>
+        <v>zonmwpa:Riskanalysisandprognostics</v>
       </c>
       <c r="B230" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C230" s="30"/>
       <c r="D230" s="48" t="s">
@@ -8648,10 +8651,10 @@
     <row r="231" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A231" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Clinicaltreatment</v>
+        <v>zonmwpa:Virus-immunity-immuneresponseandpathogenesis</v>
       </c>
       <c r="B231" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C231" s="30"/>
       <c r="D231" s="48" t="s">
@@ -8680,10 +8683,10 @@
     <row r="232" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Animalfreeinnovations</v>
+        <v>zonmwpa:Clinicaltreatment</v>
       </c>
       <c r="B232" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C232" s="30"/>
       <c r="D232" s="48" t="s">
@@ -8712,10 +8715,10 @@
     <row r="233" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A233" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>zonmwpa:Organisationofcareandprevention</v>
+        <v>zonmwpa:Animalfreeinnovations</v>
       </c>
       <c r="B233" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C233" s="30"/>
       <c r="D233" s="48" t="s">
@@ -8743,11 +8746,11 @@
     </row>
     <row r="234" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" s="26" t="str">
-        <f t="shared" ref="A234:A254" si="4">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B234," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>zonmwpa:Careandpreventionforvulnerablecitizens</v>
+        <f t="shared" si="3"/>
+        <v>zonmwpa:Organisationofcareandprevention</v>
       </c>
       <c r="B234" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C234" s="30"/>
       <c r="D234" s="48" t="s">
@@ -8775,11 +8778,11 @@
     </row>
     <row r="235" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A235" s="26" t="str">
-        <f t="shared" si="4"/>
-        <v>zonmwpa:Transmissionandepidemiology</v>
+        <f t="shared" ref="A235:A255" si="4">"zonmwpa:"&amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B235," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>zonmwpa:Careandpreventionforvulnerablecitizens</v>
       </c>
       <c r="B235" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C235" s="30"/>
       <c r="D235" s="48" t="s">
@@ -8808,10 +8811,10 @@
     <row r="236" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A236" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Palliativecare</v>
+        <v>zonmwpa:Transmissionandepidemiology</v>
       </c>
       <c r="B236" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C236" s="30"/>
       <c r="D236" s="48" t="s">
@@ -8840,10 +8843,10 @@
     <row r="237" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A237" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Impactofmeasuresorstrategies</v>
+        <v>zonmwpa:Palliativecare</v>
       </c>
       <c r="B237" s="31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C237" s="30"/>
       <c r="D237" s="48" t="s">
@@ -8872,10 +8875,10 @@
     <row r="238" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A238" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Resilienceofsociety</v>
+        <v>zonmwpa:Impactofmeasuresorstrategies</v>
       </c>
       <c r="B238" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C238" s="30"/>
       <c r="D238" s="48" t="s">
@@ -8904,10 +8907,10 @@
     <row r="239" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A239" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Economicresilience</v>
+        <v>zonmwpa:Resilienceofsociety</v>
       </c>
       <c r="B239" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C239" s="30"/>
       <c r="D239" s="48" t="s">
@@ -8936,10 +8939,10 @@
     <row r="240" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A240" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:OtherTheme</v>
+        <v>zonmwpa:Economicresilience</v>
       </c>
       <c r="B240" s="31" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="C240" s="30"/>
       <c r="D240" s="48" t="s">
@@ -8966,25 +8969,25 @@
       <c r="U240" s="3"/>
     </row>
     <row r="241" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A241" s="16" t="str">
+      <c r="A241" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Province</v>
-      </c>
-      <c r="B241" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="C241" s="16"/>
-      <c r="D241" s="46"/>
-      <c r="E241" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="F241" s="17"/>
-      <c r="G241" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H241" s="18"/>
-      <c r="I241" s="18"/>
-      <c r="J241" s="18"/>
+        <v>zonmwpa:OtherTheme</v>
+      </c>
+      <c r="B241" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="C241" s="30"/>
+      <c r="D241" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="E241" s="26"/>
+      <c r="F241" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="G241" s="30"/>
+      <c r="H241" s="30"/>
+      <c r="I241" s="30"/>
+      <c r="J241" s="30"/>
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
       <c r="M241" s="3"/>
@@ -8998,23 +9001,25 @@
       <c r="U241" s="3"/>
     </row>
     <row r="242" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A242" s="26" t="str">
+      <c r="A242" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Drenthe</v>
-      </c>
-      <c r="B242" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="C242" s="30"/>
-      <c r="D242" s="48"/>
-      <c r="E242" s="26"/>
-      <c r="F242" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="G242" s="30"/>
-      <c r="H242" s="30"/>
-      <c r="I242" s="30"/>
-      <c r="J242" s="30"/>
+        <v>zonmwpa:Province</v>
+      </c>
+      <c r="B242" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C242" s="16"/>
+      <c r="D242" s="46"/>
+      <c r="E242" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="F242" s="17"/>
+      <c r="G242" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H242" s="18"/>
+      <c r="I242" s="18"/>
+      <c r="J242" s="18"/>
       <c r="K242" s="3"/>
       <c r="L242" s="3"/>
       <c r="M242" s="3"/>
@@ -9030,10 +9035,10 @@
     <row r="243" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A243" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Flevoland</v>
+        <v>zonmwpa:Drenthe</v>
       </c>
       <c r="B243" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C243" s="30"/>
       <c r="D243" s="48"/>
@@ -9060,10 +9065,10 @@
     <row r="244" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A244" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Friesland</v>
+        <v>zonmwpa:Flevoland</v>
       </c>
       <c r="B244" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C244" s="30"/>
       <c r="D244" s="48"/>
@@ -9090,10 +9095,10 @@
     <row r="245" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A245" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Gelderland</v>
+        <v>zonmwpa:Friesland</v>
       </c>
       <c r="B245" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C245" s="30"/>
       <c r="D245" s="48"/>
@@ -9120,10 +9125,10 @@
     <row r="246" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A246" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Groningen</v>
+        <v>zonmwpa:Gelderland</v>
       </c>
       <c r="B246" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C246" s="30"/>
       <c r="D246" s="48"/>
@@ -9150,10 +9155,10 @@
     <row r="247" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A247" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Limburg</v>
+        <v>zonmwpa:Groningen</v>
       </c>
       <c r="B247" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C247" s="30"/>
       <c r="D247" s="48"/>
@@ -9180,10 +9185,10 @@
     <row r="248" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A248" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Noord-Brabant</v>
+        <v>zonmwpa:Limburg</v>
       </c>
       <c r="B248" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C248" s="30"/>
       <c r="D248" s="48"/>
@@ -9210,10 +9215,10 @@
     <row r="249" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A249" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Noord-Holland</v>
+        <v>zonmwpa:Noord-Brabant</v>
       </c>
       <c r="B249" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C249" s="30"/>
       <c r="D249" s="48"/>
@@ -9240,10 +9245,10 @@
     <row r="250" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A250" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Overijssel</v>
+        <v>zonmwpa:Noord-Holland</v>
       </c>
       <c r="B250" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C250" s="30"/>
       <c r="D250" s="48"/>
@@ -9270,10 +9275,10 @@
     <row r="251" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A251" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Utrecht</v>
+        <v>zonmwpa:Overijssel</v>
       </c>
       <c r="B251" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C251" s="30"/>
       <c r="D251" s="48"/>
@@ -9300,10 +9305,10 @@
     <row r="252" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A252" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Zeeland</v>
+        <v>zonmwpa:Utrecht</v>
       </c>
       <c r="B252" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C252" s="30"/>
       <c r="D252" s="48"/>
@@ -9330,10 +9335,10 @@
     <row r="253" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A253" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:Zuid-Holland</v>
+        <v>zonmwpa:Zeeland</v>
       </c>
       <c r="B253" s="26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C253" s="30"/>
       <c r="D253" s="48"/>
@@ -9360,10 +9365,10 @@
     <row r="254" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A254" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>zonmwpa:OtherProvince</v>
-      </c>
-      <c r="B254" s="31" t="s">
-        <v>215</v>
+        <v>zonmwpa:Zuid-Holland</v>
+      </c>
+      <c r="B254" s="26" t="s">
+        <v>214</v>
       </c>
       <c r="C254" s="30"/>
       <c r="D254" s="48"/>
@@ -9388,16 +9393,23 @@
       <c r="U254" s="3"/>
     </row>
     <row r="255" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A255" s="3"/>
-      <c r="B255" s="32"/>
-      <c r="C255" s="3"/>
-      <c r="D255" s="41"/>
-      <c r="E255" s="3"/>
-      <c r="F255" s="3"/>
-      <c r="G255" s="3"/>
-      <c r="H255" s="3"/>
-      <c r="I255" s="3"/>
-      <c r="J255" s="3"/>
+      <c r="A255" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v>zonmwpa:OtherProvince</v>
+      </c>
+      <c r="B255" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="C255" s="30"/>
+      <c r="D255" s="48"/>
+      <c r="E255" s="26"/>
+      <c r="F255" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="G255" s="30"/>
+      <c r="H255" s="30"/>
+      <c r="I255" s="30"/>
+      <c r="J255" s="30"/>
       <c r="K255" s="3"/>
       <c r="L255" s="3"/>
       <c r="M255" s="3"/>
@@ -9596,7 +9608,7 @@
     </row>
     <row r="264" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A264" s="3"/>
-      <c r="B264" s="3"/>
+      <c r="B264" s="32"/>
       <c r="C264" s="3"/>
       <c r="D264" s="41"/>
       <c r="E264" s="3"/>
@@ -9619,7 +9631,7 @@
     </row>
     <row r="265" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A265" s="3"/>
-      <c r="B265" s="32"/>
+      <c r="B265" s="3"/>
       <c r="C265" s="3"/>
       <c r="D265" s="41"/>
       <c r="E265" s="3"/>
@@ -9665,7 +9677,7 @@
     </row>
     <row r="267" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A267" s="3"/>
-      <c r="B267" s="3"/>
+      <c r="B267" s="32"/>
       <c r="C267" s="3"/>
       <c r="D267" s="41"/>
       <c r="E267" s="3"/>
@@ -9688,7 +9700,7 @@
     </row>
     <row r="268" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A268" s="3"/>
-      <c r="B268" s="32"/>
+      <c r="B268" s="3"/>
       <c r="C268" s="3"/>
       <c r="D268" s="41"/>
       <c r="E268" s="3"/>
@@ -9826,7 +9838,7 @@
     </row>
     <row r="274" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A274" s="3"/>
-      <c r="B274" s="3"/>
+      <c r="B274" s="32"/>
       <c r="C274" s="3"/>
       <c r="D274" s="41"/>
       <c r="E274" s="3"/>
@@ -9849,7 +9861,7 @@
     </row>
     <row r="275" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A275" s="3"/>
-      <c r="B275" s="32"/>
+      <c r="B275" s="3"/>
       <c r="C275" s="3"/>
       <c r="D275" s="41"/>
       <c r="E275" s="3"/>
@@ -9941,7 +9953,7 @@
     </row>
     <row r="279" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A279" s="3"/>
-      <c r="B279" s="3"/>
+      <c r="B279" s="32"/>
       <c r="C279" s="3"/>
       <c r="D279" s="41"/>
       <c r="E279" s="3"/>
@@ -9964,7 +9976,7 @@
     </row>
     <row r="280" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A280" s="3"/>
-      <c r="B280" s="32"/>
+      <c r="B280" s="3"/>
       <c r="C280" s="3"/>
       <c r="D280" s="41"/>
       <c r="E280" s="3"/>
@@ -9987,7 +9999,7 @@
     </row>
     <row r="281" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A281" s="3"/>
-      <c r="B281" s="3"/>
+      <c r="B281" s="32"/>
       <c r="C281" s="3"/>
       <c r="D281" s="41"/>
       <c r="E281" s="3"/>
@@ -10010,7 +10022,7 @@
     </row>
     <row r="282" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A282" s="3"/>
-      <c r="B282" s="32"/>
+      <c r="B282" s="3"/>
       <c r="C282" s="3"/>
       <c r="D282" s="41"/>
       <c r="E282" s="3"/>
@@ -10079,7 +10091,7 @@
     </row>
     <row r="285" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A285" s="3"/>
-      <c r="B285" s="3"/>
+      <c r="B285" s="32"/>
       <c r="C285" s="3"/>
       <c r="D285" s="41"/>
       <c r="E285" s="3"/>
@@ -27143,10 +27155,33 @@
       <c r="T1026" s="3"/>
       <c r="U1026" s="3"/>
     </row>
+    <row r="1027" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1027" s="3"/>
+      <c r="B1027" s="3"/>
+      <c r="C1027" s="3"/>
+      <c r="D1027" s="41"/>
+      <c r="E1027" s="3"/>
+      <c r="F1027" s="3"/>
+      <c r="G1027" s="3"/>
+      <c r="H1027" s="3"/>
+      <c r="I1027" s="3"/>
+      <c r="J1027" s="3"/>
+      <c r="K1027" s="3"/>
+      <c r="L1027" s="3"/>
+      <c r="M1027" s="3"/>
+      <c r="N1027" s="3"/>
+      <c r="O1027" s="3"/>
+      <c r="P1027" s="3"/>
+      <c r="Q1027" s="3"/>
+      <c r="R1027" s="3"/>
+      <c r="S1027" s="3"/>
+      <c r="T1027" s="3"/>
+      <c r="U1027" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>